<commit_message>
docs: update design documents
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/Design_general_mem_alloc.xlsx
+++ b/libalconcurrent/doc/Design_general_mem_alloc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my_dev\alpha_concurrent\libalconcurrent\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A7B72F-0E05-456A-9CB1-8C709A023ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5487E257-8E71-4E3A-B2AE-1CA9F9DE58A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>param_chunk_allocation</t>
   </si>
@@ -46,10 +46,6 @@
   </si>
   <si>
     <t>param_chunk_comb の配列(param_chunk_allocationでソート済み)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>internal::chunk_listへのunique_ptr</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -376,13 +372,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>560295</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>134471</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -472,172 +468,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="直線矢印コネクタ 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAD8EA4F-9E66-406C-B2A9-A97209A105F5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5905500" y="2505075"/>
-          <a:ext cx="2286000" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="フリーフォーム: 図形 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A370C66B-20EE-41C3-A300-6274DD9357F1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5181600" y="2247900"/>
-          <a:ext cx="3686175" cy="523875"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst>
-            <a:gd name="connsiteX0" fmla="*/ 0 w 3686175"/>
-            <a:gd name="connsiteY0" fmla="*/ 0 h 523875"/>
-            <a:gd name="connsiteX1" fmla="*/ 1895475 w 3686175"/>
-            <a:gd name="connsiteY1" fmla="*/ 0 h 523875"/>
-            <a:gd name="connsiteX2" fmla="*/ 2600325 w 3686175"/>
-            <a:gd name="connsiteY2" fmla="*/ 523875 h 523875"/>
-            <a:gd name="connsiteX3" fmla="*/ 3686175 w 3686175"/>
-            <a:gd name="connsiteY3" fmla="*/ 523875 h 523875"/>
-          </a:gdLst>
-          <a:ahLst/>
-          <a:cxnLst>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX0" y="connsiteY0"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX1" y="connsiteY1"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX2" y="connsiteY2"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX3" y="connsiteY3"/>
-            </a:cxn>
-          </a:cxnLst>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="3686175" h="523875">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="1895475" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="2600325" y="523875"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="3686175" y="523875"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1666875</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>666751</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -737,13 +574,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>3000375</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>638175</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -790,13 +627,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>3086100</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
@@ -896,13 +733,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>1743075</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -949,13 +786,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>3086100</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
@@ -1055,13 +892,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1743075</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -1108,13 +945,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>2466975</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>114298</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>657225</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
@@ -1214,13 +1051,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>1704976</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>428626</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1289,13 +1126,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>2828925</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -1387,13 +1224,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -1441,13 +1278,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -1495,13 +1332,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -1549,13 +1386,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -1603,13 +1440,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -1657,13 +1494,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>390526</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>676276</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
@@ -1724,13 +1561,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>381001</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>666751</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
@@ -1791,13 +1628,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>219075</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -1845,13 +1682,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>14288</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>114304</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>157166</xdr:rowOff>
@@ -1906,13 +1743,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>681038</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>133357</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>176219</xdr:rowOff>
@@ -1967,13 +1804,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>44822</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>190508</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>661146</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>233370</xdr:rowOff>
@@ -2028,13 +1865,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
@@ -2126,13 +1963,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>14288</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>171458</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>214320</xdr:rowOff>
@@ -2187,13 +2024,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>2428876</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>352425</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>672354</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -2285,13 +2122,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -2364,13 +2201,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>219076</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -2439,13 +2276,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1657350</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -2514,13 +2351,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>14287</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>133357</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>657224</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>176219</xdr:rowOff>
@@ -2575,13 +2412,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -2683,13 +2520,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -2791,13 +2628,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -2888,13 +2725,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>224117</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>302559</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>89647</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>78441</xdr:rowOff>
@@ -3010,13 +2847,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>170890</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>102533</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>1242732</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3131,13 +2968,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>573182</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>231963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>661146</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>134472</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3197,13 +3034,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>6722</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>62760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>3216088</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>105623</xdr:rowOff>
@@ -3258,13 +3095,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1557618</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>134471</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1456765</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>56029</xdr:rowOff>
@@ -3364,13 +3201,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>178734</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>89084</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>246530</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>156881</xdr:rowOff>
@@ -3707,277 +3544,266 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AE40"/>
+  <dimension ref="B3:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col min="13" max="13" width="42.75" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="42.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="42.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:31">
-      <c r="B2" t="s">
+    <row r="3" spans="2:25">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:31">
-      <c r="C3" t="s">
+    <row r="4" spans="2:25">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:31">
-      <c r="D7" t="s">
+    <row r="8" spans="2:25">
+      <c r="D8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:31">
-      <c r="E8" t="s">
+    <row r="9" spans="2:25">
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
+    </row>
+    <row r="10" spans="2:25">
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25">
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" ht="37.5">
+      <c r="G13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="X13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" ht="37.5">
+      <c r="G14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" t="s">
+        <v>12</v>
+      </c>
+      <c r="U15" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25">
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="5:15">
+      <c r="E17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="5:15">
+      <c r="E18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="5:15">
+      <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="9" spans="2:31">
-      <c r="E9" t="s">
-        <v>4</v>
+    <row r="22" spans="5:15">
+      <c r="M22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:31">
-      <c r="E10">
+    <row r="23" spans="5:15">
+      <c r="M23" s="4">
         <v>0</v>
       </c>
-      <c r="F10" t="s">
-        <v>0</v>
+      <c r="O23" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:31">
-      <c r="F11" t="s">
+    <row r="24" spans="5:15">
+      <c r="M24" s="4">
+        <v>1</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="5:15">
+      <c r="M25" s="4">
+        <v>2</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="5:15">
+      <c r="M26" s="4">
+        <v>3</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="5:15">
+      <c r="M27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L11" t="s">
-        <v>10</v>
+      <c r="O27" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:31">
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>0</v>
-      </c>
-      <c r="M12" t="s">
-        <v>0</v>
+    <row r="28" spans="5:15">
+      <c r="M28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:31" ht="37.5">
-      <c r="F13" t="s">
-        <v>5</v>
-      </c>
-      <c r="M13" s="2" t="s">
+    <row r="29" spans="5:15">
+      <c r="M29" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>12</v>
+      <c r="O29" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:31" ht="37.5">
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q14" s="6" t="s">
+    <row r="36" spans="18:22">
+      <c r="R36" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AA14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE14" s="3" t="s">
-        <v>11</v>
+      <c r="S36" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="T36" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V36" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:31">
-      <c r="E15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>13</v>
+    <row r="37" spans="18:22">
+      <c r="R37" t="s">
+        <v>33</v>
+      </c>
+      <c r="S37" t="s">
+        <v>33</v>
+      </c>
+      <c r="T37" t="s">
+        <v>33</v>
+      </c>
+      <c r="V37" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="16" spans="2:31">
-      <c r="E16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>15</v>
+    <row r="38" spans="18:22">
+      <c r="R38" t="s">
+        <v>34</v>
+      </c>
+      <c r="S38" t="s">
+        <v>34</v>
+      </c>
+      <c r="T38" t="s">
+        <v>32</v>
+      </c>
+      <c r="V38" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="17" spans="5:21">
-      <c r="E17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>16</v>
+    <row r="39" spans="18:22">
+      <c r="R39" t="s">
+        <v>34</v>
+      </c>
+      <c r="S39" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="18" spans="5:21">
-      <c r="F18" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="5:21">
-      <c r="Q19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="5:21">
-      <c r="S22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="U22" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="5:21">
-      <c r="S23" s="4">
-        <v>0</v>
-      </c>
-      <c r="U23" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="5:21">
-      <c r="S24" s="4">
-        <v>1</v>
-      </c>
-      <c r="U24" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="5:21">
-      <c r="S25" s="4">
-        <v>2</v>
-      </c>
-      <c r="U25" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="5:21">
-      <c r="S26" s="4">
-        <v>3</v>
-      </c>
-      <c r="U26" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="5:21">
-      <c r="S27" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="U27" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="5:21">
-      <c r="S28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="U28" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="5:21">
-      <c r="S29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="U29" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="24:28">
-      <c r="X36" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y36" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z36" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA36" s="5" t="s">
+    <row r="40" spans="18:22">
+      <c r="R40" t="s">
         <v>36</v>
-      </c>
-      <c r="AB36" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="24:28">
-      <c r="X37" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y37" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z37" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="24:28">
-      <c r="X38" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z38" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="24:28">
-      <c r="X39" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="24:28">
-      <c r="X40" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add source code for new slot design
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/Design_general_mem_alloc.xlsx
+++ b/libalconcurrent/doc/Design_general_mem_alloc.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5487E257-8E71-4E3A-B2AE-1CA9F9DE58A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA293FE0-07E7-4FEE-9112-5FA60D7085B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="68">
   <si>
     <t>param_chunk_allocation</t>
   </si>
@@ -273,6 +274,273 @@
     <rPh sb="45" eb="46">
       <t>タメ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0番スロットの固有情報</t>
+    <rPh sb="1" eb="2">
+      <t>バン</t>
+    </rPh>
+    <rPh sb="7" eb="11">
+      <t>コユウジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1番スロットの固有情報</t>
+    <rPh sb="1" eb="2">
+      <t>バン</t>
+    </rPh>
+    <rPh sb="7" eb="11">
+      <t>コユウジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n-1番スロットの固有情報</t>
+    <rPh sb="3" eb="4">
+      <t>バン</t>
+    </rPh>
+    <rPh sb="9" eb="13">
+      <t>コユウジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0番スロットのメモリ領域</t>
+    <rPh sb="1" eb="2">
+      <t>バン</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>リョウイキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1番スロットのメモリ領域</t>
+    <rPh sb="1" eb="2">
+      <t>バン</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>リョウイキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n-1番スロットのメモリ情報</t>
+    <rPh sb="3" eb="4">
+      <t>バン</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>空きスロットスタックリストの先頭スロットへのポインタ</t>
+    <rPh sb="0" eb="1">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>セントウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スレッドローカルスタックリストの回収用スタックリストの先頭スロットへのポインタ</t>
+    <rPh sb="16" eb="18">
+      <t>カイシュウ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>セントウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ハザード開放待ちのスロットを保持するスレッドローカルスタックの先頭スロットへのポインタ（スレッドローカル）</t>
+    <rPh sb="4" eb="7">
+      <t>カイホウマ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>セントウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>chunk_header_multi_slot</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>オーナーとなっているchunk_header_multi_slotへのポインタ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットデータへのポインタ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>各種のスタックリストで共用される次のスロットへのポインタ。nullptrなら割り当て中</t>
+    <rPh sb="0" eb="2">
+      <t>カクシュ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>キョウヨウ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>チュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>back_offset</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>offset_to_mgr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロット集合の管理情報</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>（この要素の先頭アドレスに対する飽和演算を考慮した（減算ではなく）加算演算でoffset_to_mgrのアドレスが算出できるoffset値。）</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>（この要素の先頭アドレスに対する飽和演算を考慮した（減算ではなく）加算演算で「スロット集合の管理情報」のアドレスが算出できるoffset値。）</t>
+  </si>
+  <si>
+    <t>padding_for_alignment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「スロット集合の管理情報」へのオフセット(std::uintptr_t)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>offset_to_mgrへのオフセット(std::uintptr_t)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>offset_to_mgrに対するチェック値(std::uintptr_t) （コンパイルオプション）</t>
+    <rPh sb="14" eb="15">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>オーバーラン書き込み検出のためのpaddingバッファ。1byte以上を確保する。</t>
+    <rPh sb="6" eb="7">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ケンシュツ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>カクホ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>alloc_size</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「割り当てるメモリ領域本体」のアライメント要求に従ってサイズが可変(ゼロ以上)となる。</t>
+    <rPh sb="1" eb="2">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="9" eb="13">
+      <t>リョウイキホンタイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ヨウキュウ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>カヘン</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>イジョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>この個別割り当てスロットの全体サイズ(offset_to_mgr～padding)</t>
+    <rPh sb="2" eb="5">
+      <t>コベツワ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ゼンタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>常に１</t>
+    <rPh sb="0" eb="1">
+      <t>ツネ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bt_info</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>（コンパイルオプション）allocation時のバックトレース情報</t>
+    <rPh sb="22" eb="23">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>（コンパイルオプション）deallocation時のバックトレース情報</t>
+    <rPh sb="24" eb="25">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>tail_padding</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -331,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -349,6 +617,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -3272,6 +3544,2524 @@
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
             <a:t>で確保された領域であることを示す。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>493059</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4482</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="左中かっこ 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F388BE00-2625-8547-4780-729978B682C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10197353" y="1696571"/>
+          <a:ext cx="307041" cy="877420"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 30208"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1695450</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>6163</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>493059</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="直線矢印コネクタ 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E14F822-1896-744D-E1DD-DCE41CFD6B57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="2" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7589744" y="2135281"/>
+          <a:ext cx="2607609" cy="1058956"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1914525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="直線矢印コネクタ 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2023659-9BA9-5311-9D3C-938DC6D356C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3971925" y="2238375"/>
+          <a:ext cx="1943100" cy="904875"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2362200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="フリーフォーム: 図形 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{497CA8F9-7136-AB9D-EA3C-6997FF82171A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1057275" y="361950"/>
+          <a:ext cx="13401675" cy="1438275"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 13020675 w 13277850"/>
+            <a:gd name="connsiteY0" fmla="*/ 1438275 h 1438275"/>
+            <a:gd name="connsiteX1" fmla="*/ 13277850 w 13277850"/>
+            <a:gd name="connsiteY1" fmla="*/ 1266825 h 1438275"/>
+            <a:gd name="connsiteX2" fmla="*/ 13277850 w 13277850"/>
+            <a:gd name="connsiteY2" fmla="*/ 828675 h 1438275"/>
+            <a:gd name="connsiteX3" fmla="*/ 11896725 w 13277850"/>
+            <a:gd name="connsiteY3" fmla="*/ 0 h 1438275"/>
+            <a:gd name="connsiteX4" fmla="*/ 133350 w 13277850"/>
+            <a:gd name="connsiteY4" fmla="*/ 0 h 1438275"/>
+            <a:gd name="connsiteX5" fmla="*/ 0 w 13277850"/>
+            <a:gd name="connsiteY5" fmla="*/ 133350 h 1438275"/>
+            <a:gd name="connsiteX6" fmla="*/ 0 w 13277850"/>
+            <a:gd name="connsiteY6" fmla="*/ 323850 h 1438275"/>
+            <a:gd name="connsiteX7" fmla="*/ 123825 w 13277850"/>
+            <a:gd name="connsiteY7" fmla="*/ 447675 h 1438275"/>
+            <a:gd name="connsiteX8" fmla="*/ 314325 w 13277850"/>
+            <a:gd name="connsiteY8" fmla="*/ 447675 h 1438275"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="13277850" h="1438275">
+              <a:moveTo>
+                <a:pt x="13020675" y="1438275"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="13277850" y="1266825"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="13277850" y="828675"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="11896725" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="133350" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="133350"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="323850"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="123825" y="447675"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="314325" y="447675"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>481853</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4482</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>200026</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="左中かっこ 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0937376B-7E0A-4DC3-ACEF-228F81EBAF16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10186147" y="3118038"/>
+          <a:ext cx="318247" cy="623047"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 30208"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1619250</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>481853</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>123827</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="直線矢印コネクタ 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29737DBD-91AE-4519-9562-430F0C0AE046}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="10" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7513544" y="3429561"/>
+          <a:ext cx="2672603" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>14288</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114304</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>157166</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="左中かっこ 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24E10E4A-375D-49C1-BA21-711A2CCCA881}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="20726400" y="5605467"/>
+          <a:ext cx="280987" cy="5967412"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 29610"/>
+            <a:gd name="adj2" fmla="val 93097"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>133357</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>981075</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>176219</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="左中かっこ 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C8532DE-DDC9-465B-92FE-205E2EE81A71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="12106275" y="7586670"/>
+          <a:ext cx="280987" cy="4424362"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 29610"/>
+            <a:gd name="adj2" fmla="val 48808"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>44822</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133358</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>661146</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>176220</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="左中かっこ 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{356E2CA0-EE4A-4887-AB93-BCD28B3514CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="14232450" y="1140906"/>
+          <a:ext cx="278186" cy="7698442"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 29610"/>
+            <a:gd name="adj2" fmla="val 54402"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>171457</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1590673</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>214319</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="左中かっこ 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{001313B0-1613-43E0-B046-AAA0503FBB96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="13137355" y="8093876"/>
+          <a:ext cx="280987" cy="1581149"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 29610"/>
+            <a:gd name="adj2" fmla="val 50162"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>219074</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="吹き出し: 角を丸めた四角形 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{814FD68E-645B-481A-BEE0-B9BBE2907EBA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12744450" y="9267824"/>
+          <a:ext cx="2447925" cy="304801"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -29380"/>
+            <a:gd name="adj2" fmla="val -106562"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>struct array_</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>slot_sheader</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1664634</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>108136</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>174811</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="吹き出し: 角を丸めた四角形 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81E49C5E-6A15-4D2D-8A31-65C2A43A7BB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7558928" y="10944224"/>
+          <a:ext cx="3118597" cy="301999"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 109755"/>
+            <a:gd name="adj2" fmla="val -252451"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>std::size_t get_slot_header_size()</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>22414</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>32504</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1086971</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>75366</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="左中かっこ 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{327FC85C-D93A-4A6F-A17B-989A62AAF5D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="16260717" y="8267848"/>
+          <a:ext cx="278186" cy="4538380"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 29610"/>
+            <a:gd name="adj2" fmla="val 48808"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>248771</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>154079</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>687482</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>211230</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="吹き出し: 角を丸めた四角形 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58C56E05-8AB7-4694-A3E5-CFD87C6C58B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11869271" y="11225491"/>
+          <a:ext cx="2904005" cy="998445"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 61446"/>
+            <a:gd name="adj2" fmla="val -152346"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>170890</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>102533</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1242732</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="吹き出し: 角を丸めた四角形 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC57F01F-C93B-448E-9E9F-48D9F37F5D45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24021490" y="10103783"/>
+          <a:ext cx="2443442" cy="849967"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -69663"/>
+            <a:gd name="adj2" fmla="val -111562"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="0" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>必ず、１</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>byte</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>以上の</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>padding</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>を入れる。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2400301</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1562101</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="フリーフォーム: 図形 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23E53456-37AD-6A06-B1A4-1A519BE0F2E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4457701" y="1285875"/>
+          <a:ext cx="9582150" cy="3667125"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 7962900"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 3667125"/>
+            <a:gd name="connsiteX1" fmla="*/ 2038350 w 7962900"/>
+            <a:gd name="connsiteY1" fmla="*/ 0 h 3667125"/>
+            <a:gd name="connsiteX2" fmla="*/ 4705350 w 7962900"/>
+            <a:gd name="connsiteY2" fmla="*/ 2667000 h 3667125"/>
+            <a:gd name="connsiteX3" fmla="*/ 7962900 w 7962900"/>
+            <a:gd name="connsiteY3" fmla="*/ 3457575 h 3667125"/>
+            <a:gd name="connsiteX4" fmla="*/ 7962900 w 7962900"/>
+            <a:gd name="connsiteY4" fmla="*/ 3667125 h 3667125"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="7962900" h="3667125">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2038350" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="4705350" y="2667000"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="7962900" y="3457575"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="7962900" y="3667125"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1771650</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>549173</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114304</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="直線矢印コネクタ 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D7D753A-751D-4376-BDCC-C840847C819F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="13" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7667625" y="4638675"/>
+          <a:ext cx="3368573" cy="714379"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>44823</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>98621</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>981075</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>141483</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="左中かっこ 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{259FEE8E-71B0-49A4-BD2A-CC4C75D14025}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="11759033" y="10000558"/>
+          <a:ext cx="278186" cy="6382311"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 29610"/>
+            <a:gd name="adj2" fmla="val 48808"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1664634</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>108136</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>174811</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="吹き出し: 角を丸めた四角形 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAA28D53-78E5-4761-82D5-8FF414EA3CC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7558928" y="10944224"/>
+          <a:ext cx="3141009" cy="301999"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 87683"/>
+            <a:gd name="adj2" fmla="val 614523"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>std::size_t get_slot_header_size()</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>67234</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>117670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1075765</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>160533</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="左中かっこ 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4C95586-5A98-487E-B701-2DB332715B1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="16277524" y="10498939"/>
+          <a:ext cx="278186" cy="4482354"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 29610"/>
+            <a:gd name="adj2" fmla="val 48808"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>239245</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>677956</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="吹き出し: 角を丸めた四角形 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11B3CBEB-0E41-4FEA-960C-D55F471230B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11859745" y="11233336"/>
+          <a:ext cx="2904005" cy="998445"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 59306"/>
+            <a:gd name="adj2" fmla="val 136708"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>呼び出し側が指定したアライメント値か、デフォルトのアライメント値の最小公倍数でアライメントされる。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>33617</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>76203</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1590675</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>119065</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="左中かっこ 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62C9655B-F55C-441D-8E8D-FE9984FE6B60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="12170289" y="12570061"/>
+          <a:ext cx="278185" cy="3551705"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 29610"/>
+            <a:gd name="adj2" fmla="val 50162"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>104765</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>171441</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="吹き出し: 角を丸めた四角形 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87D26FEA-4D45-4109-9555-49E80B4CD03E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11849100" y="12963515"/>
+          <a:ext cx="2447925" cy="304801"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -10314"/>
+            <a:gd name="adj2" fmla="val 80937"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>struct alloc_</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>slot_sheader</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>33336</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>171457</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>819149</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>214319</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="左中かっこ 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{797847BF-80DD-4D9F-B41C-710FD2C4C47A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="11344274" y="7920044"/>
+          <a:ext cx="280987" cy="1928813"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 29610"/>
+            <a:gd name="adj2" fmla="val 50162"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609601</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="吹き出し: 角を丸めた四角形 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8173D203-A307-4EFA-8600-2F4E8A69560A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9963151" y="9410699"/>
+          <a:ext cx="1828800" cy="304801"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 32599"/>
+            <a:gd name="adj2" fmla="val -144062"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>struct </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>slot_mheader</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>17369</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>85732</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>750794</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>128594</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="左中かっこ 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3374191F-B3EE-4E14-A9F0-0C15FC75A865}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="9428209" y="13467657"/>
+          <a:ext cx="278185" cy="1775572"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 29610"/>
+            <a:gd name="adj2" fmla="val 50162"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>197785</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>98050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>164726</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="吹き出し: 角を丸めた四角形 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{326C2C19-17ED-4D49-AC0E-32FAD03652CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8859932" y="13758021"/>
+          <a:ext cx="1827119" cy="301999"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 307"/>
+            <a:gd name="adj2" fmla="val 93437"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>struct </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>slot_mheader</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>7284</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>31932</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>456080</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="吹き出し: 角を丸めた四角形 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{341DA94B-8E6C-49BD-8333-93C02E911929}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5901578" y="14868520"/>
+          <a:ext cx="2533090" cy="2702303"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 83913"/>
+            <a:gd name="adj2" fmla="val -54506"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>の場合、スロットの確保が個別に</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>allocator</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>で確保されたことを示す。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>ゼロは、未初期化状態を意味するものとする。よって、不正値とする。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>解放処理等では、何もしないで、放置する。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2476500</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>204107</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="正方形/長方形 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E38D7D92-F3B3-E293-3F7C-AEF5AAB28686}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4527176" y="13603941"/>
+          <a:ext cx="15178368" cy="6143225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2209160</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1255060</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="正方形/長方形 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C74769D7-E8F6-D6B7-861E-CFBB897DDE55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4259836" y="13574326"/>
+          <a:ext cx="2889518" cy="634733"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>個別確保された場合のスロット構造</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>261257</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>220436</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>397329</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>40821</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="正方形/長方形 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44418142-7D4B-4CC4-82A5-651932375453}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8901793" y="4615543"/>
+          <a:ext cx="15131143" cy="5698671"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1553687</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>545520</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="正方形/長方形 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{020EC76F-D83A-4388-830D-2E06E9FEC38D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7447981" y="6555441"/>
+          <a:ext cx="1759686" cy="874059"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>chunk_header_multi_slot</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>で確保されたスロット配列の場合の構造</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>109818</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>127185</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>548529</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>184336</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="吹き出し: 角を丸めた四角形 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30B28C81-B11C-4FC4-ACFD-8827EA36245A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15204142" y="11198597"/>
+          <a:ext cx="2904005" cy="998445"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -15729"/>
+            <a:gd name="adj2" fmla="val -99596"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>116542</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>122703</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>555253</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>179854</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="吹き出し: 角を丸めた四角形 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3996276-B069-4063-9933-66002428C44D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15210866" y="11194115"/>
+          <a:ext cx="2904005" cy="998445"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -15343"/>
+            <a:gd name="adj2" fmla="val 88956"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>共通構造</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3092824</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>224118</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1782296</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>102538</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="吹き出し: 角を丸めた四角形 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8D43D6B-B709-4EF9-A5FB-392A888B4C09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5143500" y="8001000"/>
+          <a:ext cx="2533090" cy="2702303"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 161772"/>
+            <a:gd name="adj2" fmla="val -44139"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>の場合、スロットの確保が個別に</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>allocator</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>で確保されたことを示す。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>ゼロは、未初期化状態を意味するものとする。よって、不正値とする。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>解放処理等では、何もしないで、放置する。</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3546,8 +6336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView topLeftCell="K28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P59" sqref="P32:Y59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -3812,4 +6602,543 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FCA077-D2DC-4602-9CF2-A8F5DAEA3F68}">
+  <dimension ref="C4:O78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O74" sqref="O74"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <cols>
+    <col min="4" max="4" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.875" customWidth="1"/>
+    <col min="6" max="6" width="27.375" customWidth="1"/>
+    <col min="8" max="8" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="11.125" customWidth="1"/>
+    <col min="12" max="12" width="21.125" customWidth="1"/>
+    <col min="13" max="13" width="13.25" customWidth="1"/>
+    <col min="14" max="14" width="32.375" customWidth="1"/>
+    <col min="15" max="15" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:10">
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" ht="37.5">
+      <c r="D5" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10">
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10">
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10">
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10">
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10">
+      <c r="J10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10">
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10">
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10">
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10">
+      <c r="F16" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="6:15">
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="6:15">
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="6:15">
+      <c r="F19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="6:15">
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="6:15">
+      <c r="F21" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="6:15">
+      <c r="F22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="6:15">
+      <c r="F23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="6:15">
+      <c r="J24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="6:15">
+      <c r="J25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" t="s">
+        <v>33</v>
+      </c>
+      <c r="L25" t="s">
+        <v>33</v>
+      </c>
+      <c r="M25" t="s">
+        <v>33</v>
+      </c>
+      <c r="O25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="6:15">
+      <c r="J26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" t="s">
+        <v>34</v>
+      </c>
+      <c r="L26" t="s">
+        <v>34</v>
+      </c>
+      <c r="M26" t="s">
+        <v>34</v>
+      </c>
+      <c r="O26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="6:15">
+      <c r="J27" t="s">
+        <v>34</v>
+      </c>
+      <c r="K27" t="s">
+        <v>34</v>
+      </c>
+      <c r="L27" t="s">
+        <v>34</v>
+      </c>
+      <c r="M27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="6:15">
+      <c r="J28" t="s">
+        <v>34</v>
+      </c>
+      <c r="K28" t="s">
+        <v>34</v>
+      </c>
+      <c r="L28" t="s">
+        <v>34</v>
+      </c>
+      <c r="M28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="6:15">
+      <c r="J29" t="s">
+        <v>34</v>
+      </c>
+      <c r="K29" t="s">
+        <v>34</v>
+      </c>
+      <c r="L29" t="s">
+        <v>34</v>
+      </c>
+      <c r="M29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="6:15">
+      <c r="J30" t="s">
+        <v>34</v>
+      </c>
+      <c r="K30" t="s">
+        <v>34</v>
+      </c>
+      <c r="L30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="6:15">
+      <c r="J31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K31" t="s">
+        <v>34</v>
+      </c>
+      <c r="L31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="6:15">
+      <c r="J32" t="s">
+        <v>34</v>
+      </c>
+      <c r="K32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="10:11">
+      <c r="J33" t="s">
+        <v>34</v>
+      </c>
+      <c r="K33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="10:11">
+      <c r="J34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="10:11">
+      <c r="J35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="8:15">
+      <c r="H62" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K62" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="L62" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M62" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="N62" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O62" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="8:15">
+      <c r="H63" t="s">
+        <v>33</v>
+      </c>
+      <c r="I63" t="s">
+        <v>33</v>
+      </c>
+      <c r="J63" t="s">
+        <v>33</v>
+      </c>
+      <c r="K63" t="s">
+        <v>33</v>
+      </c>
+      <c r="L63" t="s">
+        <v>33</v>
+      </c>
+      <c r="M63" t="s">
+        <v>33</v>
+      </c>
+      <c r="O63" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="8:15">
+      <c r="H64" t="s">
+        <v>34</v>
+      </c>
+      <c r="I64" t="s">
+        <v>34</v>
+      </c>
+      <c r="J64" t="s">
+        <v>34</v>
+      </c>
+      <c r="K64" t="s">
+        <v>34</v>
+      </c>
+      <c r="L64" t="s">
+        <v>34</v>
+      </c>
+      <c r="M64" t="s">
+        <v>34</v>
+      </c>
+      <c r="O64" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="8:13">
+      <c r="H65" t="s">
+        <v>34</v>
+      </c>
+      <c r="I65" t="s">
+        <v>34</v>
+      </c>
+      <c r="J65" t="s">
+        <v>34</v>
+      </c>
+      <c r="K65" t="s">
+        <v>34</v>
+      </c>
+      <c r="L65" t="s">
+        <v>34</v>
+      </c>
+      <c r="M65" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="8:13">
+      <c r="H66" t="s">
+        <v>34</v>
+      </c>
+      <c r="I66" t="s">
+        <v>34</v>
+      </c>
+      <c r="J66" t="s">
+        <v>34</v>
+      </c>
+      <c r="K66" t="s">
+        <v>34</v>
+      </c>
+      <c r="L66" t="s">
+        <v>34</v>
+      </c>
+      <c r="M66" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" spans="8:13">
+      <c r="H67" t="s">
+        <v>34</v>
+      </c>
+      <c r="I67" t="s">
+        <v>34</v>
+      </c>
+      <c r="J67" t="s">
+        <v>34</v>
+      </c>
+      <c r="K67" t="s">
+        <v>34</v>
+      </c>
+      <c r="L67" t="s">
+        <v>34</v>
+      </c>
+      <c r="M67" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="8:13">
+      <c r="H68" t="s">
+        <v>34</v>
+      </c>
+      <c r="I68" t="s">
+        <v>34</v>
+      </c>
+      <c r="J68" t="s">
+        <v>34</v>
+      </c>
+      <c r="K68" t="s">
+        <v>34</v>
+      </c>
+      <c r="L68" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="69" spans="8:13">
+      <c r="H69" t="s">
+        <v>34</v>
+      </c>
+      <c r="I69" t="s">
+        <v>34</v>
+      </c>
+      <c r="J69" t="s">
+        <v>34</v>
+      </c>
+      <c r="K69" t="s">
+        <v>34</v>
+      </c>
+      <c r="L69" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="8:13">
+      <c r="H70" t="s">
+        <v>34</v>
+      </c>
+      <c r="I70" t="s">
+        <v>34</v>
+      </c>
+      <c r="J70" t="s">
+        <v>34</v>
+      </c>
+      <c r="K70" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="8:13">
+      <c r="H71" t="s">
+        <v>34</v>
+      </c>
+      <c r="I71" t="s">
+        <v>34</v>
+      </c>
+      <c r="J71" t="s">
+        <v>34</v>
+      </c>
+      <c r="K71" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="72" spans="8:13">
+      <c r="H72" t="s">
+        <v>34</v>
+      </c>
+      <c r="I72" t="s">
+        <v>34</v>
+      </c>
+      <c r="J72" t="s">
+        <v>34</v>
+      </c>
+      <c r="K72" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="73" spans="8:13">
+      <c r="H73" t="s">
+        <v>34</v>
+      </c>
+      <c r="I73" t="s">
+        <v>34</v>
+      </c>
+      <c r="J73" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="74" spans="8:13">
+      <c r="H74" t="s">
+        <v>34</v>
+      </c>
+      <c r="I74" t="s">
+        <v>34</v>
+      </c>
+      <c r="J74" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="75" spans="8:13">
+      <c r="H75" t="s">
+        <v>34</v>
+      </c>
+      <c r="I75" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" spans="8:13">
+      <c r="H76" t="s">
+        <v>34</v>
+      </c>
+      <c r="I76" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="77" spans="8:13">
+      <c r="H77" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="78" spans="8:13">
+      <c r="H78" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add slot array source code files
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/Design_general_mem_alloc.xlsx
+++ b/libalconcurrent/doc/Design_general_mem_alloc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA293FE0-07E7-4FEE-9112-5FA60D7085B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C8BB90-33AB-49D2-913C-14D6D3009A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="72">
   <si>
     <t>param_chunk_allocation</t>
   </si>
@@ -543,12 +543,37 @@
     <t>tail_padding</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>offset_to_assignment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>slot_mheaderから「割り当てるメモリ領域本体」へのオフセット</t>
+    <rPh sb="15" eb="16">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="23" eb="27">
+      <t>リョウイキホンタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>offset_to_tail_padding</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>slot_mheaderからtail_paddingへのオフセット</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,6 +586,14 @@
       <name val="Yu Gothic"/>
       <family val="3"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -599,7 +632,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -620,7 +653,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -3732,7 +3766,7 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>2362200</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -3994,7 +4028,7 @@
       <xdr:rowOff>114304</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>157166</xdr:rowOff>
@@ -4051,13 +4085,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>681038</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>133357</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>981075</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>176219</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4116,7 +4150,7 @@
       <xdr:rowOff>133358</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>661146</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>176220</xdr:rowOff>
@@ -4171,15 +4205,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>171457</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1590673</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>214319</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4232,15 +4266,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>219074</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4313,13 +4347,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1664634</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>108136</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>174811</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4386,15 +4420,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>22414</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>32504</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1086971</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>75366</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4449,13 +4483,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>248771</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>154079</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>687482</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>211230</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4511,15 +4545,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>170890</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>350185</xdr:colOff>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>102533</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>1242732</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>186019</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4535,13 +4569,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="24021490" y="10103783"/>
-          <a:ext cx="2443442" cy="849967"/>
+          <a:off x="20744891" y="5055533"/>
+          <a:ext cx="1886510" cy="838761"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -69663"/>
-            <a:gd name="adj2" fmla="val -111562"/>
+            <a:gd name="adj1" fmla="val -65505"/>
+            <a:gd name="adj2" fmla="val 40743"/>
             <a:gd name="adj3" fmla="val 16667"/>
           </a:avLst>
         </a:prstGeom>
@@ -4636,7 +4670,7 @@
       <xdr:rowOff>333375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1562101</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
@@ -4801,13 +4835,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>44823</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>98621</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>981075</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>141483</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4862,13 +4896,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1664634</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>108136</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>174811</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4935,15 +4969,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>67234</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>117670</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1075765</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>160533</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4998,13 +5032,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>239245</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>677956</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>219075</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5063,15 +5097,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>33617</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>33616</xdr:colOff>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>76203</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1590675</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1590674</xdr:colOff>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>119065</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5087,8 +5121,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="12170289" y="12570061"/>
-          <a:ext cx="278185" cy="3551705"/>
+          <a:off x="14019258" y="12715738"/>
+          <a:ext cx="278185" cy="3260352"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
@@ -5126,13 +5160,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>104765</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>171441</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5204,15 +5238,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>33336</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>171457</xdr:rowOff>
+      <xdr:colOff>33335</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>171455</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>819149</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>214319</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>818029</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>214317</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5227,8 +5261,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="11344274" y="7920044"/>
-          <a:ext cx="280987" cy="1928813"/>
+          <a:off x="12209648" y="6977907"/>
+          <a:ext cx="278185" cy="3630988"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
@@ -5266,13 +5300,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>609601</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>161926</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5344,15 +5378,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>17369</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>85732</xdr:rowOff>
+      <xdr:colOff>17368</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>85733</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>750794</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>128594</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>806822</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>128595</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5367,8 +5401,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="9428209" y="13467657"/>
-          <a:ext cx="278185" cy="1775572"/>
+          <a:off x="10425532" y="12470334"/>
+          <a:ext cx="278185" cy="3770219"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
@@ -5406,13 +5440,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>197785</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>98050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>209551</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>164726</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5485,13 +5519,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>7284</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>31932</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>456080</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>145676</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5584,13 +5618,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2476500</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>179294</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>204107</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5648,13 +5682,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2209160</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>149679</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1255060</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>78441</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5715,9 +5749,9 @@
       <xdr:rowOff>220436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>397329</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>40821</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5840,15 +5874,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>109818</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>127185</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>548529</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>184336</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5904,15 +5938,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>116542</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>122703</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>555253</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>179854</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5973,13 +6007,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>3092824</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>224118</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1782296</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>102538</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6606,10 +6640,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FCA077-D2DC-4602-9CF2-A8F5DAEA3F68}">
-  <dimension ref="C4:O78"/>
+  <dimension ref="C4:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O74" sqref="O74"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -6620,11 +6654,11 @@
     <col min="8" max="8" width="13.625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="11.125" customWidth="1"/>
-    <col min="12" max="12" width="21.125" customWidth="1"/>
-    <col min="13" max="13" width="13.25" customWidth="1"/>
-    <col min="14" max="14" width="32.375" customWidth="1"/>
-    <col min="15" max="15" width="14.5" customWidth="1"/>
+    <col min="11" max="13" width="11.125" customWidth="1"/>
+    <col min="14" max="14" width="21.125" customWidth="1"/>
+    <col min="15" max="15" width="13.25" customWidth="1"/>
+    <col min="16" max="16" width="32.375" customWidth="1"/>
+    <col min="17" max="17" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:10">
@@ -6700,62 +6734,68 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="6:15">
+    <row r="17" spans="6:17">
       <c r="F17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="6:15">
+    <row r="18" spans="6:17">
       <c r="F18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="6:15">
+    <row r="19" spans="6:17">
       <c r="F19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="6:15">
+    <row r="20" spans="6:17">
       <c r="F20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="6:15">
+    <row r="21" spans="6:17">
       <c r="F21" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="6:15">
+    <row r="22" spans="6:17">
       <c r="F22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="6:15">
+    <row r="23" spans="6:17">
       <c r="F23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="6:15">
+    <row r="24" spans="6:17">
       <c r="J24" s="5" t="s">
         <v>51</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="L24" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="N24" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="M24" s="5" t="s">
+      <c r="O24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="N24" s="5" t="s">
+      <c r="P24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="O24" s="5" t="s">
+      <c r="Q24" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="6:15">
+    <row r="25" spans="6:17">
       <c r="J25" t="s">
         <v>33</v>
       </c>
@@ -6768,11 +6808,17 @@
       <c r="M25" t="s">
         <v>33</v>
       </c>
+      <c r="N25" t="s">
+        <v>33</v>
+      </c>
       <c r="O25" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="6:15">
+      <c r="Q25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="6:17">
       <c r="J26" t="s">
         <v>34</v>
       </c>
@@ -6785,11 +6831,17 @@
       <c r="M26" t="s">
         <v>34</v>
       </c>
+      <c r="N26" t="s">
+        <v>34</v>
+      </c>
       <c r="O26" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q26" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="6:15">
+    <row r="27" spans="6:17">
       <c r="J27" t="s">
         <v>34</v>
       </c>
@@ -6802,8 +6854,14 @@
       <c r="M27" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="6:15">
+      <c r="N27" t="s">
+        <v>34</v>
+      </c>
+      <c r="O27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="6:17">
       <c r="J28" t="s">
         <v>34</v>
       </c>
@@ -6814,10 +6872,16 @@
         <v>34</v>
       </c>
       <c r="M28" t="s">
+        <v>34</v>
+      </c>
+      <c r="N28" t="s">
+        <v>34</v>
+      </c>
+      <c r="O28" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="6:15">
+    <row r="29" spans="6:17">
       <c r="J29" t="s">
         <v>34</v>
       </c>
@@ -6828,10 +6892,16 @@
         <v>34</v>
       </c>
       <c r="M29" t="s">
+        <v>34</v>
+      </c>
+      <c r="N29" t="s">
+        <v>34</v>
+      </c>
+      <c r="O29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="6:15">
+    <row r="30" spans="6:17">
       <c r="J30" t="s">
         <v>34</v>
       </c>
@@ -6841,8 +6911,14 @@
       <c r="L30" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" spans="6:15">
+      <c r="M30" t="s">
+        <v>34</v>
+      </c>
+      <c r="N30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="6:17">
       <c r="J31" t="s">
         <v>34</v>
       </c>
@@ -6850,288 +6926,472 @@
         <v>34</v>
       </c>
       <c r="L31" t="s">
+        <v>34</v>
+      </c>
+      <c r="M31" t="s">
+        <v>34</v>
+      </c>
+      <c r="N31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="6:15">
+    <row r="32" spans="6:17">
       <c r="J32" t="s">
         <v>34</v>
       </c>
       <c r="K32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="10:11">
+      <c r="L32" t="s">
+        <v>34</v>
+      </c>
+      <c r="M32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="10:13">
       <c r="J33" t="s">
         <v>34</v>
       </c>
       <c r="K33" t="s">
+        <v>34</v>
+      </c>
+      <c r="L33" t="s">
+        <v>34</v>
+      </c>
+      <c r="M33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="10:13">
+      <c r="J34" t="s">
+        <v>34</v>
+      </c>
+      <c r="K34" t="s">
+        <v>34</v>
+      </c>
+      <c r="L34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="10:13">
+      <c r="J35" t="s">
+        <v>34</v>
+      </c>
+      <c r="K35" t="s">
+        <v>34</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="10:13">
+      <c r="J36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="10:13">
+      <c r="J37" t="s">
+        <v>34</v>
+      </c>
+      <c r="K37" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="10:11">
-      <c r="J34" t="s">
+    <row r="38" spans="10:13">
+      <c r="J38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="10:11">
-      <c r="J35" t="s">
+    <row r="39" spans="10:13">
+      <c r="J39" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="8:15">
-      <c r="H62" s="5" t="s">
+    <row r="66" spans="8:17">
+      <c r="H66" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="I62" s="5" t="s">
+      <c r="I66" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J62" s="5" t="s">
+      <c r="J66" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K66" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L66" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K62" s="8" t="s">
+      <c r="M66" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="L62" s="5" t="s">
+      <c r="N66" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="M62" s="5" t="s">
+      <c r="O66" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="N62" s="5" t="s">
+      <c r="P66" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="O62" s="5" t="s">
+      <c r="Q66" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="8:15">
-      <c r="H63" t="s">
+    <row r="67" spans="8:17">
+      <c r="H67" t="s">
         <v>33</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I67" t="s">
         <v>33</v>
       </c>
-      <c r="J63" t="s">
+      <c r="J67" t="s">
         <v>33</v>
       </c>
-      <c r="K63" t="s">
+      <c r="K67" t="s">
         <v>33</v>
       </c>
-      <c r="L63" t="s">
+      <c r="L67" t="s">
         <v>33</v>
       </c>
-      <c r="M63" t="s">
+      <c r="M67" t="s">
         <v>33</v>
       </c>
-      <c r="O63" t="s">
+      <c r="N67" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="64" spans="8:15">
-      <c r="H64" t="s">
-        <v>34</v>
-      </c>
-      <c r="I64" t="s">
-        <v>34</v>
-      </c>
-      <c r="J64" t="s">
-        <v>34</v>
-      </c>
-      <c r="K64" t="s">
-        <v>34</v>
-      </c>
-      <c r="L64" t="s">
-        <v>34</v>
-      </c>
-      <c r="M64" t="s">
-        <v>34</v>
-      </c>
-      <c r="O64" t="s">
+      <c r="O67" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="8:17">
+      <c r="H68" t="s">
+        <v>34</v>
+      </c>
+      <c r="I68" t="s">
+        <v>34</v>
+      </c>
+      <c r="J68" t="s">
+        <v>34</v>
+      </c>
+      <c r="K68" t="s">
+        <v>34</v>
+      </c>
+      <c r="L68" t="s">
+        <v>34</v>
+      </c>
+      <c r="M68" t="s">
+        <v>34</v>
+      </c>
+      <c r="N68" t="s">
+        <v>34</v>
+      </c>
+      <c r="O68" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q68" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="8:13">
-      <c r="H65" t="s">
-        <v>34</v>
-      </c>
-      <c r="I65" t="s">
-        <v>34</v>
-      </c>
-      <c r="J65" t="s">
-        <v>34</v>
-      </c>
-      <c r="K65" t="s">
-        <v>34</v>
-      </c>
-      <c r="L65" t="s">
-        <v>34</v>
-      </c>
-      <c r="M65" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="66" spans="8:13">
-      <c r="H66" t="s">
-        <v>34</v>
-      </c>
-      <c r="I66" t="s">
-        <v>34</v>
-      </c>
-      <c r="J66" t="s">
-        <v>34</v>
-      </c>
-      <c r="K66" t="s">
-        <v>34</v>
-      </c>
-      <c r="L66" t="s">
-        <v>34</v>
-      </c>
-      <c r="M66" t="s">
+    <row r="69" spans="8:17">
+      <c r="H69" t="s">
+        <v>34</v>
+      </c>
+      <c r="I69" t="s">
+        <v>34</v>
+      </c>
+      <c r="J69" t="s">
+        <v>34</v>
+      </c>
+      <c r="K69" t="s">
+        <v>34</v>
+      </c>
+      <c r="L69" t="s">
+        <v>34</v>
+      </c>
+      <c r="M69" t="s">
+        <v>34</v>
+      </c>
+      <c r="N69" t="s">
+        <v>34</v>
+      </c>
+      <c r="O69" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="8:17">
+      <c r="H70" t="s">
+        <v>34</v>
+      </c>
+      <c r="I70" t="s">
+        <v>34</v>
+      </c>
+      <c r="J70" t="s">
+        <v>34</v>
+      </c>
+      <c r="K70" t="s">
+        <v>34</v>
+      </c>
+      <c r="L70" t="s">
+        <v>34</v>
+      </c>
+      <c r="M70" t="s">
+        <v>34</v>
+      </c>
+      <c r="N70" t="s">
+        <v>34</v>
+      </c>
+      <c r="O70" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="8:13">
-      <c r="H67" t="s">
-        <v>34</v>
-      </c>
-      <c r="I67" t="s">
-        <v>34</v>
-      </c>
-      <c r="J67" t="s">
-        <v>34</v>
-      </c>
-      <c r="K67" t="s">
-        <v>34</v>
-      </c>
-      <c r="L67" t="s">
-        <v>34</v>
-      </c>
-      <c r="M67" t="s">
+    <row r="71" spans="8:17">
+      <c r="H71" t="s">
+        <v>34</v>
+      </c>
+      <c r="I71" t="s">
+        <v>34</v>
+      </c>
+      <c r="J71" t="s">
+        <v>34</v>
+      </c>
+      <c r="K71" t="s">
+        <v>34</v>
+      </c>
+      <c r="L71" t="s">
+        <v>34</v>
+      </c>
+      <c r="M71" t="s">
+        <v>34</v>
+      </c>
+      <c r="N71" t="s">
+        <v>34</v>
+      </c>
+      <c r="O71" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="8:13">
-      <c r="H68" t="s">
-        <v>34</v>
-      </c>
-      <c r="I68" t="s">
-        <v>34</v>
-      </c>
-      <c r="J68" t="s">
-        <v>34</v>
-      </c>
-      <c r="K68" t="s">
-        <v>34</v>
-      </c>
-      <c r="L68" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="69" spans="8:13">
-      <c r="H69" t="s">
-        <v>34</v>
-      </c>
-      <c r="I69" t="s">
-        <v>34</v>
-      </c>
-      <c r="J69" t="s">
-        <v>34</v>
-      </c>
-      <c r="K69" t="s">
-        <v>34</v>
-      </c>
-      <c r="L69" t="s">
+    <row r="72" spans="8:17">
+      <c r="H72" t="s">
+        <v>34</v>
+      </c>
+      <c r="I72" t="s">
+        <v>34</v>
+      </c>
+      <c r="J72" t="s">
+        <v>34</v>
+      </c>
+      <c r="K72" t="s">
+        <v>34</v>
+      </c>
+      <c r="L72" t="s">
+        <v>34</v>
+      </c>
+      <c r="M72" t="s">
+        <v>34</v>
+      </c>
+      <c r="N72" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="8:17">
+      <c r="H73" t="s">
+        <v>34</v>
+      </c>
+      <c r="I73" t="s">
+        <v>34</v>
+      </c>
+      <c r="J73" t="s">
+        <v>34</v>
+      </c>
+      <c r="K73" t="s">
+        <v>34</v>
+      </c>
+      <c r="L73" t="s">
+        <v>34</v>
+      </c>
+      <c r="M73" t="s">
+        <v>34</v>
+      </c>
+      <c r="N73" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="8:13">
-      <c r="H70" t="s">
-        <v>34</v>
-      </c>
-      <c r="I70" t="s">
-        <v>34</v>
-      </c>
-      <c r="J70" t="s">
-        <v>34</v>
-      </c>
-      <c r="K70" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="71" spans="8:13">
-      <c r="H71" t="s">
-        <v>34</v>
-      </c>
-      <c r="I71" t="s">
-        <v>34</v>
-      </c>
-      <c r="J71" t="s">
-        <v>34</v>
-      </c>
-      <c r="K71" t="s">
+    <row r="74" spans="8:17">
+      <c r="H74" t="s">
+        <v>34</v>
+      </c>
+      <c r="I74" t="s">
+        <v>34</v>
+      </c>
+      <c r="J74" t="s">
+        <v>34</v>
+      </c>
+      <c r="K74" t="s">
+        <v>34</v>
+      </c>
+      <c r="L74" t="s">
+        <v>34</v>
+      </c>
+      <c r="M74" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="8:17">
+      <c r="H75" t="s">
+        <v>34</v>
+      </c>
+      <c r="I75" t="s">
+        <v>34</v>
+      </c>
+      <c r="J75" t="s">
+        <v>34</v>
+      </c>
+      <c r="K75" t="s">
+        <v>34</v>
+      </c>
+      <c r="L75" t="s">
+        <v>34</v>
+      </c>
+      <c r="M75" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="72" spans="8:13">
-      <c r="H72" t="s">
-        <v>34</v>
-      </c>
-      <c r="I72" t="s">
-        <v>34</v>
-      </c>
-      <c r="J72" t="s">
-        <v>34</v>
-      </c>
-      <c r="K72" t="s">
+    <row r="76" spans="8:17">
+      <c r="H76" t="s">
+        <v>34</v>
+      </c>
+      <c r="I76" t="s">
+        <v>34</v>
+      </c>
+      <c r="J76" t="s">
+        <v>34</v>
+      </c>
+      <c r="K76" t="s">
+        <v>34</v>
+      </c>
+      <c r="L76" t="s">
+        <v>34</v>
+      </c>
+      <c r="M76" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="73" spans="8:13">
-      <c r="H73" t="s">
-        <v>34</v>
-      </c>
-      <c r="I73" t="s">
-        <v>34</v>
-      </c>
-      <c r="J73" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="74" spans="8:13">
-      <c r="H74" t="s">
-        <v>34</v>
-      </c>
-      <c r="I74" t="s">
-        <v>34</v>
-      </c>
-      <c r="J74" t="s">
+    <row r="77" spans="8:17">
+      <c r="H77" t="s">
+        <v>34</v>
+      </c>
+      <c r="I77" t="s">
+        <v>34</v>
+      </c>
+      <c r="J77" t="s">
+        <v>34</v>
+      </c>
+      <c r="K77" t="s">
+        <v>34</v>
+      </c>
+      <c r="L77" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="78" spans="8:17">
+      <c r="H78" t="s">
+        <v>34</v>
+      </c>
+      <c r="I78" t="s">
+        <v>34</v>
+      </c>
+      <c r="J78" t="s">
+        <v>34</v>
+      </c>
+      <c r="K78" t="s">
+        <v>34</v>
+      </c>
+      <c r="L78" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="8:13">
-      <c r="H75" t="s">
-        <v>34</v>
-      </c>
-      <c r="I75" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="76" spans="8:13">
-      <c r="H76" t="s">
-        <v>34</v>
-      </c>
-      <c r="I76" t="s">
+    <row r="79" spans="8:17">
+      <c r="H79" t="s">
+        <v>34</v>
+      </c>
+      <c r="I79" t="s">
+        <v>34</v>
+      </c>
+      <c r="J79" t="s">
+        <v>34</v>
+      </c>
+      <c r="K79" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="80" spans="8:17">
+      <c r="H80" t="s">
+        <v>34</v>
+      </c>
+      <c r="I80" t="s">
+        <v>34</v>
+      </c>
+      <c r="J80" t="s">
+        <v>34</v>
+      </c>
+      <c r="K80" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="81" spans="8:10">
+      <c r="H81" t="s">
+        <v>34</v>
+      </c>
+      <c r="I81" t="s">
+        <v>34</v>
+      </c>
+      <c r="J81" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="82" spans="8:10">
+      <c r="H82" t="s">
+        <v>34</v>
+      </c>
+      <c r="I82" t="s">
+        <v>34</v>
+      </c>
+      <c r="J82" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="83" spans="8:10">
+      <c r="H83" t="s">
+        <v>34</v>
+      </c>
+      <c r="I83" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="84" spans="8:10">
+      <c r="H84" t="s">
+        <v>34</v>
+      </c>
+      <c r="I84" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="77" spans="8:13">
-      <c r="H77" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="78" spans="8:13">
-      <c r="H78" t="s">
+    <row r="85" spans="8:10">
+      <c r="H85" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="86" spans="8:10">
+      <c r="H86" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: change back trace information placement
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/Design_general_mem_alloc.xlsx
+++ b/libalconcurrent/doc/Design_general_mem_alloc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789F7CBE-BBA9-49B5-BFBF-22028D210B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DADF4C-087D-43F6-8577-26A2CE5239FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="69">
   <si>
     <t>param_chunk_allocation</t>
   </si>
@@ -457,10 +457,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>bt_info</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>（コンパイルオプション）allocation時のバックトレース情報</t>
     <rPh sb="22" eb="23">
       <t>ジ</t>
@@ -510,6 +506,17 @@
     </rPh>
     <rPh sb="49" eb="50">
       <t>ナド</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bt_info_</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>その他。。。</t>
+    <rPh sb="2" eb="3">
+      <t>ホカ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -3529,13 +3536,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>493059</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>4482</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>224116</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3550,8 +3557,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10197353" y="1696571"/>
-          <a:ext cx="307041" cy="877420"/>
+          <a:off x="10197353" y="1696570"/>
+          <a:ext cx="307041" cy="1127311"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
@@ -3590,7 +3597,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>1695450</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>6163</xdr:rowOff>
+      <xdr:rowOff>131108</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -3613,8 +3620,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7589744" y="2135281"/>
-          <a:ext cx="2607609" cy="1058956"/>
+          <a:off x="7589744" y="2260226"/>
+          <a:ext cx="2607609" cy="934011"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3902,75 +3909,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>44822</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>133358</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>1086972</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>176220</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="左中かっこ 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{356E2CA0-EE4A-4887-AB93-BCD28B3514CF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="15745246" y="-349478"/>
-          <a:ext cx="278186" cy="10679209"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftBrace">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 29610"/>
-            <a:gd name="adj2" fmla="val 54402"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>67235</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>56028</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>171456</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1590673</xdr:colOff>
+      <xdr:colOff>1590672</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>214318</xdr:rowOff>
     </xdr:to>
@@ -3987,8 +3933,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="14887714" y="8827301"/>
-          <a:ext cx="278185" cy="3226732"/>
+          <a:off x="15307934" y="9247521"/>
+          <a:ext cx="278185" cy="2386291"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
@@ -4025,15 +3971,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>289112</xdr:colOff>
+      <xdr:colOff>726141</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>207869</xdr:rowOff>
+      <xdr:rowOff>219075</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>274544</xdr:colOff>
+      <xdr:colOff>711573</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>36420</xdr:rowOff>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4048,7 +3994,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14486965" y="10808634"/>
+          <a:off x="14923994" y="10819840"/>
           <a:ext cx="2450726" cy="299198"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
@@ -4347,120 +4293,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2400301</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>333375</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>358588</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="フリーフォーム: 図形 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23E53456-37AD-6A06-B1A4-1A519BE0F2E6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4450977" y="1274669"/>
-          <a:ext cx="10957111" cy="3633507"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst>
-            <a:gd name="connsiteX0" fmla="*/ 0 w 7962900"/>
-            <a:gd name="connsiteY0" fmla="*/ 0 h 3667125"/>
-            <a:gd name="connsiteX1" fmla="*/ 2038350 w 7962900"/>
-            <a:gd name="connsiteY1" fmla="*/ 0 h 3667125"/>
-            <a:gd name="connsiteX2" fmla="*/ 4705350 w 7962900"/>
-            <a:gd name="connsiteY2" fmla="*/ 2667000 h 3667125"/>
-            <a:gd name="connsiteX3" fmla="*/ 7962900 w 7962900"/>
-            <a:gd name="connsiteY3" fmla="*/ 3457575 h 3667125"/>
-            <a:gd name="connsiteX4" fmla="*/ 7962900 w 7962900"/>
-            <a:gd name="connsiteY4" fmla="*/ 3667125 h 3667125"/>
-          </a:gdLst>
-          <a:ahLst/>
-          <a:cxnLst>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX0" y="connsiteY0"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX1" y="connsiteY1"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX2" y="connsiteY2"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX3" y="connsiteY3"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX4" y="connsiteY4"/>
-            </a:cxn>
-          </a:cxnLst>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="7962900" h="3667125">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="2038350" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="4705350" y="2667000"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="7962900" y="3457575"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="7962900" y="3667125"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1759324</xdr:colOff>
       <xdr:row>13</xdr:row>
@@ -4644,7 +4476,7 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>44822</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>76203</xdr:rowOff>
@@ -4668,8 +4500,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="14876508" y="13662635"/>
-          <a:ext cx="278185" cy="3249145"/>
+          <a:off x="15302331" y="14794429"/>
+          <a:ext cx="278186" cy="2397498"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
@@ -4705,14 +4537,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>291352</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>104765</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:colOff>209549</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>171441</xdr:rowOff>
     </xdr:to>
@@ -4729,8 +4561,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11849100" y="12963515"/>
-          <a:ext cx="2447925" cy="304801"/>
+          <a:off x="14489205" y="15412000"/>
+          <a:ext cx="2383491" cy="302000"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -4785,15 +4617,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>33335</xdr:colOff>
+      <xdr:colOff>33334</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>171455</xdr:rowOff>
+      <xdr:rowOff>171454</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>806823</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>795617</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>214317</xdr:rowOff>
+      <xdr:rowOff>214316</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4808,8 +4640,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="11778222" y="8350627"/>
-          <a:ext cx="278186" cy="2768135"/>
+          <a:off x="12198442" y="8636376"/>
+          <a:ext cx="278185" cy="3608577"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
@@ -4845,16 +4677,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>609601</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>620806</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:rowOff>101412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>161926</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>117102</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>168088</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4869,8 +4701,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9963151" y="9410699"/>
-          <a:ext cx="1828800" cy="304801"/>
+          <a:off x="11120718" y="10937500"/>
+          <a:ext cx="1490943" cy="302000"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -4930,8 +4762,8 @@
       <xdr:rowOff>85734</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>818027</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>795617</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>128596</xdr:rowOff>
     </xdr:to>
@@ -4948,8 +4780,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="11783965" y="14613180"/>
-          <a:ext cx="278186" cy="2779057"/>
+          <a:off x="12198583" y="14198562"/>
+          <a:ext cx="278186" cy="3608294"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
@@ -4985,16 +4817,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>197785</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>926167</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>98050</xdr:rowOff>
+      <xdr:rowOff>86844</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>209551</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>781051</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>164726</xdr:rowOff>
+      <xdr:rowOff>153520</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5009,8 +4841,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8859932" y="13758021"/>
-          <a:ext cx="1827119" cy="301999"/>
+          <a:off x="11426079" y="15394079"/>
+          <a:ext cx="1849531" cy="302000"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -6292,8 +6124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FCA077-D2DC-4602-9CF2-A8F5DAEA3F68}">
   <dimension ref="C4:R87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView tabSelected="1" topLeftCell="C40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -6355,6 +6187,11 @@
         <v>42</v>
       </c>
     </row>
+    <row r="11" spans="3:10">
+      <c r="J11" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="13" spans="3:10">
       <c r="F13" t="s">
         <v>48</v>
@@ -6380,11 +6217,6 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="6:18">
-      <c r="F18" t="s">
-        <v>32</v>
-      </c>
-    </row>
     <row r="24" spans="6:18">
       <c r="J24" s="5" t="s">
         <v>47</v>
@@ -6393,13 +6225,13 @@
         <v>29</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="O24" s="5" t="s">
         <v>51</v>
@@ -6411,7 +6243,7 @@
         <v>35</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="6:18">
@@ -6606,7 +6438,7 @@
         <v>34</v>
       </c>
       <c r="N33" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="10:14">
@@ -6622,9 +6454,6 @@
       <c r="M34" t="s">
         <v>34</v>
       </c>
-      <c r="N34" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="35" spans="10:14">
       <c r="J35" t="s">
@@ -6637,7 +6466,7 @@
         <v>34</v>
       </c>
       <c r="M35" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="10:14">
@@ -6651,7 +6480,7 @@
         <v>34</v>
       </c>
       <c r="M36" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="10:14">
@@ -6673,7 +6502,7 @@
         <v>34</v>
       </c>
       <c r="L38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="10:14">
@@ -6710,13 +6539,13 @@
         <v>29</v>
       </c>
       <c r="L69" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M69" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N69" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="N69" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="O69" s="5" t="s">
         <v>51</v>
@@ -6728,7 +6557,7 @@
         <v>35</v>
       </c>
       <c r="R69" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="10:18">
@@ -6923,7 +6752,7 @@
         <v>34</v>
       </c>
       <c r="N78" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="79" spans="10:18">
@@ -6939,9 +6768,6 @@
       <c r="M79" t="s">
         <v>34</v>
       </c>
-      <c r="N79" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="80" spans="10:18">
       <c r="J80" t="s">
@@ -6954,7 +6780,7 @@
         <v>34</v>
       </c>
       <c r="M80" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="81" spans="10:13">
@@ -6968,7 +6794,7 @@
         <v>34</v>
       </c>
       <c r="M81" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="82" spans="10:13">
@@ -6990,7 +6816,7 @@
         <v>34</v>
       </c>
       <c r="L83" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="84" spans="10:13">
@@ -7016,7 +6842,7 @@
     </row>
     <row r="87" spans="10:13">
       <c r="J87" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: change slot_array_mgr design concept
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/Design_general_mem_alloc.xlsx
+++ b/libalconcurrent/doc/Design_general_mem_alloc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DADF4C-087D-43F6-8577-26A2CE5239FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388B858B-DB22-4AB3-9DCF-DAD88E50D0FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="73">
   <si>
     <t>param_chunk_allocation</t>
   </si>
@@ -517,6 +517,34 @@
     <t>その他。。。</t>
     <rPh sb="2" eb="3">
       <t>ホカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>back_offsetへのオフセット(std::uintptr_t)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0番スロットの管理情報</t>
+    <rPh sb="1" eb="2">
+      <t>バン</t>
+    </rPh>
+    <rPh sb="7" eb="11">
+      <t>カンリジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1番スロットの管理情報</t>
+    <rPh sb="1" eb="2">
+      <t>バン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n-1番スロットの管理情報</t>
+    <rPh sb="3" eb="4">
+      <t>バン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -576,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -597,6 +625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -3850,14 +3879,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>14288</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114304</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>58277</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>157166</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>829235</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>101139</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3872,8 +3901,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="20726400" y="5605467"/>
-          <a:ext cx="280987" cy="5967412"/>
+          <a:off x="12631551" y="1481985"/>
+          <a:ext cx="278185" cy="4512888"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
@@ -3910,15 +3939,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>56028</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>171456</xdr:rowOff>
+      <xdr:colOff>22408</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>171454</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1590672</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>214318</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>829234</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>214315</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3933,8 +3962,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="15307934" y="9247521"/>
-          <a:ext cx="278185" cy="2386291"/>
+          <a:off x="14484581" y="6742722"/>
+          <a:ext cx="278185" cy="806826"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
@@ -3970,16 +3999,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>726141</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>219075</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>737347</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>207869</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>711573</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1484779</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>36421</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3994,8 +4023,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14923994" y="10819840"/>
-          <a:ext cx="2450726" cy="299198"/>
+          <a:off x="14083553" y="7514104"/>
+          <a:ext cx="2450726" cy="299199"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -4051,13 +4080,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>22414</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>32504</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>1086971</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>75366</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4073,13 +4102,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="16260717" y="8267848"/>
-          <a:ext cx="278186" cy="4538380"/>
+          <a:off x="19319923" y="8940201"/>
+          <a:ext cx="278185" cy="5546910"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
             <a:gd name="adj1" fmla="val 29610"/>
-            <a:gd name="adj2" fmla="val 48808"/>
+            <a:gd name="adj2" fmla="val 90828"/>
           </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
@@ -4110,16 +4139,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>248771</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>154079</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>324970</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>100851</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>687482</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>211230</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>952499</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>65551</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4134,13 +4163,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11891683" y="12872755"/>
-          <a:ext cx="5458946" cy="998446"/>
+          <a:off x="14522823" y="12584204"/>
+          <a:ext cx="1479176" cy="670671"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 56930"/>
-            <a:gd name="adj2" fmla="val -162447"/>
+            <a:gd name="adj1" fmla="val 126701"/>
+            <a:gd name="adj2" fmla="val -150296"/>
             <a:gd name="adj3" fmla="val 16667"/>
           </a:avLst>
         </a:prstGeom>
@@ -4166,6 +4195,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>slot_container</a:t>
+          </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -4174,13 +4207,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>350185</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>102533</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>186019</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4294,15 +4327,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1759324</xdr:colOff>
+      <xdr:colOff>1580030</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>156883</xdr:rowOff>
+      <xdr:rowOff>112059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>755129</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114304</xdr:rowOff>
+      <xdr:colOff>325813</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>58278</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4319,8 +4352,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7653618" y="3462618"/>
-          <a:ext cx="3601423" cy="1840010"/>
+          <a:off x="7474324" y="3417794"/>
+          <a:ext cx="3351401" cy="181543"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4349,15 +4382,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>67234</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>117670</xdr:rowOff>
+      <xdr:colOff>44823</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>5612</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>1075765</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>160533</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1053354</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>48474</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4372,13 +4405,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="16277524" y="10498939"/>
-          <a:ext cx="278186" cy="4482354"/>
+          <a:off x="19314319" y="11294557"/>
+          <a:ext cx="278186" cy="5490884"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
             <a:gd name="adj1" fmla="val 29610"/>
-            <a:gd name="adj2" fmla="val 48808"/>
+            <a:gd name="adj2" fmla="val 90645"/>
           </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
@@ -4409,16 +4442,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>239245</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>291353</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>150719</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>677956</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>219075</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1058956</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>207870</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4433,13 +4466,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11882157" y="12880600"/>
-          <a:ext cx="5458946" cy="998446"/>
+          <a:off x="16954500" y="12398748"/>
+          <a:ext cx="2784662" cy="998446"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 56022"/>
-            <a:gd name="adj2" fmla="val 151298"/>
+            <a:gd name="adj1" fmla="val 13298"/>
+            <a:gd name="adj2" fmla="val 137830"/>
             <a:gd name="adj3" fmla="val 16667"/>
           </a:avLst>
         </a:prstGeom>
@@ -4478,13 +4511,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>44822</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>76203</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>1590673</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>119065</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4539,13 +4572,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>291352</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>104765</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>171441</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4617,15 +4650,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>33334</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:colOff>55746</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>171454</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>795617</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>214316</xdr:rowOff>
+      <xdr:colOff>818029</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>214315</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4640,7 +4673,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="12198442" y="8636376"/>
+          <a:off x="12220854" y="5341846"/>
           <a:ext cx="278185" cy="3608577"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
@@ -4678,15 +4711,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>620806</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>101412</xdr:rowOff>
+      <xdr:colOff>643218</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>67794</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>117102</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>168088</xdr:rowOff>
+      <xdr:colOff>139514</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4701,7 +4734,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11120718" y="10937500"/>
+          <a:off x="11143130" y="7609353"/>
           <a:ext cx="1490943" cy="302000"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
@@ -4758,13 +4791,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>33617</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>85734</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>795617</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>128596</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4819,13 +4852,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>926167</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>86844</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>781051</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>153520</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4898,7 +4931,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1183901</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>65550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -4978,11 +5011,11 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2476500</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>179294</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>90</xdr:row>
       <xdr:rowOff>204107</xdr:rowOff>
@@ -5042,13 +5075,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2209160</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>149679</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1255060</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>78441</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5105,13 +5138,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>261257</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>220436</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123264</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>397329</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>40821</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5127,8 +5160,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8901793" y="4615543"/>
-          <a:ext cx="15131143" cy="5698671"/>
+          <a:off x="8923404" y="3193676"/>
+          <a:ext cx="19197278" cy="8859851"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5167,16 +5200,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1553687</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>489127</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>67236</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>545520</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>123265</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>523107</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5191,8 +5224,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7447981" y="6555441"/>
-          <a:ext cx="1759686" cy="874059"/>
+          <a:off x="8467715" y="4078942"/>
+          <a:ext cx="1759686" cy="874058"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5234,16 +5267,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>109818</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>127185</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1264024</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>115979</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>548529</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>184336</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>593353</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>173130</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5258,13 +5291,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15204142" y="11198597"/>
-          <a:ext cx="2904005" cy="998445"/>
+          <a:off x="19944230" y="12364008"/>
+          <a:ext cx="2904005" cy="998446"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -15729"/>
-            <a:gd name="adj2" fmla="val -99596"/>
+            <a:gd name="adj1" fmla="val -47757"/>
+            <a:gd name="adj2" fmla="val -125410"/>
             <a:gd name="adj3" fmla="val 16667"/>
           </a:avLst>
         </a:prstGeom>
@@ -5298,16 +5331,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>116542</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>122703</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1248335</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>100291</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>555253</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>179854</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>638735</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5322,13 +5355,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15210866" y="11194115"/>
-          <a:ext cx="2904005" cy="998445"/>
+          <a:off x="19928541" y="12348320"/>
+          <a:ext cx="3648635" cy="1154768"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -15343"/>
-            <a:gd name="adj2" fmla="val 88956"/>
+            <a:gd name="adj1" fmla="val -48821"/>
+            <a:gd name="adj2" fmla="val 105452"/>
             <a:gd name="adj3" fmla="val 16667"/>
           </a:avLst>
         </a:prstGeom>
@@ -5358,6 +5391,51 @@
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
             <a:t>共通構造</a:t>
           </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>割り当て要望サイズ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>+</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>アライメント要求値 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>&lt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>「割り当てるメモリ」＋</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>sizeof(uintptr_t)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> (tail_padding</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t>分</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t>であれば、割り当て可能</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5365,114 +5443,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3092824</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>224118</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1782296</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>102538</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="42" name="吹き出し: 角を丸めた四角形 41">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8D43D6B-B709-4EF9-A5FB-392A888B4C09}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5143500" y="8001000"/>
-          <a:ext cx="2533090" cy="2702303"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRoundRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 161772"/>
-            <a:gd name="adj2" fmla="val -44139"/>
-            <a:gd name="adj3" fmla="val 16667"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>1</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>の場合、スロットの確保が個別に</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>allocator</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>で確保されたことを示す。</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>ゼロは、未初期化状態を意味するものとする。よって、不正値とする。</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>解放処理等では、何もしないで、放置する。</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>44823</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>95259</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>2442882</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>138122</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5525,15 +5504,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>44827</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>189385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>2454089</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>232247</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5578,6 +5557,314 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1860177</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1557618</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="フリーフォーム: 図形 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A527C70-BE35-27C1-4C79-64857BA083FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7754471" y="5087471"/>
+          <a:ext cx="8852647" cy="3989294"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 8852647"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 3989294"/>
+            <a:gd name="connsiteX1" fmla="*/ 2588558 w 8852647"/>
+            <a:gd name="connsiteY1" fmla="*/ 3989294 h 3989294"/>
+            <a:gd name="connsiteX2" fmla="*/ 8852647 w 8852647"/>
+            <a:gd name="connsiteY2" fmla="*/ 3989294 h 3989294"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="8852647" h="3989294">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2588558" y="3989294"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="8852647" y="3989294"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>531160</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>358589</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>638736</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>233646</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="吹き出し: 角を丸めた四角形 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{251AEE55-0A8A-42EF-A333-CD51B41B7E66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5820336" y="1299883"/>
+          <a:ext cx="2796988" cy="1298204"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -29667"/>
+            <a:gd name="adj2" fmla="val 84535"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>スロット毎に管理情報を配置するよりも、</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>管理情報を集める方が、ページキャッシュにやさしくなると思われる。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>298076</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>146236</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1065679</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>203387</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="吹き出し: 角を丸めた四角形 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B1429E2-282F-46E3-8A10-503917B3D5FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16961223" y="12394265"/>
+          <a:ext cx="2784662" cy="998446"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 13700"/>
+            <a:gd name="adj2" fmla="val -142753"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>呼び出し側が指定したアライメント値か、デフォルトのアライメント値の最小公倍数でアライメントされる。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>331693</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>96368</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>959222</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>61068</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="吹き出し: 角を丸めた四角形 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92A9CDAF-FDEF-44F1-98A2-4742A8AA7AB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14529546" y="12579721"/>
+          <a:ext cx="1479176" cy="670671"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 128974"/>
+            <a:gd name="adj2" fmla="val 135419"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>slot_container</a:t>
+          </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -6122,10 +6409,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FCA077-D2DC-4602-9CF2-A8F5DAEA3F68}">
-  <dimension ref="C4:R87"/>
+  <dimension ref="C4:S87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="E32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -6138,9 +6425,9 @@
     <col min="10" max="10" width="15" customWidth="1"/>
     <col min="11" max="14" width="11.125" customWidth="1"/>
     <col min="15" max="15" width="21.125" customWidth="1"/>
-    <col min="16" max="16" width="13.25" customWidth="1"/>
-    <col min="17" max="17" width="32.375" customWidth="1"/>
-    <col min="18" max="18" width="14.5" customWidth="1"/>
+    <col min="16" max="17" width="13.25" customWidth="1"/>
+    <col min="18" max="18" width="32.375" customWidth="1"/>
+    <col min="19" max="19" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:10">
@@ -6199,12 +6486,12 @@
     </row>
     <row r="14" spans="3:10">
       <c r="F14" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="3:10">
       <c r="F15" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="3:10">
@@ -6212,407 +6499,373 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="6:18">
+    <row r="17" spans="6:15">
       <c r="F17" t="s">
+        <v>72</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="6:15">
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" t="s">
+        <v>33</v>
+      </c>
+      <c r="N18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="6:15">
+      <c r="F19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19" t="s">
+        <v>34</v>
+      </c>
+      <c r="N19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="6:15">
+      <c r="F20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" t="s">
+        <v>34</v>
+      </c>
+      <c r="L20" t="s">
+        <v>34</v>
+      </c>
+      <c r="M20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="6:15">
+      <c r="F21" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="6:18">
-      <c r="J24" s="5" t="s">
+      <c r="J21" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" t="s">
+        <v>34</v>
+      </c>
+      <c r="L21" t="s">
+        <v>34</v>
+      </c>
+      <c r="M21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="6:15">
+      <c r="J22" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" t="s">
+        <v>34</v>
+      </c>
+      <c r="L22" t="s">
+        <v>34</v>
+      </c>
+      <c r="M22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="6:15">
+      <c r="J23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23" t="s">
+        <v>34</v>
+      </c>
+      <c r="L23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="6:15">
+      <c r="J24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K24" t="s">
+        <v>34</v>
+      </c>
+      <c r="L24" t="s">
+        <v>63</v>
+      </c>
+      <c r="O24" s="8"/>
+    </row>
+    <row r="25" spans="6:15">
+      <c r="J25" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="6:15">
+      <c r="J26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="6:15">
+      <c r="J27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="6:15">
+      <c r="J28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="16:19">
+      <c r="P38" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q38" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R38" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S38" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="16:19">
+      <c r="P39" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>33</v>
+      </c>
+      <c r="S39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="16:19">
+      <c r="P40" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>34</v>
+      </c>
+      <c r="S40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="16:19">
+      <c r="P41" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="16:19">
+      <c r="P42" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="16:19">
+      <c r="P43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="16:19">
+      <c r="P44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="16:19">
+      <c r="P45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67" spans="10:19">
+      <c r="J67" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="K67" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="L67" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="M24" s="5" t="s">
+      <c r="M67" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="N24" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="O24" s="5" t="s">
+      <c r="N67" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="O67" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="P24" s="5" t="s">
+      <c r="P67" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Q24" s="5" t="s">
+      <c r="Q67" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R67" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="R24" s="5" t="s">
+      <c r="S67" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="6:18">
-      <c r="J25" t="s">
+    <row r="68" spans="10:19">
+      <c r="J68" t="s">
         <v>33</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K68" t="s">
         <v>33</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L68" t="s">
         <v>33</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M68" t="s">
         <v>33</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N68" t="s">
         <v>33</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O68" t="s">
         <v>33</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P68" t="s">
         <v>33</v>
       </c>
-      <c r="R25" t="s">
+      <c r="Q68" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="6:18">
-      <c r="J26" t="s">
-        <v>34</v>
-      </c>
-      <c r="K26" t="s">
-        <v>34</v>
-      </c>
-      <c r="L26" t="s">
-        <v>34</v>
-      </c>
-      <c r="M26" t="s">
-        <v>34</v>
-      </c>
-      <c r="N26" t="s">
-        <v>34</v>
-      </c>
-      <c r="O26" t="s">
-        <v>34</v>
-      </c>
-      <c r="P26" t="s">
-        <v>34</v>
-      </c>
-      <c r="R26" t="s">
+      <c r="S68" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="10:19">
+      <c r="J69" t="s">
+        <v>34</v>
+      </c>
+      <c r="K69" t="s">
+        <v>34</v>
+      </c>
+      <c r="L69" t="s">
+        <v>34</v>
+      </c>
+      <c r="M69" t="s">
+        <v>34</v>
+      </c>
+      <c r="N69" t="s">
+        <v>34</v>
+      </c>
+      <c r="O69" t="s">
+        <v>34</v>
+      </c>
+      <c r="P69" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>34</v>
+      </c>
+      <c r="S69" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="6:18">
-      <c r="J27" t="s">
-        <v>34</v>
-      </c>
-      <c r="K27" t="s">
-        <v>34</v>
-      </c>
-      <c r="L27" t="s">
-        <v>34</v>
-      </c>
-      <c r="M27" t="s">
-        <v>34</v>
-      </c>
-      <c r="N27" t="s">
-        <v>34</v>
-      </c>
-      <c r="O27" t="s">
-        <v>34</v>
-      </c>
-      <c r="P27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="6:18">
-      <c r="J28" t="s">
-        <v>34</v>
-      </c>
-      <c r="K28" t="s">
-        <v>34</v>
-      </c>
-      <c r="L28" t="s">
-        <v>34</v>
-      </c>
-      <c r="M28" t="s">
-        <v>34</v>
-      </c>
-      <c r="N28" t="s">
-        <v>34</v>
-      </c>
-      <c r="O28" t="s">
-        <v>34</v>
-      </c>
-      <c r="P28" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="6:18">
-      <c r="J29" t="s">
-        <v>34</v>
-      </c>
-      <c r="K29" t="s">
-        <v>34</v>
-      </c>
-      <c r="L29" t="s">
-        <v>34</v>
-      </c>
-      <c r="M29" t="s">
-        <v>34</v>
-      </c>
-      <c r="N29" t="s">
-        <v>34</v>
-      </c>
-      <c r="O29" t="s">
-        <v>34</v>
-      </c>
-      <c r="P29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="6:18">
-      <c r="J30" t="s">
-        <v>34</v>
-      </c>
-      <c r="K30" t="s">
-        <v>34</v>
-      </c>
-      <c r="L30" t="s">
-        <v>34</v>
-      </c>
-      <c r="M30" t="s">
-        <v>34</v>
-      </c>
-      <c r="N30" t="s">
-        <v>34</v>
-      </c>
-      <c r="O30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="6:18">
-      <c r="J31" t="s">
-        <v>34</v>
-      </c>
-      <c r="K31" t="s">
-        <v>34</v>
-      </c>
-      <c r="L31" t="s">
-        <v>34</v>
-      </c>
-      <c r="M31" t="s">
-        <v>34</v>
-      </c>
-      <c r="N31" t="s">
-        <v>34</v>
-      </c>
-      <c r="O31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="6:18">
-      <c r="J32" t="s">
-        <v>34</v>
-      </c>
-      <c r="K32" t="s">
-        <v>34</v>
-      </c>
-      <c r="L32" t="s">
-        <v>34</v>
-      </c>
-      <c r="M32" t="s">
-        <v>34</v>
-      </c>
-      <c r="N32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="10:14">
-      <c r="J33" t="s">
-        <v>34</v>
-      </c>
-      <c r="K33" t="s">
-        <v>34</v>
-      </c>
-      <c r="L33" t="s">
-        <v>34</v>
-      </c>
-      <c r="M33" t="s">
-        <v>34</v>
-      </c>
-      <c r="N33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="10:14">
-      <c r="J34" t="s">
-        <v>34</v>
-      </c>
-      <c r="K34" t="s">
-        <v>34</v>
-      </c>
-      <c r="L34" t="s">
-        <v>34</v>
-      </c>
-      <c r="M34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="10:14">
-      <c r="J35" t="s">
-        <v>34</v>
-      </c>
-      <c r="K35" t="s">
-        <v>34</v>
-      </c>
-      <c r="L35" t="s">
-        <v>34</v>
-      </c>
-      <c r="M35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="10:14">
-      <c r="J36" t="s">
-        <v>34</v>
-      </c>
-      <c r="K36" t="s">
-        <v>34</v>
-      </c>
-      <c r="L36" t="s">
-        <v>34</v>
-      </c>
-      <c r="M36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="10:14">
-      <c r="J37" t="s">
-        <v>34</v>
-      </c>
-      <c r="K37" t="s">
-        <v>34</v>
-      </c>
-      <c r="L37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="10:14">
-      <c r="J38" t="s">
-        <v>34</v>
-      </c>
-      <c r="K38" t="s">
-        <v>34</v>
-      </c>
-      <c r="L38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="10:14">
-      <c r="J39" t="s">
-        <v>34</v>
-      </c>
-      <c r="K39" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="10:14">
-      <c r="J40" t="s">
-        <v>34</v>
-      </c>
-      <c r="K40" t="s">
+    <row r="70" spans="10:19">
+      <c r="J70" t="s">
+        <v>34</v>
+      </c>
+      <c r="K70" t="s">
+        <v>34</v>
+      </c>
+      <c r="L70" t="s">
+        <v>34</v>
+      </c>
+      <c r="M70" t="s">
+        <v>34</v>
+      </c>
+      <c r="N70" t="s">
+        <v>34</v>
+      </c>
+      <c r="O70" t="s">
+        <v>34</v>
+      </c>
+      <c r="P70" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="10:19">
+      <c r="J71" t="s">
+        <v>34</v>
+      </c>
+      <c r="K71" t="s">
+        <v>34</v>
+      </c>
+      <c r="L71" t="s">
+        <v>34</v>
+      </c>
+      <c r="M71" t="s">
+        <v>34</v>
+      </c>
+      <c r="N71" t="s">
+        <v>34</v>
+      </c>
+      <c r="O71" t="s">
+        <v>34</v>
+      </c>
+      <c r="P71" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q71" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="10:14">
-      <c r="J41" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="42" spans="10:14">
-      <c r="J42" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="69" spans="10:18">
-      <c r="J69" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K69" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L69" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="M69" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="N69" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="O69" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="P69" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q69" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R69" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="70" spans="10:18">
-      <c r="J70" t="s">
-        <v>33</v>
-      </c>
-      <c r="K70" t="s">
-        <v>33</v>
-      </c>
-      <c r="L70" t="s">
-        <v>33</v>
-      </c>
-      <c r="M70" t="s">
-        <v>33</v>
-      </c>
-      <c r="N70" t="s">
-        <v>33</v>
-      </c>
-      <c r="O70" t="s">
-        <v>33</v>
-      </c>
-      <c r="P70" t="s">
-        <v>33</v>
-      </c>
-      <c r="R70" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="71" spans="10:18">
-      <c r="J71" t="s">
-        <v>34</v>
-      </c>
-      <c r="K71" t="s">
-        <v>34</v>
-      </c>
-      <c r="L71" t="s">
-        <v>34</v>
-      </c>
-      <c r="M71" t="s">
-        <v>34</v>
-      </c>
-      <c r="N71" t="s">
-        <v>34</v>
-      </c>
-      <c r="O71" t="s">
-        <v>34</v>
-      </c>
-      <c r="P71" t="s">
-        <v>34</v>
-      </c>
-      <c r="R71" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="72" spans="10:18">
+    <row r="72" spans="10:19">
       <c r="J72" t="s">
         <v>34</v>
       </c>
@@ -6635,7 +6888,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="10:18">
+    <row r="73" spans="10:19">
       <c r="J73" t="s">
         <v>34</v>
       </c>
@@ -6658,7 +6911,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="10:18">
+    <row r="74" spans="10:19">
       <c r="J74" t="s">
         <v>34</v>
       </c>
@@ -6681,7 +6934,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="75" spans="10:18">
+    <row r="75" spans="10:19">
       <c r="J75" t="s">
         <v>34</v>
       </c>
@@ -6701,7 +6954,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="10:18">
+    <row r="76" spans="10:19">
       <c r="J76" t="s">
         <v>34</v>
       </c>
@@ -6721,7 +6974,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="77" spans="10:18">
+    <row r="77" spans="10:19">
       <c r="J77" t="s">
         <v>34</v>
       </c>
@@ -6738,7 +6991,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="10:18">
+    <row r="78" spans="10:19">
       <c r="J78" t="s">
         <v>34</v>
       </c>
@@ -6755,7 +7008,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="10:18">
+    <row r="79" spans="10:19">
       <c r="J79" t="s">
         <v>34</v>
       </c>
@@ -6769,7 +7022,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="10:18">
+    <row r="80" spans="10:19">
       <c r="J80" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
refactor: support outer alloc_only_chamber for hazard_ptr
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/Design_general_mem_alloc.xlsx
+++ b/libalconcurrent/doc/Design_general_mem_alloc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388B858B-DB22-4AB3-9DCF-DAD88E50D0FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CCE3BA-7910-471E-ADC0-75A0015859D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="75">
   <si>
     <t>param_chunk_allocation</t>
   </si>
@@ -548,6 +548,14 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>slot_array_mgr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -577,7 +585,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -600,11 +608,194 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top style="mediumDashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="mediumDashed">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top style="mediumDashed">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -622,10 +813,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -3562,13 +3782,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>493059</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>4482</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>224116</xdr:rowOff>
@@ -3623,13 +3843,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>1695450</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>131108</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>493059</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -3678,13 +3898,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>1914525</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -3731,13 +3951,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>425823</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -3877,13 +4097,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>14288</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>58277</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>829235</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>101139</xdr:rowOff>
@@ -3938,13 +4158,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>22408</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>171454</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>829234</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>214315</xdr:rowOff>
@@ -3999,13 +4219,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>737347</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>207869</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1484779</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>36421</xdr:rowOff>
@@ -4078,13 +4298,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>22414</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>32504</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>1086971</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>75366</xdr:rowOff>
@@ -4139,13 +4359,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>324970</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>100851</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>952499</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>65551</xdr:rowOff>
@@ -4207,13 +4427,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>350185</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>102533</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>186019</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4326,13 +4546,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>1580030</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>112059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>325813</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>58278</xdr:rowOff>
@@ -4381,13 +4601,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>44823</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>5612</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>1053354</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>48474</xdr:rowOff>
@@ -4442,13 +4662,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>291353</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>150719</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>1058956</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>207870</xdr:rowOff>
@@ -4509,13 +4729,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>44822</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>76203</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1590673</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>119065</xdr:rowOff>
@@ -4570,13 +4790,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>291352</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>104765</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>209549</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>171441</xdr:rowOff>
@@ -4649,13 +4869,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>55746</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>171454</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>818029</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>214315</xdr:rowOff>
@@ -4710,13 +4930,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>643218</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>67794</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>139514</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>134471</xdr:rowOff>
@@ -4789,13 +5009,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>33617</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>85734</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>795617</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>128596</xdr:rowOff>
@@ -4850,13 +5070,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>926167</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>86844</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>781051</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>153520</xdr:rowOff>
@@ -4929,13 +5149,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>1183901</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>65550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>949138</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>145676</xdr:rowOff>
@@ -5009,13 +5229,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>2476500</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>179294</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>90</xdr:row>
       <xdr:rowOff>204107</xdr:rowOff>
@@ -5073,13 +5293,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>2209160</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>149679</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>1255060</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>78441</xdr:rowOff>
@@ -5136,13 +5356,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>261257</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>123264</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>397329</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>40821</xdr:rowOff>
@@ -5200,13 +5420,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>489127</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>67236</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>523107</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5267,13 +5487,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>1264024</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>115979</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>593353</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>173130</xdr:rowOff>
@@ -5331,13 +5551,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>1248335</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>100291</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>638735</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>78441</xdr:rowOff>
@@ -5443,13 +5663,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>44823</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>95259</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>2442882</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>138122</xdr:rowOff>
@@ -5504,13 +5724,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>44827</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>189385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>2454089</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>232247</xdr:rowOff>
@@ -5565,13 +5785,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>1860177</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>134471</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1557618</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>123265</xdr:rowOff>
@@ -5663,16 +5883,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>531160</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>358589</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>367874</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>81642</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>638736</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>233646</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>136070</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>70360</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5687,13 +5907,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5820336" y="1299883"/>
-          <a:ext cx="2796988" cy="1298204"/>
+          <a:off x="12301338" y="1782535"/>
+          <a:ext cx="3129161" cy="968432"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -29667"/>
-            <a:gd name="adj2" fmla="val 84535"/>
+            <a:gd name="adj1" fmla="val -26623"/>
+            <a:gd name="adj2" fmla="val 78915"/>
             <a:gd name="adj3" fmla="val 16667"/>
           </a:avLst>
         </a:prstGeom>
@@ -5738,13 +5958,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>298076</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>146236</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>1065679</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>203387</xdr:rowOff>
@@ -5805,13 +6025,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>331693</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>96368</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>959222</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>61068</xdr:rowOff>
@@ -5869,6 +6089,543 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>560295</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="フリーフォーム: 図形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95F7B7CA-9C3E-4496-8BED-17E75921E668}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1514475" y="981075"/>
+          <a:ext cx="1103220" cy="1296521"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 523875"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 819150"/>
+            <a:gd name="connsiteX1" fmla="*/ 95250 w 523875"/>
+            <a:gd name="connsiteY1" fmla="*/ 619125 h 819150"/>
+            <a:gd name="connsiteX2" fmla="*/ 523875 w 523875"/>
+            <a:gd name="connsiteY2" fmla="*/ 819150 h 819150"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="523875" h="819150">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="95250" y="619125"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="523875" y="819150"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>573182</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>231963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>661146</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>134472</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="吹き出し: 角を丸めた四角形 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83EC6408-2711-43E4-BE8B-B2FA5E2BCE07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1258982" y="2375088"/>
+          <a:ext cx="773764" cy="378759"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 60445"/>
+            <a:gd name="adj2" fmla="val -107646"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>copy</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2801471</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>22411</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>257735</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="フリーフォーム: 図形 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D82F00F-75EA-C92D-3ABF-6B3333788D0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6219265" y="963706"/>
+          <a:ext cx="1848970" cy="2364441"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 1848970"/>
+            <a:gd name="connsiteY0" fmla="*/ 2364441 h 2364441"/>
+            <a:gd name="connsiteX1" fmla="*/ 649941 w 1848970"/>
+            <a:gd name="connsiteY1" fmla="*/ 2364441 h 2364441"/>
+            <a:gd name="connsiteX2" fmla="*/ 1848970 w 1848970"/>
+            <a:gd name="connsiteY2" fmla="*/ 0 h 2364441"/>
+            <a:gd name="connsiteX3" fmla="*/ 1848970 w 1848970"/>
+            <a:gd name="connsiteY3" fmla="*/ 0 h 2364441"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="1848970" h="2364441">
+              <a:moveTo>
+                <a:pt x="0" y="2364441"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="649941" y="2364441"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1848970" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1848970" y="0"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3007179</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>122464</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>40821</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="フリーフォーム: 図形 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{876AD3F2-256C-B3DC-5A53-4DF357F1B56E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11702143" y="857250"/>
+          <a:ext cx="12600214" cy="734786"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 12600214"/>
+            <a:gd name="connsiteY0" fmla="*/ 734786 h 734786"/>
+            <a:gd name="connsiteX1" fmla="*/ 476250 w 12600214"/>
+            <a:gd name="connsiteY1" fmla="*/ 734786 h 734786"/>
+            <a:gd name="connsiteX2" fmla="*/ 12096750 w 12600214"/>
+            <a:gd name="connsiteY2" fmla="*/ 0 h 734786"/>
+            <a:gd name="connsiteX3" fmla="*/ 12600214 w 12600214"/>
+            <a:gd name="connsiteY3" fmla="*/ 0 h 734786"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="12600214" h="734786">
+              <a:moveTo>
+                <a:pt x="0" y="734786"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="476250" y="734786"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="12096750" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="12600214" y="0"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>299357</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>231321</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>449036</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="直線矢印コネクタ 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{570F4AFF-7552-45D4-BC91-A98FBC99472F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25567821" y="966107"/>
+          <a:ext cx="149679" cy="802822"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>2354036</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>122464</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>54428</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>122464</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="直線矢印コネクタ 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A47C184-1F71-A107-AC5B-770BDED04D86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27622500" y="857250"/>
+          <a:ext cx="1265464" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>408214</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>217714</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>544286</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="直線矢印コネクタ 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45C55EA5-318D-4D46-3B37-837045BC8EE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="29922107" y="952500"/>
+          <a:ext cx="136072" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6139,8 +6896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:Y40"/>
   <sheetViews>
-    <sheetView topLeftCell="K28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P59" sqref="P32:Y59"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G1" sqref="B1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -6409,692 +7166,818 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FCA077-D2DC-4602-9CF2-A8F5DAEA3F68}">
-  <dimension ref="C4:S87"/>
+  <dimension ref="A3:AA87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col min="4" max="4" width="42.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.875" customWidth="1"/>
-    <col min="6" max="6" width="27.375" customWidth="1"/>
-    <col min="8" max="8" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" customWidth="1"/>
-    <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="14" width="11.125" customWidth="1"/>
-    <col min="15" max="15" width="21.125" customWidth="1"/>
-    <col min="16" max="17" width="13.25" customWidth="1"/>
-    <col min="18" max="18" width="32.375" customWidth="1"/>
-    <col min="19" max="19" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="42.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.875" customWidth="1"/>
+    <col min="12" max="12" width="27.375" customWidth="1"/>
+    <col min="14" max="14" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="17" max="20" width="11.125" customWidth="1"/>
+    <col min="21" max="21" width="21.125" customWidth="1"/>
+    <col min="22" max="23" width="13.25" customWidth="1"/>
+    <col min="24" max="24" width="32.375" customWidth="1"/>
+    <col min="25" max="25" width="14.5" customWidth="1"/>
+    <col min="27" max="27" width="15.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10">
-      <c r="C4" t="s">
+    <row r="3" spans="1:27" ht="19.5" thickBot="1">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="20.25" thickTop="1" thickBot="1">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="3:10" ht="37.5">
-      <c r="D5" s="6" t="s">
+      <c r="J4" s="17"/>
+      <c r="W4" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="X4" s="28"/>
+      <c r="Z4" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA4" s="28"/>
+    </row>
+    <row r="5" spans="1:27" ht="38.25" thickTop="1">
+      <c r="I5" s="18"/>
+      <c r="J5" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="3:10">
-      <c r="D6" t="s">
+    <row r="6" spans="1:27" ht="19.5" thickBot="1">
+      <c r="I6" s="18"/>
+      <c r="J6" s="20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="3:10">
-      <c r="D7" t="s">
+    <row r="7" spans="1:27" ht="19.5" thickBot="1">
+      <c r="I7" s="18"/>
+      <c r="J7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J7" t="s">
+      <c r="P7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="3:10">
-      <c r="D8" t="s">
+      <c r="X7" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA7" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="19.5" thickTop="1">
+      <c r="C8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="17"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J8" t="s">
+      <c r="P8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="3:10">
-      <c r="D9" t="s">
+    <row r="9" spans="1:27" ht="19.5" thickBot="1">
+      <c r="C9" s="18"/>
+      <c r="D9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="21"/>
+      <c r="J9" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="J9" t="s">
+      <c r="P9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="3:10">
-      <c r="J10" t="s">
+    <row r="10" spans="1:27" ht="19.5" thickTop="1">
+      <c r="C10" s="18"/>
+      <c r="D10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="20"/>
+      <c r="P10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="3:10">
-      <c r="J11" t="s">
+    <row r="11" spans="1:27" ht="19.5" thickBot="1">
+      <c r="C11" s="18"/>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="P11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="3:10">
-      <c r="F13" t="s">
+    <row r="12" spans="1:27">
+      <c r="C12" s="18"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:27" ht="37.5">
+      <c r="C13" s="18"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="11"/>
+      <c r="L13" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="3:10">
-      <c r="F14" t="s">
+    <row r="14" spans="1:27" ht="37.5">
+      <c r="C14" s="18"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="11"/>
+      <c r="L14" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="3:10">
-      <c r="F15" t="s">
+    <row r="15" spans="1:27">
+      <c r="C15" s="18"/>
+      <c r="D15" s="7">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="20"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="3:10">
-      <c r="F16" s="7" t="s">
+    <row r="16" spans="1:27">
+      <c r="C16" s="18"/>
+      <c r="D16" s="7">
+        <v>2</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="6:15">
-      <c r="F17" t="s">
+    <row r="17" spans="3:20">
+      <c r="C17" s="18"/>
+      <c r="D17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="20"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="P17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="Q17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="R17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="S17" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="N17" s="5" t="s">
+      <c r="T17" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="6:15">
-      <c r="F18" t="s">
+    <row r="18" spans="3:20">
+      <c r="C18" s="18"/>
+      <c r="D18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="20"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="J18" t="s">
+      <c r="P18" t="s">
         <v>33</v>
       </c>
-      <c r="K18" t="s">
+      <c r="Q18" t="s">
         <v>33</v>
       </c>
-      <c r="L18" t="s">
+      <c r="R18" t="s">
         <v>33</v>
       </c>
-      <c r="M18" t="s">
+      <c r="S18" t="s">
         <v>33</v>
       </c>
-      <c r="N18" t="s">
+      <c r="T18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="6:15">
-      <c r="F19" t="s">
+    <row r="19" spans="3:20" ht="19.5" thickBot="1">
+      <c r="C19" s="21"/>
+      <c r="D19" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="J19" t="s">
-        <v>34</v>
-      </c>
-      <c r="K19" t="s">
-        <v>34</v>
-      </c>
-      <c r="L19" t="s">
-        <v>34</v>
-      </c>
-      <c r="M19" t="s">
-        <v>34</v>
-      </c>
-      <c r="N19" t="s">
+      <c r="P19" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>34</v>
+      </c>
+      <c r="R19" t="s">
+        <v>34</v>
+      </c>
+      <c r="S19" t="s">
+        <v>34</v>
+      </c>
+      <c r="T19" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="6:15">
-      <c r="F20" s="7" t="s">
+    <row r="20" spans="3:20" ht="19.5" thickTop="1">
+      <c r="K20" s="11"/>
+      <c r="L20" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="J20" t="s">
-        <v>34</v>
-      </c>
-      <c r="K20" t="s">
-        <v>34</v>
-      </c>
-      <c r="L20" t="s">
-        <v>34</v>
-      </c>
-      <c r="M20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="6:15">
-      <c r="F21" t="s">
+      <c r="P20" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>34</v>
+      </c>
+      <c r="R20" t="s">
+        <v>34</v>
+      </c>
+      <c r="S20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="3:20" ht="19.5" thickBot="1">
+      <c r="K21" s="14"/>
+      <c r="L21" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="J21" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21" t="s">
-        <v>34</v>
-      </c>
-      <c r="L21" t="s">
-        <v>34</v>
-      </c>
-      <c r="M21" t="s">
+      <c r="P21" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>34</v>
+      </c>
+      <c r="R21" t="s">
+        <v>34</v>
+      </c>
+      <c r="S21" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="6:15">
-      <c r="J22" t="s">
-        <v>34</v>
-      </c>
-      <c r="K22" t="s">
-        <v>34</v>
-      </c>
-      <c r="L22" t="s">
-        <v>34</v>
-      </c>
-      <c r="M22" t="s">
+    <row r="22" spans="3:20">
+      <c r="P22" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>34</v>
+      </c>
+      <c r="R22" t="s">
+        <v>34</v>
+      </c>
+      <c r="S22" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="6:15">
-      <c r="J23" t="s">
-        <v>34</v>
-      </c>
-      <c r="K23" t="s">
-        <v>34</v>
-      </c>
-      <c r="L23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="6:15">
-      <c r="J24" t="s">
-        <v>34</v>
-      </c>
-      <c r="K24" t="s">
-        <v>34</v>
-      </c>
-      <c r="L24" t="s">
+    <row r="23" spans="3:20">
+      <c r="P23" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>34</v>
+      </c>
+      <c r="R23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="3:20">
+      <c r="P24" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>34</v>
+      </c>
+      <c r="R24" t="s">
         <v>63</v>
       </c>
-      <c r="O24" s="8"/>
-    </row>
-    <row r="25" spans="6:15">
-      <c r="J25" t="s">
-        <v>34</v>
-      </c>
-      <c r="K25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="6:15">
-      <c r="J26" t="s">
-        <v>34</v>
-      </c>
-      <c r="K26" t="s">
+    </row>
+    <row r="25" spans="3:20">
+      <c r="P25" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="3:20">
+      <c r="P26" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="6:15">
-      <c r="J27" t="s">
+    <row r="27" spans="3:20">
+      <c r="P27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="6:15">
-      <c r="J28" t="s">
+    <row r="28" spans="3:20">
+      <c r="P28" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="16:19">
-      <c r="P38" s="5" t="s">
+    <row r="38" spans="22:25">
+      <c r="V38" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Q38" s="5" t="s">
+      <c r="W38" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="R38" s="5" t="s">
+      <c r="X38" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="S38" s="5" t="s">
+      <c r="Y38" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="16:19">
-      <c r="P39" t="s">
+    <row r="39" spans="22:25">
+      <c r="V39" t="s">
         <v>33</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="W39" t="s">
         <v>33</v>
       </c>
-      <c r="S39" t="s">
+      <c r="Y39" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="16:19">
-      <c r="P40" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>34</v>
-      </c>
-      <c r="S40" t="s">
+    <row r="40" spans="22:25">
+      <c r="V40" t="s">
+        <v>34</v>
+      </c>
+      <c r="W40" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y40" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="16:19">
-      <c r="P41" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="42" spans="16:19">
-      <c r="P42" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q42" t="s">
+    <row r="41" spans="22:25">
+      <c r="V41" t="s">
+        <v>34</v>
+      </c>
+      <c r="W41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="22:25">
+      <c r="V42" t="s">
+        <v>34</v>
+      </c>
+      <c r="W42" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="16:19">
-      <c r="P43" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="16:19">
-      <c r="P44" t="s">
+    <row r="43" spans="22:25">
+      <c r="V43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="22:25">
+      <c r="V44" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="16:19">
-      <c r="P45" t="s">
+    <row r="45" spans="22:25">
+      <c r="V45" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="10:19">
-      <c r="J67" s="5" t="s">
+    <row r="67" spans="16:25">
+      <c r="P67" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="K67" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L67" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="M67" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="N67" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="O67" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="P67" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="Q67" s="5" t="s">
         <v>29</v>
       </c>
       <c r="R67" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="S67" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="T67" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="U67" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="V67" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="W67" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="X67" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="S67" s="5" t="s">
+      <c r="Y67" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="68" spans="10:19">
-      <c r="J68" t="s">
-        <v>33</v>
-      </c>
-      <c r="K68" t="s">
-        <v>33</v>
-      </c>
-      <c r="L68" t="s">
-        <v>33</v>
-      </c>
-      <c r="M68" t="s">
-        <v>33</v>
-      </c>
-      <c r="N68" t="s">
-        <v>33</v>
-      </c>
-      <c r="O68" t="s">
-        <v>33</v>
-      </c>
+    <row r="68" spans="16:25">
       <c r="P68" t="s">
         <v>33</v>
       </c>
       <c r="Q68" t="s">
         <v>33</v>
       </c>
+      <c r="R68" t="s">
+        <v>33</v>
+      </c>
       <c r="S68" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="69" spans="10:19">
-      <c r="J69" t="s">
-        <v>34</v>
-      </c>
-      <c r="K69" t="s">
-        <v>34</v>
-      </c>
-      <c r="L69" t="s">
-        <v>34</v>
-      </c>
-      <c r="M69" t="s">
-        <v>34</v>
-      </c>
-      <c r="N69" t="s">
-        <v>34</v>
-      </c>
-      <c r="O69" t="s">
-        <v>34</v>
-      </c>
+      <c r="T68" t="s">
+        <v>33</v>
+      </c>
+      <c r="U68" t="s">
+        <v>33</v>
+      </c>
+      <c r="V68" t="s">
+        <v>33</v>
+      </c>
+      <c r="W68" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y68" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="16:25">
       <c r="P69" t="s">
         <v>34</v>
       </c>
       <c r="Q69" t="s">
         <v>34</v>
       </c>
+      <c r="R69" t="s">
+        <v>34</v>
+      </c>
       <c r="S69" t="s">
+        <v>34</v>
+      </c>
+      <c r="T69" t="s">
+        <v>34</v>
+      </c>
+      <c r="U69" t="s">
+        <v>34</v>
+      </c>
+      <c r="V69" t="s">
+        <v>34</v>
+      </c>
+      <c r="W69" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y69" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="70" spans="10:19">
-      <c r="J70" t="s">
-        <v>34</v>
-      </c>
-      <c r="K70" t="s">
-        <v>34</v>
-      </c>
-      <c r="L70" t="s">
-        <v>34</v>
-      </c>
-      <c r="M70" t="s">
-        <v>34</v>
-      </c>
-      <c r="N70" t="s">
-        <v>34</v>
-      </c>
-      <c r="O70" t="s">
-        <v>34</v>
-      </c>
+    <row r="70" spans="16:25">
       <c r="P70" t="s">
         <v>34</v>
       </c>
       <c r="Q70" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="71" spans="10:19">
-      <c r="J71" t="s">
-        <v>34</v>
-      </c>
-      <c r="K71" t="s">
-        <v>34</v>
-      </c>
-      <c r="L71" t="s">
-        <v>34</v>
-      </c>
-      <c r="M71" t="s">
-        <v>34</v>
-      </c>
-      <c r="N71" t="s">
-        <v>34</v>
-      </c>
-      <c r="O71" t="s">
-        <v>34</v>
-      </c>
+      <c r="R70" t="s">
+        <v>34</v>
+      </c>
+      <c r="S70" t="s">
+        <v>34</v>
+      </c>
+      <c r="T70" t="s">
+        <v>34</v>
+      </c>
+      <c r="U70" t="s">
+        <v>34</v>
+      </c>
+      <c r="V70" t="s">
+        <v>34</v>
+      </c>
+      <c r="W70" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="16:25">
       <c r="P71" t="s">
         <v>34</v>
       </c>
       <c r="Q71" t="s">
+        <v>34</v>
+      </c>
+      <c r="R71" t="s">
+        <v>34</v>
+      </c>
+      <c r="S71" t="s">
+        <v>34</v>
+      </c>
+      <c r="T71" t="s">
+        <v>34</v>
+      </c>
+      <c r="U71" t="s">
+        <v>34</v>
+      </c>
+      <c r="V71" t="s">
+        <v>34</v>
+      </c>
+      <c r="W71" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="72" spans="10:19">
-      <c r="J72" t="s">
-        <v>34</v>
-      </c>
-      <c r="K72" t="s">
-        <v>34</v>
-      </c>
-      <c r="L72" t="s">
-        <v>34</v>
-      </c>
-      <c r="M72" t="s">
-        <v>34</v>
-      </c>
-      <c r="N72" t="s">
-        <v>34</v>
-      </c>
-      <c r="O72" t="s">
-        <v>34</v>
-      </c>
+    <row r="72" spans="16:25">
       <c r="P72" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="73" spans="10:19">
-      <c r="J73" t="s">
-        <v>34</v>
-      </c>
-      <c r="K73" t="s">
-        <v>34</v>
-      </c>
-      <c r="L73" t="s">
-        <v>34</v>
-      </c>
-      <c r="M73" t="s">
-        <v>34</v>
-      </c>
-      <c r="N73" t="s">
-        <v>34</v>
-      </c>
-      <c r="O73" t="s">
-        <v>34</v>
-      </c>
+      <c r="Q72" t="s">
+        <v>34</v>
+      </c>
+      <c r="R72" t="s">
+        <v>34</v>
+      </c>
+      <c r="S72" t="s">
+        <v>34</v>
+      </c>
+      <c r="T72" t="s">
+        <v>34</v>
+      </c>
+      <c r="U72" t="s">
+        <v>34</v>
+      </c>
+      <c r="V72" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="16:25">
       <c r="P73" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>34</v>
+      </c>
+      <c r="R73" t="s">
+        <v>34</v>
+      </c>
+      <c r="S73" t="s">
+        <v>34</v>
+      </c>
+      <c r="T73" t="s">
+        <v>34</v>
+      </c>
+      <c r="U73" t="s">
+        <v>34</v>
+      </c>
+      <c r="V73" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="10:19">
-      <c r="J74" t="s">
-        <v>34</v>
-      </c>
-      <c r="K74" t="s">
-        <v>34</v>
-      </c>
-      <c r="L74" t="s">
-        <v>34</v>
-      </c>
-      <c r="M74" t="s">
-        <v>34</v>
-      </c>
-      <c r="N74" t="s">
-        <v>34</v>
-      </c>
-      <c r="O74" t="s">
-        <v>34</v>
-      </c>
+    <row r="74" spans="16:25">
       <c r="P74" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>34</v>
+      </c>
+      <c r="R74" t="s">
+        <v>34</v>
+      </c>
+      <c r="S74" t="s">
+        <v>34</v>
+      </c>
+      <c r="T74" t="s">
+        <v>34</v>
+      </c>
+      <c r="U74" t="s">
+        <v>34</v>
+      </c>
+      <c r="V74" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="75" spans="10:19">
-      <c r="J75" t="s">
-        <v>34</v>
-      </c>
-      <c r="K75" t="s">
-        <v>34</v>
-      </c>
-      <c r="L75" t="s">
-        <v>34</v>
-      </c>
-      <c r="M75" t="s">
-        <v>34</v>
-      </c>
-      <c r="N75" t="s">
-        <v>34</v>
-      </c>
-      <c r="O75" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="76" spans="10:19">
-      <c r="J76" t="s">
-        <v>34</v>
-      </c>
-      <c r="K76" t="s">
-        <v>34</v>
-      </c>
-      <c r="L76" t="s">
-        <v>34</v>
-      </c>
-      <c r="M76" t="s">
-        <v>34</v>
-      </c>
-      <c r="N76" t="s">
-        <v>34</v>
-      </c>
-      <c r="O76" t="s">
+    <row r="75" spans="16:25">
+      <c r="P75" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>34</v>
+      </c>
+      <c r="R75" t="s">
+        <v>34</v>
+      </c>
+      <c r="S75" t="s">
+        <v>34</v>
+      </c>
+      <c r="T75" t="s">
+        <v>34</v>
+      </c>
+      <c r="U75" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" spans="16:25">
+      <c r="P76" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>34</v>
+      </c>
+      <c r="R76" t="s">
+        <v>34</v>
+      </c>
+      <c r="S76" t="s">
+        <v>34</v>
+      </c>
+      <c r="T76" t="s">
+        <v>34</v>
+      </c>
+      <c r="U76" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="77" spans="10:19">
-      <c r="J77" t="s">
-        <v>34</v>
-      </c>
-      <c r="K77" t="s">
-        <v>34</v>
-      </c>
-      <c r="L77" t="s">
-        <v>34</v>
-      </c>
-      <c r="M77" t="s">
-        <v>34</v>
-      </c>
-      <c r="N77" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="78" spans="10:19">
-      <c r="J78" t="s">
-        <v>34</v>
-      </c>
-      <c r="K78" t="s">
-        <v>34</v>
-      </c>
-      <c r="L78" t="s">
-        <v>34</v>
-      </c>
-      <c r="M78" t="s">
-        <v>34</v>
-      </c>
-      <c r="N78" t="s">
+    <row r="77" spans="16:25">
+      <c r="P77" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>34</v>
+      </c>
+      <c r="R77" t="s">
+        <v>34</v>
+      </c>
+      <c r="S77" t="s">
+        <v>34</v>
+      </c>
+      <c r="T77" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="78" spans="16:25">
+      <c r="P78" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>34</v>
+      </c>
+      <c r="R78" t="s">
+        <v>34</v>
+      </c>
+      <c r="S78" t="s">
+        <v>34</v>
+      </c>
+      <c r="T78" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="10:19">
-      <c r="J79" t="s">
-        <v>34</v>
-      </c>
-      <c r="K79" t="s">
-        <v>34</v>
-      </c>
-      <c r="L79" t="s">
-        <v>34</v>
-      </c>
-      <c r="M79" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="80" spans="10:19">
-      <c r="J80" t="s">
-        <v>34</v>
-      </c>
-      <c r="K80" t="s">
-        <v>34</v>
-      </c>
-      <c r="L80" t="s">
-        <v>34</v>
-      </c>
-      <c r="M80" t="s">
+    <row r="79" spans="16:25">
+      <c r="P79" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>34</v>
+      </c>
+      <c r="R79" t="s">
+        <v>34</v>
+      </c>
+      <c r="S79" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="80" spans="16:25">
+      <c r="P80" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>34</v>
+      </c>
+      <c r="R80" t="s">
+        <v>34</v>
+      </c>
+      <c r="S80" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="10:13">
-      <c r="J81" t="s">
-        <v>34</v>
-      </c>
-      <c r="K81" t="s">
-        <v>34</v>
-      </c>
-      <c r="L81" t="s">
-        <v>34</v>
-      </c>
-      <c r="M81" t="s">
+    <row r="81" spans="16:19">
+      <c r="P81" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>34</v>
+      </c>
+      <c r="R81" t="s">
+        <v>34</v>
+      </c>
+      <c r="S81" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="10:13">
-      <c r="J82" t="s">
-        <v>34</v>
-      </c>
-      <c r="K82" t="s">
-        <v>34</v>
-      </c>
-      <c r="L82" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="83" spans="10:13">
-      <c r="J83" t="s">
-        <v>34</v>
-      </c>
-      <c r="K83" t="s">
-        <v>34</v>
-      </c>
-      <c r="L83" t="s">
+    <row r="82" spans="16:19">
+      <c r="P82" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>34</v>
+      </c>
+      <c r="R82" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="83" spans="16:19">
+      <c r="P83" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>34</v>
+      </c>
+      <c r="R83" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="84" spans="10:13">
-      <c r="J84" t="s">
-        <v>34</v>
-      </c>
-      <c r="K84" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="85" spans="10:13">
-      <c r="J85" t="s">
-        <v>34</v>
-      </c>
-      <c r="K85" t="s">
+    <row r="84" spans="16:19">
+      <c r="P84" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="16:19">
+      <c r="P85" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q85" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="86" spans="10:13">
-      <c r="J86" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="87" spans="10:13">
-      <c r="J87" t="s">
+    <row r="86" spans="16:19">
+      <c r="P86" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="87" spans="16:19">
+      <c r="P87" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: partly implement of new semi lock-free memory allocator
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/Design_general_mem_alloc.xlsx
+++ b/libalconcurrent/doc/Design_general_mem_alloc.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CCE3BA-7910-471E-ADC0-75A0015859D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCE364A-880D-400B-8951-748F8CE76B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="-&gt; redesigning" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="152">
   <si>
     <t>param_chunk_allocation</t>
   </si>
@@ -554,6 +556,862 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>小さいメモリ</t>
+    <rPh sb="0" eb="1">
+      <t>チイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>固定サイズで配列として用意された領域から割り当てる</t>
+    <rPh sb="0" eb="2">
+      <t>コテイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ハイレツ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ヨウイ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>リョウイキ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ア</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>大きいメモリ</t>
+    <rPh sb="0" eb="1">
+      <t>オオ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>大きすぎるメモリ</t>
+    <rPh sb="0" eb="1">
+      <t>オオ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmapで割り当てる。解放処理も即時解放</t>
+    <rPh sb="5" eb="6">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="11" eb="15">
+      <t>カイホウショリ</t>
+    </rPh>
+    <rPh sb="16" eb="20">
+      <t>ソクジカイホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmapで割り当てる。ただし、再割り当てしやすいように、解放処理は遅延させる。</t>
+    <rPh sb="5" eb="6">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>カイホウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>チエン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>例えば、再割り当てはスタックの先頭から、解放はスタック構造の後ろからスティールして解放する等。</t>
+    <rPh sb="0" eb="1">
+      <t>タト</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>サイワ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>セントウ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>カイホウ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>コウゾウ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>ウシ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>カイホウ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>ナド</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>不定値</t>
+    <rPh sb="0" eb="3">
+      <t>フテイチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>小さいメモリ： 01</t>
+    <rPh sb="0" eb="1">
+      <t>チイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>大きいメモリ： 10</t>
+    <rPh sb="0" eb="1">
+      <t>オオ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>大きすぎるメモリ： 11</t>
+    <rPh sb="0" eb="1">
+      <t>オオ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>uintptr_t</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">     :</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>不定値（確保した場所の先頭アドレスとして返却する場所）</t>
+    <rPh sb="0" eb="3">
+      <t>フテイチ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>カクホ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>バショ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>セントウ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ヘンキャク</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>バショ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>不定値</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>未割当先頭ポインタの指す先</t>
+    <rPh sb="0" eb="3">
+      <t>ミワリアテ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>セントウ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>サ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>サキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>未割当先頭ポインタの指す先</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>+アライメント要求により先頭アドレスがずれた場合</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>+アライメント要求と先頭アドレスが一致した場合</t>
+    <rPh sb="17" eb="19">
+      <t>イッチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>小さいメモリ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmap確保し、割り当て中</t>
+    <rPh sb="4" eb="6">
+      <t>カクホ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>チュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>未割当(使用しない見込み)： 00</t>
+    <rPh sb="0" eb="3">
+      <t>ミワリアテ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ミコ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>下位3ビットのフラグ情報の構成</t>
+    <rPh sb="0" eb="2">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>コウセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>第0，および第1ビット：　メモリ種別を表す2ビットの情報</t>
+    <rPh sb="0" eb="1">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>シュベツ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>アラワ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メモリ種別</t>
+    <rPh sb="3" eb="5">
+      <t>シュベツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>上記3種類と未割当を示す4種類を区別するための2ビットのフラグ情報</t>
+    <rPh sb="0" eb="2">
+      <t>ジョウキ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>シュルイ</t>
+    </rPh>
+    <rPh sb="6" eb="9">
+      <t>ミワリアテ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>シメ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>シュルイ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>クベツ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>管理構造体へのアドレス
+下位3ビットのフラグ情報(101)</t>
+    <rPh sb="0" eb="5">
+      <t>カンリコウゾウタイ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>確保したメモリサイズ</t>
+    <rPh sb="0" eb="2">
+      <t>カクホ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>+アライメント要求と先頭アドレスが一致した場合</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>先頭のアドレス
+下位3ビットのフラグ情報(111)</t>
+    <rPh sb="0" eb="2">
+      <t>セントウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>確保したメモリサイズ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スタック構造を構成するための、次の「回収済み再割り当て待ち」スロットへのアドレスを保持するアトミック変数
++
+下位3ビットのフラグ情報(010)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>先頭へのアドレスを保持するアトミック変数
+下位3ビットのフラグ情報(110)</t>
+    <rPh sb="0" eb="2">
+      <t>セントウ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>先頭へのアドレスを保持するアトミック変数
+下位3ビットのフラグ情報(110)</t>
+    <rPh sb="0" eb="2">
+      <t>セントウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>+アライメント要求により先頭アドレスがずれた場合#2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>magic number</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次の追加構造体へのポインタを保持するアトミック変数</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="4" eb="7">
+      <t>コウゾウタイ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットグループ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>１スロットのバイトサイズ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットグループリスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットグループとして確保するバイトサイズの最大サイズ</t>
+    <rPh sb="11" eb="13">
+      <t>カクホ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>サイダイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>グローバル変数</t>
+    <rPh sb="5" eb="7">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>グローバル定数</t>
+    <rPh sb="5" eb="7">
+      <t>テイスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>先頭のスロットグループへのポインタを保持するアトミック変数</t>
+    <rPh sb="0" eb="2">
+      <t>セントウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>現在参照している未割当スロットを参照するスロットグループへのポインタを保持するアトミック変数</t>
+    <rPh sb="0" eb="2">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ワリアテ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「回収済み＋再割り当て待ち」のスタックリストの先頭ポインタを保持するアトミック変数</t>
+    <rPh sb="23" eb="25">
+      <t>セントウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">      :</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「割り当て中」のスロット</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「未割当」のスロット</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「回収済み＋再割り当て待ち」スロット</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「小さいメモリ」スロットの配列[0]</t>
+    <rPh sb="1" eb="2">
+      <t>チイ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ハイレツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「小さいメモリ」スロットの配列[1]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「小さいメモリ」スロットの配列[n]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>１スロットのバイトサイズ（定数）</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>管理構造体へのアドレスを保持するアトミック変数
+下位3ビットのフラグ情報(101)</t>
+    <rPh sb="0" eb="2">
+      <t>カンリ</t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t>コウゾウタイ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>下位3ビットのフラグ情報(001)
+第3ビット以上の上位ビットは、不定値という値を保持するアトミック変数</t>
+    <rPh sb="0" eb="2">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ジョウイ</t>
+    </rPh>
+    <rPh sb="33" eb="36">
+      <t>フテイチ</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「小さいメモリ」スロットグループの管理構造体</t>
+    <rPh sb="1" eb="2">
+      <t>チイ</t>
+    </rPh>
+    <rPh sb="17" eb="22">
+      <t>カンリコウゾウタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「大きいメモリ」の管理構造体</t>
+    <rPh sb="1" eb="2">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="9" eb="14">
+      <t>カンリコウゾウタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>不定値</t>
+    <rPh sb="0" eb="2">
+      <t>フテイ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「小さいメモリ」スロットグループリストをスロットサイズ毎に保持する配列</t>
+    <rPh sb="1" eb="2">
+      <t>チイ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>マイ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ハイレツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットグループリスト[0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットグループリスト[n]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットグループリスト[1]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットグループリストの数</t>
+    <rPh sb="12" eb="13">
+      <t>カズ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>第2ビット： 割り当て中、あるいは解放済みを表す。0: 解放済み、1: 割り当て中</t>
+    <rPh sb="0" eb="1">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>チュウ</t>
+    </rPh>
+    <rPh sb="17" eb="20">
+      <t>カイホウズ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>アラワ</t>
+    </rPh>
+    <rPh sb="28" eb="31">
+      <t>カイホウズ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>チュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「小さいメモリ」の確保/解放のコールスタック情報[0] (オプション)</t>
+    <rPh sb="9" eb="11">
+      <t>カクホ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>カイホウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「小さいメモリ」の確保/解放のコールスタック情報[1] (オプション)</t>
+    <rPh sb="9" eb="11">
+      <t>カクホ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>カイホウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「小さいメモリ」の確保/解放のコールスタック情報[n] (オプション)</t>
+    <rPh sb="9" eb="11">
+      <t>カクホ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>カイホウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「大きいメモリ」の確保/解放のコールスタック情報 (オプション)</t>
+    <rPh sb="1" eb="2">
+      <t>オオ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「大きすぎるメモリ」の確保/解放のコールスタック情報 (オプション)</t>
+    <rPh sb="1" eb="2">
+      <t>オオ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>下位3ビットのフラグ情報(010)
+第3ビット以上の上位ビットは、不定値を保持するアトミック変数</t>
+    <rPh sb="0" eb="2">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ジョウイ</t>
+    </rPh>
+    <rPh sb="33" eb="36">
+      <t>フテイチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>+アライメント要求により先頭アドレスがずれた場合#1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スタック構造を構成するための、次の「回収済み再割り当て待ち」スロットへのアドレスを保持するアトミック変数
++
+下位3ビットのフラグ情報(001)</t>
+    <rPh sb="4" eb="6">
+      <t>コウゾウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>コウセイ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>カイシュウ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ズ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>サイワ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>マ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メモリスロットの最終アドレスへのポインタ（定数）</t>
+    <rPh sb="8" eb="10">
+      <t>サイシュウ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>テイスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>未割当の先頭スロットへのポインタを保持するアトミック変数</t>
+    <rPh sb="0" eb="3">
+      <t>ミワリアテ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>セントウ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロット数（定数）</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次に行うスロットグループのためのバッファ確保時に使用するバイトサイズの値を保持するアトミック変数</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>カクホ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ヘンスウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -577,15 +1435,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -791,11 +1661,184 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -812,10 +1855,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -846,6 +1885,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -6626,6 +7745,2025 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2162175</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="吹き出し: 角を丸めた四角形 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{254CB573-5A9F-6706-B090-4F911C4CB7FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11953875" y="3524250"/>
+          <a:ext cx="2143125" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 21165"/>
+            <a:gd name="adj2" fmla="val 106362"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>この構造を構成するため、アライメントの最小値は</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+            <a:t>sizeof(uintptr_t)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>に制約される</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="吹き出し: 角を丸めた四角形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3199AE79-F0D4-48E6-B0E8-9E27D1591C23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6296024" y="1962150"/>
+          <a:ext cx="3171825" cy="1438275"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -132822"/>
+            <a:gd name="adj2" fmla="val -21675"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>このフラグ情報ビットの領域を確保するため、確保するメモリの最小サイズは</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+            <a:t>4byte</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>以上に制約される。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>これは、最小アライメント値が</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+            <a:t>4byte</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>以上に制約されることも意味する。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>342901</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1847851</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="吹き出し: 角を丸めた四角形 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AFE6EEC-BFF9-4D2B-B37B-9E988DCA9EBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16278226" y="2152650"/>
+          <a:ext cx="4343400" cy="1933576"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 22536"/>
+            <a:gd name="adj2" fmla="val 84405"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>効率的な再割り当てが行われるアルゴリズムが必要。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>検討する上で「効率的」の効率を定義する必要あり。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>そのうえで、トレードオフを考える必要がある。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>たとえば、「メモリ効率はいいが、再割り当ては遅い。ただし</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+            <a:t>lock-free</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>としてふるまえる」等</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2076450</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="吹き出し: 角を丸めた四角形 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3528380-0301-4814-BDDD-604D006437C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14754225" y="2943226"/>
+          <a:ext cx="2076450" cy="1485900"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 21165"/>
+            <a:gd name="adj2" fmla="val 106362"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>この構造を構成するため、最小スロットサイズは、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+            <a:t>sizeof(std::atomic&lt;T*&gt;)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>、あるいは</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+            <a:t>sizeof(uintptr_t)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>の大きい方に制約される。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>2057400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="直線矢印コネクタ 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12D86AD9-3AA4-241F-FCA5-EEB99F96CCDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20983575" y="8601075"/>
+          <a:ext cx="819150" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2114550</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="直線矢印コネクタ 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDBBC12C-F391-51B9-34A5-43504C9282C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11925300" y="7620000"/>
+          <a:ext cx="4410075" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2143125</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>447675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>447675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="直線矢印コネクタ 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F70BCDE-A092-1E93-792D-C0C61F1E6CD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14763750" y="8801100"/>
+          <a:ext cx="1352550" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1952625</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1104900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1104900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="直線矢印コネクタ 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{186C9F76-650B-3FEB-CC3B-83FD6013B72F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20802600" y="7553325"/>
+          <a:ext cx="3886200" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2038350</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="フリーフォーム: 図形 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F22AFD-52EC-6902-E8E3-1C85E396E347}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6162675" y="20231100"/>
+          <a:ext cx="2952750" cy="1504950"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 2952750"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 1504950"/>
+            <a:gd name="connsiteX1" fmla="*/ 838200 w 2952750"/>
+            <a:gd name="connsiteY1" fmla="*/ 0 h 1504950"/>
+            <a:gd name="connsiteX2" fmla="*/ 2276475 w 2952750"/>
+            <a:gd name="connsiteY2" fmla="*/ 1504950 h 1504950"/>
+            <a:gd name="connsiteX3" fmla="*/ 2952750 w 2952750"/>
+            <a:gd name="connsiteY3" fmla="*/ 1504950 h 1504950"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="2952750" h="1504950">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="838200" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2276475" y="1504950"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2952750" y="1504950"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2019300</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>609599</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="フリーフォーム: 図形 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04C05BEE-CD8C-4875-B3FA-E7DC3794B788}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6143625" y="21164549"/>
+          <a:ext cx="2952750" cy="4124325"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 2952750"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 1504950"/>
+            <a:gd name="connsiteX1" fmla="*/ 838200 w 2952750"/>
+            <a:gd name="connsiteY1" fmla="*/ 0 h 1504950"/>
+            <a:gd name="connsiteX2" fmla="*/ 2276475 w 2952750"/>
+            <a:gd name="connsiteY2" fmla="*/ 1504950 h 1504950"/>
+            <a:gd name="connsiteX3" fmla="*/ 2952750 w 2952750"/>
+            <a:gd name="connsiteY3" fmla="*/ 1504950 h 1504950"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="2952750" h="1504950">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="838200" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2276475" y="1504950"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2952750" y="1504950"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2009775</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>628649</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="フリーフォーム: 図形 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F96DC759-FB0B-46A5-A8B1-488BAC1A06FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6134100" y="22145624"/>
+          <a:ext cx="2952750" cy="7934326"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 2952750"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 1504950"/>
+            <a:gd name="connsiteX1" fmla="*/ 838200 w 2952750"/>
+            <a:gd name="connsiteY1" fmla="*/ 0 h 1504950"/>
+            <a:gd name="connsiteX2" fmla="*/ 2276475 w 2952750"/>
+            <a:gd name="connsiteY2" fmla="*/ 1504950 h 1504950"/>
+            <a:gd name="connsiteX3" fmla="*/ 2952750 w 2952750"/>
+            <a:gd name="connsiteY3" fmla="*/ 1504950 h 1504950"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="2952750" h="1504950">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="838200" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2276475" y="1504950"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2952750" y="1504950"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>619125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="フリーフォーム: 図形 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42A72B25-E384-4AA4-AF2D-0A83CBC4600B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22774275" y="24831675"/>
+          <a:ext cx="3429000" cy="1238250"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 3076575 w 3886200"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 2219325"/>
+            <a:gd name="connsiteX1" fmla="*/ 3571875 w 3886200"/>
+            <a:gd name="connsiteY1" fmla="*/ 0 h 2219325"/>
+            <a:gd name="connsiteX2" fmla="*/ 3886200 w 3886200"/>
+            <a:gd name="connsiteY2" fmla="*/ 314325 h 2219325"/>
+            <a:gd name="connsiteX3" fmla="*/ 3886200 w 3886200"/>
+            <a:gd name="connsiteY3" fmla="*/ 1333500 h 2219325"/>
+            <a:gd name="connsiteX4" fmla="*/ 3533775 w 3886200"/>
+            <a:gd name="connsiteY4" fmla="*/ 1685925 h 2219325"/>
+            <a:gd name="connsiteX5" fmla="*/ 685800 w 3886200"/>
+            <a:gd name="connsiteY5" fmla="*/ 1685925 h 2219325"/>
+            <a:gd name="connsiteX6" fmla="*/ 0 w 3886200"/>
+            <a:gd name="connsiteY6" fmla="*/ 1885950 h 2219325"/>
+            <a:gd name="connsiteX7" fmla="*/ 0 w 3886200"/>
+            <a:gd name="connsiteY7" fmla="*/ 2009775 h 2219325"/>
+            <a:gd name="connsiteX8" fmla="*/ 304800 w 3886200"/>
+            <a:gd name="connsiteY8" fmla="*/ 2219325 h 2219325"/>
+            <a:gd name="connsiteX9" fmla="*/ 609600 w 3886200"/>
+            <a:gd name="connsiteY9" fmla="*/ 2219325 h 2219325"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX9" y="connsiteY9"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="3886200" h="2219325">
+              <a:moveTo>
+                <a:pt x="3076575" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="3571875" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="3886200" y="314325"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="3886200" y="1333500"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="3533775" y="1685925"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="685800" y="1685925"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="1885950"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="2009775"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="304800" y="2219325"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="609600" y="2219325"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>2085975</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>476250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="フリーフォーム: 図形 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6C83F0E-FB16-48D8-88FC-F7DAA1F89282}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19621500" y="19392900"/>
+          <a:ext cx="3771900" cy="2286000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 2952750"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 1504950"/>
+            <a:gd name="connsiteX1" fmla="*/ 838200 w 2952750"/>
+            <a:gd name="connsiteY1" fmla="*/ 0 h 1504950"/>
+            <a:gd name="connsiteX2" fmla="*/ 2276475 w 2952750"/>
+            <a:gd name="connsiteY2" fmla="*/ 1504950 h 1504950"/>
+            <a:gd name="connsiteX3" fmla="*/ 2952750 w 2952750"/>
+            <a:gd name="connsiteY3" fmla="*/ 1504950 h 1504950"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="2952750" h="1504950">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="838200" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2276475" y="1504950"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2952750" y="1504950"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="フリーフォーム: 図形 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8262D4AC-0E24-6F23-FC0F-000E838D2F3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4962525" y="23831550"/>
+          <a:ext cx="1638300" cy="10020300"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 1104900 w 1638300"/>
+            <a:gd name="connsiteY0" fmla="*/ 6686550 h 6686550"/>
+            <a:gd name="connsiteX1" fmla="*/ 1400175 w 1638300"/>
+            <a:gd name="connsiteY1" fmla="*/ 6686550 h 6686550"/>
+            <a:gd name="connsiteX2" fmla="*/ 1638300 w 1638300"/>
+            <a:gd name="connsiteY2" fmla="*/ 6448425 h 6686550"/>
+            <a:gd name="connsiteX3" fmla="*/ 1638300 w 1638300"/>
+            <a:gd name="connsiteY3" fmla="*/ 5915025 h 6686550"/>
+            <a:gd name="connsiteX4" fmla="*/ 0 w 1638300"/>
+            <a:gd name="connsiteY4" fmla="*/ 0 h 6686550"/>
+            <a:gd name="connsiteX5" fmla="*/ 0 w 1638300"/>
+            <a:gd name="connsiteY5" fmla="*/ 0 h 6686550"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="1638300" h="6686550">
+              <a:moveTo>
+                <a:pt x="1104900" y="6686550"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="1400175" y="6686550"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1638300" y="6448425"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1638300" y="5915025"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="0"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="吹き出し: 角を丸めた四角形 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{662D5F3B-9928-48EB-A040-09AD50B3B039}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1038225" y="25107900"/>
+          <a:ext cx="2143125" cy="1114425"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 102943"/>
+            <a:gd name="adj2" fmla="val -91052"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+            <a:t>ABA</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>問題は発生しないはずなので、ハザードポインタの管理は不要のはず。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1895475</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>47623</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1838324</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>638175</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="吹き出し: 角を丸めた四角形 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55A00FDC-8FF7-4092-A09A-40FA52E814B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14544675" y="21602698"/>
+          <a:ext cx="3543299" cy="1323977"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 76364"/>
+            <a:gd name="adj2" fmla="val -20306"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+            <a:t>OS</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>との確保</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+            <a:t>/</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>解放が介在するため、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+            <a:t>ABA</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>問題が発生するが、メモリ領域の中身については関知しないため、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+            <a:t>ABA</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>問題が発生していても、影響を受けない。</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+          </a:br>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>よって、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+            <a:t>ABA</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>問題対応は不要。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2000250</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="直線矢印コネクタ 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB2B5758-846D-9A42-9DBC-5CC9E510150D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8696325" y="6200775"/>
+          <a:ext cx="6076950" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="フリーフォーム: 図形 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C2EDE71-8C34-C598-C6BB-310CBB317725}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8858250" y="23783925"/>
+          <a:ext cx="3571875" cy="3943350"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 2695575 w 3571875"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 3943350"/>
+            <a:gd name="connsiteX1" fmla="*/ 3333750 w 3571875"/>
+            <a:gd name="connsiteY1" fmla="*/ 0 h 3943350"/>
+            <a:gd name="connsiteX2" fmla="*/ 3571875 w 3571875"/>
+            <a:gd name="connsiteY2" fmla="*/ 238125 h 3943350"/>
+            <a:gd name="connsiteX3" fmla="*/ 3571875 w 3571875"/>
+            <a:gd name="connsiteY3" fmla="*/ 3124200 h 3943350"/>
+            <a:gd name="connsiteX4" fmla="*/ 3343275 w 3571875"/>
+            <a:gd name="connsiteY4" fmla="*/ 3352800 h 3943350"/>
+            <a:gd name="connsiteX5" fmla="*/ 209550 w 3571875"/>
+            <a:gd name="connsiteY5" fmla="*/ 3352800 h 3943350"/>
+            <a:gd name="connsiteX6" fmla="*/ 0 w 3571875"/>
+            <a:gd name="connsiteY6" fmla="*/ 3562350 h 3943350"/>
+            <a:gd name="connsiteX7" fmla="*/ 0 w 3571875"/>
+            <a:gd name="connsiteY7" fmla="*/ 3743325 h 3943350"/>
+            <a:gd name="connsiteX8" fmla="*/ 200025 w 3571875"/>
+            <a:gd name="connsiteY8" fmla="*/ 3943350 h 3943350"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="3571875" h="3943350">
+              <a:moveTo>
+                <a:pt x="2695575" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="3333750" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="3571875" y="238125"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="3571875" y="3124200"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="3343275" y="3352800"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="209550" y="3352800"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="3562350"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="3743325"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="200025" y="3943350"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="フリーフォーム: 図形 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37099590-BBD9-4020-8F7A-77654CE3B1EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8877300" y="28584525"/>
+          <a:ext cx="3571875" cy="3943350"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 2695575 w 3571875"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 3943350"/>
+            <a:gd name="connsiteX1" fmla="*/ 3333750 w 3571875"/>
+            <a:gd name="connsiteY1" fmla="*/ 0 h 3943350"/>
+            <a:gd name="connsiteX2" fmla="*/ 3571875 w 3571875"/>
+            <a:gd name="connsiteY2" fmla="*/ 238125 h 3943350"/>
+            <a:gd name="connsiteX3" fmla="*/ 3571875 w 3571875"/>
+            <a:gd name="connsiteY3" fmla="*/ 3124200 h 3943350"/>
+            <a:gd name="connsiteX4" fmla="*/ 3343275 w 3571875"/>
+            <a:gd name="connsiteY4" fmla="*/ 3352800 h 3943350"/>
+            <a:gd name="connsiteX5" fmla="*/ 209550 w 3571875"/>
+            <a:gd name="connsiteY5" fmla="*/ 3352800 h 3943350"/>
+            <a:gd name="connsiteX6" fmla="*/ 0 w 3571875"/>
+            <a:gd name="connsiteY6" fmla="*/ 3562350 h 3943350"/>
+            <a:gd name="connsiteX7" fmla="*/ 0 w 3571875"/>
+            <a:gd name="connsiteY7" fmla="*/ 3743325 h 3943350"/>
+            <a:gd name="connsiteX8" fmla="*/ 200025 w 3571875"/>
+            <a:gd name="connsiteY8" fmla="*/ 3943350 h 3943350"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="3571875" h="3943350">
+              <a:moveTo>
+                <a:pt x="2695575" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="3333750" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="3571875" y="238125"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="3571875" y="3124200"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="3343275" y="3352800"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="209550" y="3352800"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="3562350"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="3743325"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="200025" y="3943350"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1400175</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="フリーフォーム: 図形 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3FFF05A-8027-5D72-52E9-6A3D576EE156}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8810625" y="25431750"/>
+          <a:ext cx="1047750" cy="3905250"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 762000 w 762000"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 3667125"/>
+            <a:gd name="connsiteX1" fmla="*/ 285750 w 762000"/>
+            <a:gd name="connsiteY1" fmla="*/ 0 h 3667125"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 762000"/>
+            <a:gd name="connsiteY2" fmla="*/ 285750 h 3667125"/>
+            <a:gd name="connsiteX3" fmla="*/ 0 w 762000"/>
+            <a:gd name="connsiteY3" fmla="*/ 3314700 h 3667125"/>
+            <a:gd name="connsiteX4" fmla="*/ 352425 w 762000"/>
+            <a:gd name="connsiteY4" fmla="*/ 3667125 h 3667125"/>
+            <a:gd name="connsiteX5" fmla="*/ 742950 w 762000"/>
+            <a:gd name="connsiteY5" fmla="*/ 3667125 h 3667125"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="762000" h="3667125">
+              <a:moveTo>
+                <a:pt x="762000" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="285750" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="285750"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="3314700"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="352425" y="3667125"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="742950" y="3667125"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1743075</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>276225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="フリーフォーム: 図形 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{544A9333-C3D4-421E-AE45-0488ECA55E4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9153525" y="26431875"/>
+          <a:ext cx="704850" cy="2466975"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 762000 w 762000"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 3667125"/>
+            <a:gd name="connsiteX1" fmla="*/ 285750 w 762000"/>
+            <a:gd name="connsiteY1" fmla="*/ 0 h 3667125"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 762000"/>
+            <a:gd name="connsiteY2" fmla="*/ 285750 h 3667125"/>
+            <a:gd name="connsiteX3" fmla="*/ 0 w 762000"/>
+            <a:gd name="connsiteY3" fmla="*/ 3314700 h 3667125"/>
+            <a:gd name="connsiteX4" fmla="*/ 352425 w 762000"/>
+            <a:gd name="connsiteY4" fmla="*/ 3667125 h 3667125"/>
+            <a:gd name="connsiteX5" fmla="*/ 742950 w 762000"/>
+            <a:gd name="connsiteY5" fmla="*/ 3667125 h 3667125"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="762000" h="3667125">
+              <a:moveTo>
+                <a:pt x="762000" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="285750" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="285750"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="3314700"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="352425" y="3667125"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="742950" y="3667125"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6897,7 +10035,7 @@
   <dimension ref="B3:Y40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G1" sqref="B1:G1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -7168,7 +10306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FCA077-D2DC-4602-9CF2-A8F5DAEA3F68}">
   <dimension ref="A3:AA87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
@@ -7198,55 +10336,55 @@
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="17"/>
-      <c r="W4" s="27" t="s">
+      <c r="J4" s="15"/>
+      <c r="W4" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="X4" s="28"/>
-      <c r="Z4" s="27" t="s">
+      <c r="X4" s="26"/>
+      <c r="Z4" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="AA4" s="28"/>
+      <c r="AA4" s="26"/>
     </row>
     <row r="5" spans="1:27" ht="38.25" thickTop="1">
-      <c r="I5" s="18"/>
-      <c r="J5" s="19" t="s">
+      <c r="I5" s="16"/>
+      <c r="J5" s="17" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="19.5" thickBot="1">
-      <c r="I6" s="18"/>
-      <c r="J6" s="20" t="s">
+      <c r="I6" s="16"/>
+      <c r="J6" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="19.5" thickBot="1">
-      <c r="I7" s="18"/>
-      <c r="J7" s="20" t="s">
+      <c r="I7" s="16"/>
+      <c r="J7" s="18" t="s">
         <v>14</v>
       </c>
       <c r="P7" t="s">
         <v>44</v>
       </c>
-      <c r="X7" s="29" t="s">
+      <c r="X7" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="AA7" s="29" t="s">
+      <c r="AA7" s="27" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="19.5" thickTop="1">
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="17"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="20" t="s">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="18" t="s">
         <v>15</v>
       </c>
       <c r="P8" t="s">
@@ -7254,16 +10392,15 @@
       </c>
     </row>
     <row r="9" spans="1:27" ht="19.5" thickBot="1">
-      <c r="C9" s="18"/>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="22" t="s">
+      <c r="I9" s="19"/>
+      <c r="J9" s="20" t="s">
         <v>45</v>
       </c>
       <c r="P9" t="s">
@@ -7271,102 +10408,94 @@
       </c>
     </row>
     <row r="10" spans="1:27" ht="19.5" thickTop="1">
-      <c r="C10" s="18"/>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="20"/>
+      <c r="F10" s="18"/>
       <c r="P10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="19.5" thickBot="1">
-      <c r="C11" s="18"/>
-      <c r="D11" s="7">
+      <c r="C11" s="16"/>
+      <c r="D11">
         <v>0</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="20"/>
+      <c r="F11" s="18"/>
       <c r="P11" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:27">
-      <c r="C12" s="18"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="20" t="s">
+      <c r="C12" s="16"/>
+      <c r="F12" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="L12" s="10"/>
+      <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:27" ht="37.5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="24" t="s">
+      <c r="C13" s="16"/>
+      <c r="F13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="11"/>
-      <c r="L13" s="12" t="s">
+      <c r="K13" s="9"/>
+      <c r="L13" s="10" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="37.5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="24" t="s">
+      <c r="C14" s="16"/>
+      <c r="F14" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="11"/>
-      <c r="L14" s="12" t="s">
+      <c r="K14" s="9"/>
+      <c r="L14" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:27">
-      <c r="C15" s="18"/>
-      <c r="D15" s="7">
+      <c r="C15" s="16"/>
+      <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="12" t="s">
+      <c r="F15" s="18"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="10" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:27">
-      <c r="C16" s="18"/>
-      <c r="D16" s="7">
+      <c r="C16" s="16"/>
+      <c r="D16">
         <v>2</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="20"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="13" t="s">
+      <c r="F16" s="18"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="3:20">
-      <c r="C17" s="18"/>
-      <c r="D17" s="8" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="20"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="12" t="s">
+      <c r="F17" s="18"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="10" t="s">
         <v>72</v>
       </c>
       <c r="P17" s="5" t="s">
@@ -7386,14 +10515,13 @@
       </c>
     </row>
     <row r="18" spans="3:20">
-      <c r="C18" s="18"/>
-      <c r="D18" s="8" t="s">
+      <c r="C18" s="16"/>
+      <c r="D18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="20"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="12" t="s">
+      <c r="F18" s="18"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="10" t="s">
         <v>37</v>
       </c>
       <c r="P18" t="s">
@@ -7413,16 +10541,16 @@
       </c>
     </row>
     <row r="19" spans="3:20" ht="19.5" thickBot="1">
-      <c r="C19" s="21"/>
-      <c r="D19" s="25" t="s">
+      <c r="C19" s="19"/>
+      <c r="D19" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="22"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="12" t="s">
+      <c r="F19" s="20"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="10" t="s">
         <v>38</v>
       </c>
       <c r="P19" t="s">
@@ -7442,8 +10570,8 @@
       </c>
     </row>
     <row r="20" spans="3:20" ht="19.5" thickTop="1">
-      <c r="K20" s="11"/>
-      <c r="L20" s="13" t="s">
+      <c r="K20" s="9"/>
+      <c r="L20" s="11" t="s">
         <v>5</v>
       </c>
       <c r="P20" t="s">
@@ -7460,8 +10588,8 @@
       </c>
     </row>
     <row r="21" spans="3:20" ht="19.5" thickBot="1">
-      <c r="K21" s="14"/>
-      <c r="L21" s="15" t="s">
+      <c r="K21" s="12"/>
+      <c r="L21" s="13" t="s">
         <v>39</v>
       </c>
       <c r="P21" t="s">
@@ -7987,4 +11115,1424 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314F6088-FC6E-4EBC-AE09-7FE7329B554B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C554509-BFFA-4011-8804-F6F5DE023F7A}">
+  <dimension ref="B3:X127"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <cols>
+    <col min="5" max="5" width="18.125" customWidth="1"/>
+    <col min="6" max="6" width="27.5" customWidth="1"/>
+    <col min="7" max="7" width="15.625" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
+    <col min="9" max="9" width="4.5" customWidth="1"/>
+    <col min="10" max="10" width="33.75" customWidth="1"/>
+    <col min="11" max="11" width="3.5" customWidth="1"/>
+    <col min="12" max="12" width="29.75" customWidth="1"/>
+    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="14" max="14" width="27.5" customWidth="1"/>
+    <col min="16" max="16" width="28.25" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="18" max="18" width="28.25" customWidth="1"/>
+    <col min="20" max="20" width="28.125" customWidth="1"/>
+    <col min="22" max="22" width="28.375" customWidth="1"/>
+    <col min="24" max="24" width="27.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5">
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="D12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="D16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="4:24">
+      <c r="F21" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="57"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="58"/>
+      <c r="P21" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q21" s="57"/>
+      <c r="R21" s="57"/>
+      <c r="S21" s="57"/>
+      <c r="T21" s="58"/>
+      <c r="V21" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="W21" s="57"/>
+      <c r="X21" s="58"/>
+    </row>
+    <row r="23" spans="4:24">
+      <c r="F23" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H23" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="61"/>
+      <c r="N23" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="P23" s="56" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q23" s="57"/>
+      <c r="R23" s="58"/>
+      <c r="T23" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="V23" s="56" t="s">
+        <v>95</v>
+      </c>
+      <c r="W23" s="57"/>
+      <c r="X23" s="58"/>
+    </row>
+    <row r="24" spans="4:24" ht="38.25" thickBot="1">
+      <c r="H24" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="L24" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="P24" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="R24" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="V24" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="X24" s="42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="4:24" ht="113.25" thickTop="1">
+      <c r="D25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="L25" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="N25" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="P25" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="S25" s="3"/>
+      <c r="T25" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="U25" s="3"/>
+      <c r="V25" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="W25" s="3"/>
+      <c r="X25" s="51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="4:24" ht="75">
+      <c r="D26" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H26" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="52" t="s">
+        <v>129</v>
+      </c>
+      <c r="L26" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N26" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="P26" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="S26" s="3"/>
+      <c r="T26" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="U26" s="3"/>
+      <c r="V26" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="W26" s="3"/>
+      <c r="X26" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="4:24" ht="112.5">
+      <c r="D27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H27" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="J27" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="L27" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N27" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="P27" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="T27" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="V27" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="X27" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="4:24" ht="75">
+      <c r="D28" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H28" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="J28" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="L28" s="52" t="s">
+        <v>129</v>
+      </c>
+      <c r="N28" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="P28" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="R28" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="T28" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="V28" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="X28" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="4:24" ht="37.5">
+      <c r="D29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H29" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="J29" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="L29" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="N29" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="P29" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="R29" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="T29" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="V29" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="X29" s="40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="4:24" ht="75">
+      <c r="D30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H30" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="J30" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="L30" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="N30" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="P30" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="R30" s="52" t="s">
+        <v>108</v>
+      </c>
+      <c r="T30" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="V30" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="X30" s="38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="4:24" ht="37.5">
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H31" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="J31" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="L31" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="N31" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="P31" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="R31" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="T31" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="V31" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="X31" s="35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="4:24">
+      <c r="D32" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H32" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="J32" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="L32" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="N32" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="P32" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="R32" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="T32" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="V32" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="X32" s="35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="4:24">
+      <c r="D33" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="H33" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="I33" s="43"/>
+      <c r="J33" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="L33" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="N33" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="P33" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="R33" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="T33" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="V33" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="X33" s="35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="4:24">
+      <c r="D34" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H34" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="J34" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="L34" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="N34" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="P34" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q34" s="43"/>
+      <c r="R34" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="T34" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="V34" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="X34" s="36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="4:24" ht="19.5" thickBot="1">
+      <c r="D35" t="s">
+        <v>86</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="H35" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="J35" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="L35" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="N35" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="P35" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="R35" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="T35" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="V35" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="X35" s="35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="4:24" ht="39" thickTop="1" thickBot="1">
+      <c r="D36" t="s">
+        <v>86</v>
+      </c>
+      <c r="F36" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="G36" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="H36" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="J36" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="K36" s="41"/>
+      <c r="L36" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="M36" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="N36" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="P36" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="R36" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="T36" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="V36" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="X36" s="37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="4:24" ht="19.5" thickTop="1">
+      <c r="D37" t="s">
+        <v>86</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H37" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J37" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L37" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N37" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="4:24">
+      <c r="D38" t="s">
+        <v>86</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J38" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L38" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N38" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="4:24">
+      <c r="D39" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J39" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L39" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N39" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="4:24">
+      <c r="D40" t="s">
+        <v>86</v>
+      </c>
+      <c r="F40" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H40" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J40" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L40" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N40" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="4:24">
+      <c r="D41" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H41" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J41" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L41" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N41" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="4:24">
+      <c r="D42" t="s">
+        <v>86</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H42" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J42" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L42" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N42" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="4:24">
+      <c r="D43" t="s">
+        <v>86</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H43" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J43" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L43" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N43" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="4:24">
+      <c r="D44" t="s">
+        <v>86</v>
+      </c>
+      <c r="F44" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="H44" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="I44" s="43"/>
+      <c r="J44" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="L44" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="N44" s="32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="4:24">
+      <c r="D45" t="s">
+        <v>86</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H45" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J45" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L45" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N45" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="4:24" ht="19.5" thickBot="1">
+      <c r="D46" t="s">
+        <v>86</v>
+      </c>
+      <c r="F46" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="H46" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="J46" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="L46" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="N46" s="30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="4:24" ht="19.5" thickTop="1">
+      <c r="D47" t="s">
+        <v>86</v>
+      </c>
+      <c r="F47" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="H47" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="J47" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="L47" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="N47" s="28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="4:24">
+      <c r="D48" t="s">
+        <v>86</v>
+      </c>
+      <c r="F48" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H48" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J48" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L48" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N48" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="2:20">
+      <c r="D49" t="s">
+        <v>86</v>
+      </c>
+      <c r="F49" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H49" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J49" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L49" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N49" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="2:20">
+      <c r="D50" t="s">
+        <v>86</v>
+      </c>
+      <c r="F50" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H50" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J50" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L50" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N50" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="2:20">
+      <c r="D51" t="s">
+        <v>86</v>
+      </c>
+      <c r="F51" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H51" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J51" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L51" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N51" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="2:20">
+      <c r="D52" t="s">
+        <v>86</v>
+      </c>
+      <c r="F52" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H52" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J52" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L52" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N52" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="2:20">
+      <c r="D53" t="s">
+        <v>86</v>
+      </c>
+      <c r="F53" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H53" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J53" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L53" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N53" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="2:20">
+      <c r="D54" t="s">
+        <v>86</v>
+      </c>
+      <c r="F54" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H54" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J54" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L54" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N54" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="2:20">
+      <c r="D55" t="s">
+        <v>86</v>
+      </c>
+      <c r="F55" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="H55" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="I55" s="43"/>
+      <c r="J55" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="L55" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="N55" s="32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="2:20">
+      <c r="D56" t="s">
+        <v>86</v>
+      </c>
+      <c r="F56" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H56" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J56" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="L56" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N56" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="2:20" ht="19.5" thickBot="1">
+      <c r="D57" t="s">
+        <v>86</v>
+      </c>
+      <c r="F57" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="H57" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="J57" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="L57" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="N57" s="30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="2:20" ht="19.5" thickTop="1"/>
+    <row r="61" spans="2:20">
+      <c r="B61" t="s">
+        <v>131</v>
+      </c>
+      <c r="O61" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="2:20">
+      <c r="F62" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="G62" s="57"/>
+      <c r="H62" s="57"/>
+      <c r="I62" s="57"/>
+      <c r="J62" s="57"/>
+      <c r="K62" s="57"/>
+      <c r="L62" s="58"/>
+    </row>
+    <row r="63" spans="2:20">
+      <c r="P63" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q63" s="57"/>
+      <c r="R63" s="57"/>
+      <c r="S63" s="57"/>
+      <c r="T63" s="58"/>
+    </row>
+    <row r="64" spans="2:20" ht="19.5" thickBot="1">
+      <c r="F64" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" spans="5:20" ht="19.5" thickTop="1">
+      <c r="E65" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F65" s="31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="66" spans="5:20" ht="38.25" thickBot="1">
+      <c r="E66" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F66" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="O66" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="5:20" ht="76.5" thickTop="1" thickBot="1">
+      <c r="E67" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F67" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="O67" s="1"/>
+      <c r="P67" s="50" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="5:20" ht="57" thickTop="1">
+      <c r="E68" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F68" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="P68" s="2"/>
+    </row>
+    <row r="69" spans="5:20" ht="75.75" thickBot="1">
+      <c r="E69" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F69" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="J69" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="70" spans="5:20" ht="57.75" thickTop="1" thickBot="1">
+      <c r="E70" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F70" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="J70" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="T70" s="48" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="5:20" ht="19.5" thickTop="1">
+      <c r="J71" s="33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="5:20">
+      <c r="J72" s="33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="5:20" ht="37.5">
+      <c r="J73" s="33" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="5:20" ht="38.25" thickBot="1">
+      <c r="J74" s="33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="75" spans="5:20" ht="39" thickTop="1" thickBot="1">
+      <c r="J75" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="T75" s="48" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="5:20" ht="38.25" thickTop="1">
+      <c r="J76" s="33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="77" spans="5:20" ht="37.5">
+      <c r="J77" s="33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="78" spans="5:20">
+      <c r="J78" s="47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="79" spans="5:20" ht="37.5">
+      <c r="J79" s="33" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="80" spans="5:20">
+      <c r="J80" s="33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="81" spans="10:10">
+      <c r="J81" s="33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="82" spans="10:10">
+      <c r="J82" s="47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="83" spans="10:10" ht="19.5" thickBot="1">
+      <c r="J83" s="46" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="84" spans="10:10" ht="19.5" thickTop="1"/>
+    <row r="86" spans="10:10" ht="19.5" thickBot="1"/>
+    <row r="87" spans="10:10" ht="19.5" thickTop="1">
+      <c r="J87" s="31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="88" spans="10:10">
+      <c r="J88" s="33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="89" spans="10:10">
+      <c r="J89" s="33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="90" spans="10:10" ht="37.5">
+      <c r="J90" s="33" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="91" spans="10:10" ht="37.5">
+      <c r="J91" s="33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="92" spans="10:10" ht="37.5">
+      <c r="J92" s="33" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="93" spans="10:10" ht="37.5">
+      <c r="J93" s="33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="94" spans="10:10" ht="37.5">
+      <c r="J94" s="33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" spans="10:10">
+      <c r="J95" s="47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="96" spans="10:10" ht="37.5">
+      <c r="J96" s="33" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="97" spans="10:10">
+      <c r="J97" s="33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="98" spans="10:10">
+      <c r="J98" s="33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="99" spans="10:10">
+      <c r="J99" s="47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="100" spans="10:10" ht="19.5" thickBot="1">
+      <c r="J100" s="46" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="101" spans="10:10" ht="19.5" thickTop="1"/>
+    <row r="103" spans="10:10" ht="19.5" thickBot="1"/>
+    <row r="104" spans="10:10" ht="19.5" thickTop="1">
+      <c r="J104" s="31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="105" spans="10:10">
+      <c r="J105" s="33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="106" spans="10:10">
+      <c r="J106" s="33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="107" spans="10:10" ht="37.5">
+      <c r="J107" s="33" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="108" spans="10:10" ht="37.5">
+      <c r="J108" s="33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="109" spans="10:10" ht="37.5">
+      <c r="J109" s="33" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="110" spans="10:10" ht="37.5">
+      <c r="J110" s="33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="111" spans="10:10" ht="37.5">
+      <c r="J111" s="33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="112" spans="10:10">
+      <c r="J112" s="47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="113" spans="2:10" ht="37.5">
+      <c r="J113" s="33" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="114" spans="2:10">
+      <c r="J114" s="33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="115" spans="2:10">
+      <c r="J115" s="33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="116" spans="2:10">
+      <c r="J116" s="47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="117" spans="2:10" ht="19.5" thickBot="1">
+      <c r="J117" s="46" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="118" spans="2:10" ht="19.5" thickTop="1"/>
+    <row r="121" spans="2:10">
+      <c r="B121" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="123" spans="2:10">
+      <c r="E123" t="s">
+        <v>117</v>
+      </c>
+      <c r="F123" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="124" spans="2:10">
+      <c r="E124" t="s">
+        <v>116</v>
+      </c>
+      <c r="F124" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="125" spans="2:10">
+      <c r="F125" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="126" spans="2:10">
+      <c r="F126" s="43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="127" spans="2:10">
+      <c r="F127" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="V21:X21"/>
+    <mergeCell ref="V23:X23"/>
+    <mergeCell ref="F62:L62"/>
+    <mergeCell ref="P63:T63"/>
+    <mergeCell ref="H23:L23"/>
+    <mergeCell ref="F21:N21"/>
+    <mergeCell ref="P21:T21"/>
+    <mergeCell ref="P23:R23"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add I/F of general memory allocator that is implemented newly.
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/Design_general_mem_alloc.xlsx
+++ b/libalconcurrent/doc/Design_general_mem_alloc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCE364A-880D-400B-8951-748F8CE76B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B94715-91E5-4716-9B29-4D640F7EFEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="155">
   <si>
     <t>param_chunk_allocation</t>
   </si>
@@ -754,13 +754,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>+アライメント要求と先頭アドレスが一致した場合</t>
-    <rPh sb="17" eb="19">
-      <t>イッチ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>小さいメモリ</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -858,13 +851,261 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>管理構造体へのアドレス
-下位3ビットのフラグ情報(101)</t>
-    <rPh sb="0" eb="5">
+    <t>+アライメント要求と先頭アドレスが一致した場合</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>確保したメモリサイズ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>+アライメント要求により先頭アドレスがずれた場合#2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>magic number</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次の追加構造体へのポインタを保持するアトミック変数</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="4" eb="7">
+      <t>コウゾウタイ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットグループ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>１スロットのバイトサイズ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットグループリスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットグループとして確保するバイトサイズの最大サイズ</t>
+    <rPh sb="11" eb="13">
+      <t>カクホ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>サイダイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>グローバル変数</t>
+    <rPh sb="5" eb="7">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>グローバル定数</t>
+    <rPh sb="5" eb="7">
+      <t>テイスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>先頭のスロットグループへのポインタを保持するアトミック変数</t>
+    <rPh sb="0" eb="2">
+      <t>セントウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>現在参照している未割当スロットを参照するスロットグループへのポインタを保持するアトミック変数</t>
+    <rPh sb="0" eb="2">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ワリアテ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「回収済み＋再割り当て待ち」のスタックリストの先頭ポインタを保持するアトミック変数</t>
+    <rPh sb="23" eb="25">
+      <t>セントウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">      :</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「割り当て中」のスロット</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「未割当」のスロット</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「回収済み＋再割り当て待ち」スロット</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「小さいメモリ」スロットの配列[0]</t>
+    <rPh sb="1" eb="2">
+      <t>チイ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ハイレツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「小さいメモリ」スロットの配列[1]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「小さいメモリ」スロットの配列[n]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>１スロットのバイトサイズ（定数）</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「小さいメモリ」スロットグループの管理構造体</t>
+    <rPh sb="1" eb="2">
+      <t>チイ</t>
+    </rPh>
+    <rPh sb="17" eb="22">
       <t>カンリコウゾウタイ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「大きいメモリ」の管理構造体</t>
+    <rPh sb="1" eb="2">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="9" eb="14">
+      <t>カンリコウゾウタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「小さいメモリ」スロットグループリストをスロットサイズ毎に保持する配列</t>
+    <rPh sb="1" eb="2">
+      <t>チイ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>マイ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ハイレツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットグループリスト[0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットグループリスト[n]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットグループリスト[1]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットグループリストの数</t>
+    <rPh sb="12" eb="13">
+      <t>カズ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>第2ビット： 割り当て中、あるいは解放済みを表す。0: 解放済み、1: 割り当て中</t>
+    <rPh sb="0" eb="1">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>チュウ</t>
+    </rPh>
+    <rPh sb="17" eb="20">
+      <t>カイホウズ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>アラワ</t>
+    </rPh>
+    <rPh sb="28" eb="31">
+      <t>カイホウズ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>チュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「小さいメモリ」の確保/解放のコールスタック情報[0] (オプション)</t>
+    <rPh sb="9" eb="11">
+      <t>カクホ</t>
+    </rPh>
     <rPh sb="12" eb="14">
-      <t>カイ</t>
+      <t>カイホウ</t>
     </rPh>
     <rPh sb="22" eb="24">
       <t>ジョウホウ</t>
@@ -872,546 +1113,323 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>確保したメモリサイズ</t>
+    <t>「小さいメモリ」の確保/解放のコールスタック情報[1] (オプション)</t>
+    <rPh sb="9" eb="11">
+      <t>カクホ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>カイホウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「小さいメモリ」の確保/解放のコールスタック情報[n] (オプション)</t>
+    <rPh sb="9" eb="11">
+      <t>カクホ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>カイホウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「大きいメモリ」の確保/解放のコールスタック情報 (オプション)</t>
+    <rPh sb="1" eb="2">
+      <t>オオ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「大きすぎるメモリ」の確保/解放のコールスタック情報 (オプション)</t>
+    <rPh sb="1" eb="2">
+      <t>オオ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メモリスロットの最終アドレスへのポインタ（定数）</t>
+    <rPh sb="8" eb="10">
+      <t>サイシュウ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>テイスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>未割当の先頭スロットへのポインタを保持するアトミック変数</t>
+    <rPh sb="0" eb="3">
+      <t>ミワリアテ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>セントウ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロット数（定数）</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次に行うスロットグループのためのバッファ確保時に使用するバイトサイズの値を保持するアトミック変数</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>カクホ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スタック構造を構成するための、次の「回収済み再割り当て待ち」スロットへのアドレスを保持するアトミック変数によるハザードハンドラ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>不定値（確保した場所の先頭アドレスとして返却する場所）</t>
     <rPh sb="0" eb="2">
+      <t>フテイ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>チ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
       <t>カクホ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>+アライメント要求と先頭アドレスが一致した場合</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>先頭のアドレス
+    <rPh sb="8" eb="10">
+      <t>バショ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>セントウ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ヘンキャク</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>バショ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スタック構造を構成するための、次の「回収済み再割り当て待ち」スロットへのアドレスを保持するアトミック変数によるハザードハンドラ
+※ハザードポインタに登録されている間は、値を維持する必要あり。</t>
+    <rPh sb="74" eb="76">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="81" eb="82">
+      <t>アイダ</t>
+    </rPh>
+    <rPh sb="84" eb="85">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>イジ</t>
+    </rPh>
+    <rPh sb="90" eb="92">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スタック構造を構成するための、次の「回収済み再割り当て待ち」スロットへのアドレスを保持するアトミック変数によるハザードハンドラ
+※ハザードポインタに登録されている間は、値を維持する必要あり。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>管理構造体へのアドレスを保持するアトミック変数(スレッド間で共有されるため)
++
+下位3ビットのフラグ情報(101)</t>
+    <rPh sb="0" eb="2">
+      <t>カンリ</t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t>コウゾウタイ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>キョウユウ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>先頭へのアドレスを保持するアトミック変数(スレッド間で共有されるため)
+＋
+下位3ビットのフラグ情報(110)</t>
+    <rPh sb="0" eb="2">
+      <t>セントウ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>不定値を保持するアトミック変数(スレッド間で共有されるため)
++
+下位3ビットのフラグ情報(010)</t>
+    <rPh sb="0" eb="3">
+      <t>フテイチ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>管理構造体へのアドレスを保持するアトミック変数(スレッド間で共有されるため)
++
+下位3ビットのフラグ情報(101)</t>
+    <rPh sb="0" eb="2">
+      <t>カンリ</t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t>コウゾウタイ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>キョウユウ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>不定値を保持するアトミック変数(スレッド間で共有されるため)
++
+下位3ビットのフラグ情報(001)</t>
+    <rPh sb="0" eb="3">
+      <t>フテイチ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>管理構造体へのアドレスを保持するアトミック変数(スレッド間で共有されるため)
++
+下位3ビットのフラグ情報(001)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ハザードポインタ登録中の場合に使用するスタック構造を構成するためのポインタ</t>
+    <rPh sb="8" eb="11">
+      <t>トウロクチュウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>コウゾウ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>コウセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スロットとして最低限必要な範囲</t>
+    <rPh sb="7" eb="12">
+      <t>サイテイゲンヒツヨウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ハンイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>先頭へのアドレスを保持するアトミック変数(スレッド間で共有されるため)
+＋
+下位3ビットのフラグ情報(010)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>先頭へのアドレスを保持するアトミック変数(スレッド間で共有されるため)
+＋
 下位3ビットのフラグ情報(111)</t>
     <rPh sb="0" eb="2">
       <t>セントウ</t>
     </rPh>
-    <rPh sb="8" eb="10">
+    <rPh sb="38" eb="40">
       <t>カイ</t>
     </rPh>
-    <rPh sb="18" eb="20">
+    <rPh sb="48" eb="50">
       <t>ジョウホウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>確保したメモリサイズ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スタック構造を構成するための、次の「回収済み再割り当て待ち」スロットへのアドレスを保持するアトミック変数
-+
-下位3ビットのフラグ情報(010)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>先頭へのアドレスを保持するアトミック変数
-下位3ビットのフラグ情報(110)</t>
-    <rPh sb="0" eb="2">
-      <t>セントウ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>カイ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>ジョウホウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>先頭へのアドレスを保持するアトミック変数
-下位3ビットのフラグ情報(110)</t>
-    <rPh sb="0" eb="2">
-      <t>セントウ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ホジ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>ヘンスウ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>カイ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>ジョウホウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>+アライメント要求により先頭アドレスがずれた場合#2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>magic number</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>次の追加構造体へのポインタを保持するアトミック変数</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ツイカ</t>
-    </rPh>
-    <rPh sb="4" eb="7">
-      <t>コウゾウタイ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>ホジ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>ヘンスウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スロットグループ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>１スロットのバイトサイズ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スロットグループリスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スロットグループとして確保するバイトサイズの最大サイズ</t>
-    <rPh sb="11" eb="13">
-      <t>カクホ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>サイダイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>グローバル変数</t>
-    <rPh sb="5" eb="7">
-      <t>ヘンスウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>グローバル定数</t>
-    <rPh sb="5" eb="7">
-      <t>テイスウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>先頭のスロットグループへのポインタを保持するアトミック変数</t>
-    <rPh sb="0" eb="2">
-      <t>セントウ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>ホジ</t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t>ヘンスウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>現在参照している未割当スロットを参照するスロットグループへのポインタを保持するアトミック変数</t>
-    <rPh sb="0" eb="2">
-      <t>ゲンザイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>サンショウ</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ワリアテ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>サンショウ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>ホジ</t>
-    </rPh>
-    <rPh sb="44" eb="46">
-      <t>ヘンスウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「回収済み＋再割り当て待ち」のスタックリストの先頭ポインタを保持するアトミック変数</t>
-    <rPh sb="23" eb="25">
-      <t>セントウ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>ホジ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>ヘンスウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">      :</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「割り当て中」のスロット</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「未割当」のスロット</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「回収済み＋再割り当て待ち」スロット</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「小さいメモリ」スロットの配列[0]</t>
-    <rPh sb="1" eb="2">
-      <t>チイ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ハイレツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「小さいメモリ」スロットの配列[1]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「小さいメモリ」スロットの配列[n]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>１スロットのバイトサイズ（定数）</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>管理構造体へのアドレスを保持するアトミック変数
-下位3ビットのフラグ情報(101)</t>
-    <rPh sb="0" eb="2">
-      <t>カンリ</t>
-    </rPh>
-    <rPh sb="2" eb="5">
-      <t>コウゾウタイ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>カイ</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>ジョウホウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>下位3ビットのフラグ情報(001)
-第3ビット以上の上位ビットは、不定値という値を保持するアトミック変数</t>
-    <rPh sb="0" eb="2">
-      <t>カイ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>ダイ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>イジョウ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>ジョウイ</t>
-    </rPh>
-    <rPh sb="33" eb="36">
-      <t>フテイチ</t>
-    </rPh>
-    <rPh sb="39" eb="40">
-      <t>アタイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「小さいメモリ」スロットグループの管理構造体</t>
-    <rPh sb="1" eb="2">
-      <t>チイ</t>
-    </rPh>
-    <rPh sb="17" eb="22">
-      <t>カンリコウゾウタイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「大きいメモリ」の管理構造体</t>
-    <rPh sb="1" eb="2">
-      <t>オオ</t>
-    </rPh>
-    <rPh sb="9" eb="14">
-      <t>カンリコウゾウタイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>不定値</t>
-    <rPh sb="0" eb="2">
-      <t>フテイ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>チ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「小さいメモリ」スロットグループリストをスロットサイズ毎に保持する配列</t>
-    <rPh sb="1" eb="2">
-      <t>チイ</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>マイ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>ホジ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>ハイレツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スロットグループリスト[0]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スロットグループリスト[n]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スロットグループリスト[1]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スロットグループリストの数</t>
-    <rPh sb="12" eb="13">
-      <t>カズ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>第2ビット： 割り当て中、あるいは解放済みを表す。0: 解放済み、1: 割り当て中</t>
-    <rPh sb="0" eb="1">
-      <t>ダイ</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>ワ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>ア</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>チュウ</t>
-    </rPh>
-    <rPh sb="17" eb="20">
-      <t>カイホウズ</t>
-    </rPh>
-    <rPh sb="22" eb="23">
-      <t>アラワ</t>
-    </rPh>
-    <rPh sb="28" eb="31">
-      <t>カイホウズ</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>ワ</t>
-    </rPh>
-    <rPh sb="38" eb="39">
-      <t>ア</t>
-    </rPh>
-    <rPh sb="40" eb="41">
-      <t>チュウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「小さいメモリ」の確保/解放のコールスタック情報[0] (オプション)</t>
-    <rPh sb="9" eb="11">
-      <t>カクホ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>カイホウ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ジョウホウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「小さいメモリ」の確保/解放のコールスタック情報[1] (オプション)</t>
-    <rPh sb="9" eb="11">
-      <t>カクホ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>カイホウ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ジョウホウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「小さいメモリ」の確保/解放のコールスタック情報[n] (オプション)</t>
-    <rPh sb="9" eb="11">
-      <t>カクホ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>カイホウ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ジョウホウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「大きいメモリ」の確保/解放のコールスタック情報 (オプション)</t>
-    <rPh sb="1" eb="2">
-      <t>オオ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「大きすぎるメモリ」の確保/解放のコールスタック情報 (オプション)</t>
-    <rPh sb="1" eb="2">
-      <t>オオ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>下位3ビットのフラグ情報(010)
-第3ビット以上の上位ビットは、不定値を保持するアトミック変数</t>
-    <rPh sb="0" eb="2">
-      <t>カイ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>ダイ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>イジョウ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>ジョウイ</t>
-    </rPh>
-    <rPh sb="33" eb="36">
-      <t>フテイチ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>+アライメント要求により先頭アドレスがずれた場合#1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スタック構造を構成するための、次の「回収済み再割り当て待ち」スロットへのアドレスを保持するアトミック変数
-+
-下位3ビットのフラグ情報(001)</t>
-    <rPh sb="4" eb="6">
-      <t>コウゾウ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>コウセイ</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>カイシュウ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>ズ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>サイワ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>ア</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>マ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>ホジ</t>
-    </rPh>
-    <rPh sb="50" eb="52">
-      <t>ヘンスウ</t>
-    </rPh>
-    <rPh sb="55" eb="57">
-      <t>カイ</t>
-    </rPh>
-    <rPh sb="65" eb="67">
-      <t>ジョウホウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>メモリスロットの最終アドレスへのポインタ（定数）</t>
-    <rPh sb="8" eb="10">
-      <t>サイシュウ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>テイスウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>未割当の先頭スロットへのポインタを保持するアトミック変数</t>
-    <rPh sb="0" eb="3">
-      <t>ミワリアテ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>セントウ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ホジ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>ヘンスウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スロット数（定数）</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>次に行うスロットグループのためのバッファ確保時に使用するバイトサイズの値を保持するアトミック変数</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>カクホ</t>
-    </rPh>
-    <rPh sb="22" eb="23">
-      <t>ジ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
+    <t>スタック構造を構成するための、次の「回収済み再割り当て待ち」スロットへのアドレスを保持するアトミック変数によるハザードハンドラ
+※ただし、使用しない</t>
+    <rPh sb="69" eb="71">
       <t>シヨウ</t>
     </rPh>
-    <rPh sb="35" eb="36">
-      <t>アタイ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>ホジ</t>
-    </rPh>
-    <rPh sb="46" eb="48">
-      <t>ヘンスウ</t>
-    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スタック構造を構成するための、次の「回収済み再割り当て待ち」スロットへのアドレスを保持するアトミック変数によるハザードハンドラ
+※ただし、使用しない</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1435,7 +1453,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1451,6 +1469,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1838,7 +1868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1895,17 +1925,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1915,9 +1938,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1926,25 +1946,62 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
@@ -7928,8 +7985,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>1847851</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
@@ -7946,8 +8003,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16278226" y="2152650"/>
-          <a:ext cx="4343400" cy="1933576"/>
+          <a:off x="19373851" y="2152650"/>
+          <a:ext cx="5210174" cy="1933576"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -8115,15 +8172,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>2057400</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
+      <xdr:colOff>2038350</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1066800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1066800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -8138,167 +8195,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20983575" y="8601075"/>
+          <a:off x="24060150" y="14420850"/>
           <a:ext cx="819150" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>2114550</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>219075</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>219075</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="直線矢印コネクタ 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDBBC12C-F391-51B9-34A5-43504C9282C5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11925300" y="7620000"/>
-          <a:ext cx="4410075" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>2143125</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>447675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>447675</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="直線矢印コネクタ 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F70BCDE-A092-1E93-792D-C0C61F1E6CD4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14763750" y="8801100"/>
-          <a:ext cx="1352550" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1952625</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>1104900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>1104900</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="直線矢印コネクタ 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{186C9F76-650B-3FEB-CC3B-83FD6013B72F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="20802600" y="7553325"/>
-          <a:ext cx="3886200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -8637,14 +8535,14 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>619125</xdr:rowOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>266699</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8659,8 +8557,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22774275" y="24831675"/>
-          <a:ext cx="3429000" cy="1238250"/>
+          <a:off x="24955500" y="28651199"/>
+          <a:ext cx="3429000" cy="2314575"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8788,13 +8686,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>2085975</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>476250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -9187,59 +9085,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>2000250</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="直線矢印コネクタ 29">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB2B5758-846D-9A42-9DBC-5CC9E510150D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8696325" y="6200775"/>
-          <a:ext cx="6076950" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -9733,6 +9578,554 @@
               </a:lnTo>
               <a:lnTo>
                 <a:pt x="742950" y="3667125"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2114550</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1047750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1047750</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="直線矢印コネクタ 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55BB7669-5CDB-488D-97C9-F5F6158DF665}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14144625" y="13211175"/>
+          <a:ext cx="1819275" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>800100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="吹き出し: 角を丸めた四角形 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86277859-021B-C25A-6840-DE86F85A5E1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14925675" y="14154150"/>
+          <a:ext cx="1971675" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -34634"/>
+            <a:gd name="adj2" fmla="val -162615"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+            <a:t>Double Free</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>に備えて、フラグ情報体は維持される</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1019175</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="吹き出し: 角を丸めた四角形 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{510D4374-23BD-4905-8E1B-38A1D18C066C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13049250" y="9420225"/>
+          <a:ext cx="1971675" cy="971550"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 44077"/>
+            <a:gd name="adj2" fmla="val -109069"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+            <a:t>Double Free</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>に備えて、フラグ情報体は維持される</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="吹き出し: 角を丸めた四角形 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01E0203D-EFD1-4CC1-81DD-AC2934587045}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25165051" y="3276600"/>
+          <a:ext cx="5210174" cy="790576"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 23999"/>
+            <a:gd name="adj2" fmla="val 127778"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>解放処理を、専用スレッドに渡すのもあり。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="吹き出し: 角を丸めた四角形 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4860C8ED-18DF-47DA-B5CE-6E98C5B91261}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25165051" y="3286125"/>
+          <a:ext cx="5210174" cy="790576"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -26641"/>
+            <a:gd name="adj2" fmla="val 135007"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>解放処理を、専用スレッドに渡す構造とするのも、良いかもしれない。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>666750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="左中かっこ 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9455461-C427-1E97-2B8A-676790E566F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8848725" y="6162675"/>
+          <a:ext cx="266700" cy="3810000"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 61905"/>
+            <a:gd name="adj2" fmla="val 57750"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2066925</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1057275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1304925</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1057275</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="直線矢印コネクタ 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B5B1D9D-A1B2-4FE2-BEA1-C314C7FF4D4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14097000" y="8458200"/>
+          <a:ext cx="1819275" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2076450</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1066800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1295400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1400175</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="フリーフォーム: 図形 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0B2B663-CB11-D889-82F0-4B5D4796E38A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11268075" y="8467725"/>
+          <a:ext cx="4638675" cy="333375"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 4638675"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 333375"/>
+            <a:gd name="connsiteX1" fmla="*/ 333375 w 4638675"/>
+            <a:gd name="connsiteY1" fmla="*/ 333375 h 333375"/>
+            <a:gd name="connsiteX2" fmla="*/ 4314825 w 4638675"/>
+            <a:gd name="connsiteY2" fmla="*/ 333375 h 333375"/>
+            <a:gd name="connsiteX3" fmla="*/ 4638675 w 4638675"/>
+            <a:gd name="connsiteY3" fmla="*/ 57150 h 333375"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="4638675" h="333375">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="333375" y="333375"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="4314825" y="333375"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="4638675" y="57150"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -11134,8 +11527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C554509-BFFA-4011-8804-F6F5DE023F7A}">
   <dimension ref="B3:X127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+    <sheetView tabSelected="1" topLeftCell="O66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W75" sqref="W75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -11143,13 +11536,14 @@
     <col min="5" max="5" width="18.125" customWidth="1"/>
     <col min="6" max="6" width="27.5" customWidth="1"/>
     <col min="7" max="7" width="15.625" customWidth="1"/>
-    <col min="8" max="8" width="27" customWidth="1"/>
+    <col min="8" max="8" width="18.875" customWidth="1"/>
     <col min="9" max="9" width="4.5" customWidth="1"/>
     <col min="10" max="10" width="33.75" customWidth="1"/>
     <col min="11" max="11" width="3.5" customWidth="1"/>
-    <col min="12" max="12" width="29.75" customWidth="1"/>
+    <col min="12" max="12" width="33.875" customWidth="1"/>
     <col min="13" max="13" width="17.5" customWidth="1"/>
     <col min="14" max="14" width="27.5" customWidth="1"/>
+    <col min="15" max="15" width="22" customWidth="1"/>
     <col min="16" max="16" width="28.25" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
     <col min="18" max="18" width="28.25" customWidth="1"/>
@@ -11189,15 +11583,15 @@
     </row>
     <row r="8" spans="2:5">
       <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" t="s">
         <v>99</v>
-      </c>
-      <c r="D8" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="D9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -11217,93 +11611,89 @@
     </row>
     <row r="14" spans="2:5">
       <c r="B14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="2:5">
       <c r="D15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="D16" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="4:24">
-      <c r="F21" s="56" t="s">
-        <v>94</v>
-      </c>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="57"/>
-      <c r="N21" s="58"/>
-      <c r="P21" s="56" t="s">
+      <c r="F21" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="66"/>
+      <c r="J21" s="66"/>
+      <c r="K21" s="66"/>
+      <c r="L21" s="66"/>
+      <c r="M21" s="66"/>
+      <c r="N21" s="67"/>
+      <c r="P21" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="Q21" s="57"/>
-      <c r="R21" s="57"/>
-      <c r="S21" s="57"/>
-      <c r="T21" s="58"/>
-      <c r="V21" s="56" t="s">
+      <c r="Q21" s="66"/>
+      <c r="R21" s="66"/>
+      <c r="S21" s="66"/>
+      <c r="T21" s="67"/>
+      <c r="V21" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="W21" s="57"/>
-      <c r="X21" s="58"/>
+      <c r="W21" s="66"/>
+      <c r="X21" s="67"/>
     </row>
     <row r="23" spans="4:24">
       <c r="F23" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="H23" s="59" t="s">
-        <v>122</v>
-      </c>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="61"/>
+        <v>116</v>
+      </c>
+      <c r="J23" s="68" t="s">
+        <v>115</v>
+      </c>
+      <c r="K23" s="69"/>
+      <c r="L23" s="70"/>
       <c r="N23" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="P23" s="56" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q23" s="57"/>
-      <c r="R23" s="58"/>
+        <v>117</v>
+      </c>
+      <c r="P23" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q23" s="66"/>
+      <c r="R23" s="67"/>
       <c r="T23" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="V23" s="56" t="s">
-        <v>95</v>
-      </c>
-      <c r="W23" s="57"/>
-      <c r="X23" s="58"/>
+        <v>117</v>
+      </c>
+      <c r="V23" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="W23" s="66"/>
+      <c r="X23" s="67"/>
     </row>
     <row r="24" spans="4:24" ht="38.25" thickBot="1">
-      <c r="H24" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="L24" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="P24" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="R24" s="42" t="s">
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="L24" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="P24" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R24" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="V24" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="X24" s="42" t="s">
+      <c r="V24" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="X24" s="39" t="s">
         <v>92</v>
       </c>
     </row>
@@ -11317,323 +11707,305 @@
       <c r="F25" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="H25" s="51" t="s">
-        <v>101</v>
-      </c>
+      <c r="H25" s="6"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="49" t="s">
-        <v>133</v>
-      </c>
-      <c r="L25" s="49" t="s">
-        <v>133</v>
-      </c>
-      <c r="N25" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="P25" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="S25" s="3"/>
-      <c r="T25" s="51" t="s">
-        <v>102</v>
-      </c>
-      <c r="U25" s="3"/>
-      <c r="V25" s="51" t="s">
-        <v>102</v>
-      </c>
-      <c r="W25" s="3"/>
-      <c r="X25" s="51" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="4:24" ht="75">
+      <c r="J25" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="L25" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="N25" s="50" t="s">
+        <v>139</v>
+      </c>
+      <c r="P25" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="R25" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="T25" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="V25" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="X25" s="50" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="4:24" ht="93.75">
       <c r="D26" t="s">
         <v>86</v>
       </c>
       <c r="F26" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H26" s="38" t="s">
-        <v>88</v>
+      <c r="H26" s="62" t="s">
+        <v>150</v>
       </c>
       <c r="I26" s="2"/>
-      <c r="J26" s="52" t="s">
-        <v>129</v>
-      </c>
-      <c r="L26" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N26" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="P26" s="53" t="s">
+      <c r="J26" s="48" t="s">
         <v>143</v>
       </c>
+      <c r="L26" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="N26" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="P26" s="46" t="s">
+        <v>101</v>
+      </c>
       <c r="Q26" s="6"/>
-      <c r="R26" s="53" t="s">
-        <v>143</v>
+      <c r="R26" s="46" t="s">
+        <v>101</v>
       </c>
       <c r="S26" s="3"/>
-      <c r="T26" s="53" t="s">
-        <v>143</v>
+      <c r="T26" s="46" t="s">
+        <v>101</v>
       </c>
       <c r="U26" s="3"/>
-      <c r="V26" s="53" t="s">
-        <v>144</v>
+      <c r="V26" s="46" t="s">
+        <v>101</v>
       </c>
       <c r="W26" s="3"/>
-      <c r="X26" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="4:24" ht="112.5">
+      <c r="X26" s="46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="4:24" ht="150">
       <c r="D27" t="s">
         <v>86</v>
       </c>
       <c r="F27" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H27" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="J27" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="L27" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N27" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="P27" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="T27" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="V27" s="54" t="s">
-        <v>104</v>
-      </c>
-      <c r="X27" s="29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="4:24" ht="75">
+      <c r="H27" s="6"/>
+      <c r="J27" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="L27" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="N27" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="P27" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="S27" s="3"/>
+      <c r="T27" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="U27" s="3"/>
+      <c r="V27" s="64" t="s">
+        <v>153</v>
+      </c>
+      <c r="W27" s="3"/>
+      <c r="X27" s="64" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="4:24" ht="56.25">
       <c r="D28" t="s">
         <v>86</v>
       </c>
       <c r="F28" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H28" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="J28" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="L28" s="52" t="s">
-        <v>129</v>
-      </c>
-      <c r="N28" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="P28" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="R28" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="T28" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="V28" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="X28" s="29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="4:24" ht="37.5">
+      <c r="J28" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="L28" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N28" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="P28" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="S28" s="3"/>
+      <c r="T28" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="V28" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="W28" s="3"/>
+      <c r="X28" s="46" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="4:24" ht="93.75">
       <c r="D29" t="s">
         <v>86</v>
       </c>
       <c r="F29" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H29" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="J29" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="L29" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="N29" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="P29" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="R29" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="T29" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="V29" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="X29" s="40" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="4:24" ht="75">
+      <c r="J29" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="L29" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N29" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="P29" s="51" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="T29" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="V29" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="X29" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="4:24" ht="93.75">
       <c r="D30" t="s">
         <v>86</v>
       </c>
       <c r="F30" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H30" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="J30" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="L30" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="N30" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="P30" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="R30" s="52" t="s">
-        <v>108</v>
-      </c>
-      <c r="T30" s="44" t="s">
-        <v>145</v>
-      </c>
-      <c r="V30" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="X30" s="38" t="s">
+      <c r="J30" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="L30" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="N30" s="49" t="s">
+        <v>147</v>
+      </c>
+      <c r="P30" s="37" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="31" spans="4:24" ht="37.5">
+      <c r="R30" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="T30" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="V30" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="X30" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="4:24" ht="93.75">
       <c r="D31" t="s">
         <v>86</v>
       </c>
       <c r="F31" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H31" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="J31" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="L31" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="N31" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="P31" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="R31" s="38" t="s">
+      <c r="J31" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="L31" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="T31" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="V31" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="X31" s="35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="4:24">
+      <c r="N31" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="P31" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="R31" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="T31" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="V31" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="X31" s="48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="4:24" ht="93.75">
       <c r="D32" t="s">
         <v>86</v>
       </c>
       <c r="F32" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H32" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="J32" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="L32" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="N32" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="P32" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="R32" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="T32" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="V32" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="X32" s="35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="4:24">
+      <c r="J32" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="L32" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="N32" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="P32" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="R32" s="51" t="s">
+        <v>144</v>
+      </c>
+      <c r="T32" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="V32" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="X32" s="37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="4:24" ht="37.5">
       <c r="D33" t="s">
         <v>86</v>
       </c>
       <c r="F33" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="H33" s="36" t="s">
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="I33" s="43"/>
-      <c r="J33" s="36" t="s">
+      <c r="L33" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="L33" s="36" t="s">
+      <c r="N33" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="N33" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="P33" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="R33" s="35" t="s">
-        <v>82</v>
+      <c r="P33" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="R33" s="37" t="s">
+        <v>88</v>
       </c>
       <c r="T33" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="V33" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="X33" s="35" t="s">
+      <c r="V33" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="X33" s="34" t="s">
         <v>82</v>
       </c>
     </row>
@@ -11644,33 +12016,29 @@
       <c r="F34" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H34" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="J34" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="L34" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="N34" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="P34" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q34" s="43"/>
-      <c r="R34" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="T34" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="V34" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="X34" s="36" t="s">
-        <v>87</v>
+      <c r="J34" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="L34" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="N34" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="P34" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="R34" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="T34" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="V34" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="X34" s="34" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="4:24" ht="19.5" thickBot="1">
@@ -11680,133 +12048,149 @@
       <c r="F35" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="J35" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="L35" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="N35" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="P35" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="R35" s="35" t="s">
+      <c r="J35" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="L35" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="N35" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="P35" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="R35" s="34" t="s">
         <v>82</v>
       </c>
       <c r="T35" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="V35" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="X35" s="35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="4:24" ht="39" thickTop="1" thickBot="1">
+      <c r="V35" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="X35" s="34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="4:24" ht="38.25" thickTop="1">
       <c r="D36" t="s">
         <v>86</v>
       </c>
       <c r="F36" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="G36" s="41" t="s">
+      <c r="G36" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="H36" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="J36" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="K36" s="41"/>
-      <c r="L36" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="M36" s="41" t="s">
+      <c r="J36" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="K36" s="38"/>
+      <c r="L36" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="M36" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="N36" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="P36" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="R36" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="T36" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="V36" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="X36" s="37" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="4:24" ht="19.5" thickTop="1">
+      <c r="N36" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="P36" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q36" s="40"/>
+      <c r="R36" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="T36" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="V36" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="X36" s="35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="4:24">
       <c r="D37" t="s">
         <v>86</v>
       </c>
       <c r="F37" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H37" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J37" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L37" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N37" s="29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="4:24">
+      <c r="J37" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L37" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N37" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="P37" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="R37" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="T37" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="V37" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="X37" s="34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="4:24" ht="19.5" thickBot="1">
       <c r="D38" t="s">
         <v>86</v>
       </c>
       <c r="F38" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H38" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J38" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L38" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N38" s="29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="4:24">
+      <c r="J38" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L38" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N38" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="P38" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="R38" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="T38" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="V38" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="X38" s="36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="4:24" ht="19.5" thickTop="1">
       <c r="D39" t="s">
         <v>86</v>
       </c>
       <c r="F39" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H39" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J39" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L39" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N39" s="29" t="s">
+      <c r="J39" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L39" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N39" s="57" t="s">
         <v>82</v>
       </c>
     </row>
@@ -11817,16 +12201,13 @@
       <c r="F40" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H40" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J40" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L40" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N40" s="29" t="s">
+      <c r="J40" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L40" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N40" s="57" t="s">
         <v>82</v>
       </c>
     </row>
@@ -11837,16 +12218,13 @@
       <c r="F41" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H41" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J41" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L41" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N41" s="29" t="s">
+      <c r="J41" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L41" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N41" s="57" t="s">
         <v>82</v>
       </c>
     </row>
@@ -11857,16 +12235,13 @@
       <c r="F42" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H42" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J42" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L42" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N42" s="29" t="s">
+      <c r="J42" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L42" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N42" s="57" t="s">
         <v>82</v>
       </c>
     </row>
@@ -11877,16 +12252,13 @@
       <c r="F43" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H43" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J43" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L43" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N43" s="29" t="s">
+      <c r="J43" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L43" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N43" s="57" t="s">
         <v>82</v>
       </c>
     </row>
@@ -11897,17 +12269,15 @@
       <c r="F44" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="H44" s="32" t="s">
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="I44" s="43"/>
-      <c r="J44" s="32" t="s">
+      <c r="L44" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="L44" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="N44" s="32" t="s">
+      <c r="N44" s="58" t="s">
         <v>87</v>
       </c>
     </row>
@@ -11918,16 +12288,13 @@
       <c r="F45" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H45" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J45" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L45" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N45" s="29" t="s">
+      <c r="J45" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L45" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N45" s="57" t="s">
         <v>82</v>
       </c>
     </row>
@@ -11938,16 +12305,13 @@
       <c r="F46" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="H46" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="J46" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="L46" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="N46" s="30" t="s">
+      <c r="J46" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="L46" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="N46" s="59" t="s">
         <v>82</v>
       </c>
     </row>
@@ -11958,16 +12322,13 @@
       <c r="F47" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="H47" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="J47" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="L47" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="N47" s="28" t="s">
+      <c r="J47" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="L47" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="N47" s="56" t="s">
         <v>82</v>
       </c>
     </row>
@@ -11978,546 +12339,515 @@
       <c r="F48" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H48" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J48" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L48" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N48" s="29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="2:20">
+      <c r="J48" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L48" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N48" s="57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15">
       <c r="D49" t="s">
         <v>86</v>
       </c>
       <c r="F49" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H49" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J49" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L49" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N49" s="29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="2:20">
+      <c r="J49" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L49" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N49" s="57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15">
       <c r="D50" t="s">
         <v>86</v>
       </c>
       <c r="F50" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H50" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J50" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L50" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N50" s="29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="2:20">
+      <c r="J50" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L50" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N50" s="57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15">
       <c r="D51" t="s">
         <v>86</v>
       </c>
       <c r="F51" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H51" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J51" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L51" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N51" s="29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="2:20">
+      <c r="J51" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L51" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N51" s="57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15">
       <c r="D52" t="s">
         <v>86</v>
       </c>
       <c r="F52" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H52" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J52" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L52" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N52" s="29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="53" spans="2:20">
+      <c r="J52" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L52" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N52" s="57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15">
       <c r="D53" t="s">
         <v>86</v>
       </c>
       <c r="F53" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H53" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J53" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L53" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N53" s="29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="2:20">
+      <c r="J53" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L53" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N53" s="57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15">
       <c r="D54" t="s">
         <v>86</v>
       </c>
       <c r="F54" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H54" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J54" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L54" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N54" s="29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="55" spans="2:20">
+      <c r="J54" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L54" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N54" s="57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15">
       <c r="D55" t="s">
         <v>86</v>
       </c>
       <c r="F55" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="H55" s="32" t="s">
+      <c r="H55" s="40"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="I55" s="43"/>
-      <c r="J55" s="32" t="s">
+      <c r="L55" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="L55" s="32" t="s">
+      <c r="N55" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="N55" s="32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="56" spans="2:20">
+    </row>
+    <row r="56" spans="2:15">
       <c r="D56" t="s">
         <v>86</v>
       </c>
       <c r="F56" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H56" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J56" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="L56" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N56" s="29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="57" spans="2:20" ht="19.5" thickBot="1">
+      <c r="J56" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L56" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N56" s="57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" ht="19.5" thickBot="1">
       <c r="D57" t="s">
         <v>86</v>
       </c>
       <c r="F57" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="H57" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="J57" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="L57" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="N57" s="30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="58" spans="2:20" ht="19.5" thickTop="1"/>
-    <row r="61" spans="2:20">
+      <c r="J57" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="L57" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="N57" s="59" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15" ht="19.5" thickTop="1"/>
+    <row r="61" spans="2:15">
       <c r="B61" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="O61" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="62" spans="2:20">
-      <c r="F62" s="56" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="2:15">
+      <c r="F62" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="G62" s="57"/>
-      <c r="H62" s="57"/>
-      <c r="I62" s="57"/>
-      <c r="J62" s="57"/>
-      <c r="K62" s="57"/>
-      <c r="L62" s="58"/>
-    </row>
-    <row r="63" spans="2:20">
-      <c r="P63" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q63" s="57"/>
-      <c r="R63" s="57"/>
-      <c r="S63" s="57"/>
-      <c r="T63" s="58"/>
-    </row>
-    <row r="64" spans="2:20" ht="19.5" thickBot="1">
+      <c r="G62" s="66"/>
+      <c r="H62" s="66"/>
+      <c r="I62" s="66"/>
+      <c r="J62" s="66"/>
+      <c r="K62" s="66"/>
+      <c r="L62" s="67"/>
+    </row>
+    <row r="64" spans="2:15" ht="19.5" thickBot="1">
       <c r="F64" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="5:20" ht="19.5" thickTop="1">
       <c r="E65" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F65" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="P65" s="65" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q65" s="66"/>
+      <c r="R65" s="66"/>
+      <c r="S65" s="66"/>
+      <c r="T65" s="67"/>
+    </row>
+    <row r="66" spans="5:20" ht="37.5">
+      <c r="E66" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F66" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="O66" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="67" spans="5:20" ht="75">
+      <c r="E67" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F67" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="O67" s="1"/>
+    </row>
+    <row r="68" spans="5:20" ht="57" thickBot="1">
+      <c r="E68" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F68" s="33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="69" spans="5:20" ht="76.5" thickTop="1" thickBot="1">
+      <c r="E69" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F69" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="J69" t="s">
+        <v>105</v>
+      </c>
+      <c r="P69" s="45" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="66" spans="5:20" ht="38.25" thickBot="1">
-      <c r="E66" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F66" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="O66" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="67" spans="5:20" ht="76.5" thickTop="1" thickBot="1">
-      <c r="E67" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F67" s="33" t="s">
-        <v>151</v>
-      </c>
-      <c r="O67" s="1"/>
-      <c r="P67" s="50" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="68" spans="5:20" ht="57" thickTop="1">
-      <c r="E68" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F68" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="P68" s="2"/>
-    </row>
-    <row r="69" spans="5:20" ht="75.75" thickBot="1">
-      <c r="E69" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F69" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="J69" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="70" spans="5:20" ht="57.75" thickTop="1" thickBot="1">
       <c r="E70" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F70" s="46" t="s">
-        <v>120</v>
+        <v>109</v>
+      </c>
+      <c r="F70" s="42" t="s">
+        <v>113</v>
       </c>
       <c r="J70" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="T70" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="P70" s="2"/>
+    </row>
+    <row r="71" spans="5:20" ht="20.25" thickTop="1" thickBot="1">
+      <c r="J71" s="33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" spans="5:20" ht="20.25" thickTop="1" thickBot="1">
+      <c r="J72" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="T72" s="44" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="5:20" ht="19.5" thickTop="1">
-      <c r="J71" s="33" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="72" spans="5:20">
-      <c r="J72" s="33" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="73" spans="5:20" ht="37.5">
+    <row r="73" spans="5:20" ht="38.25" thickTop="1">
       <c r="J73" s="33" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="74" spans="5:20" ht="38.25" thickBot="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="5:20" ht="37.5">
       <c r="J74" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="75" spans="5:20" ht="39" thickTop="1" thickBot="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="5:20" ht="37.5">
       <c r="J75" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="T75" s="48" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="76" spans="5:20" ht="38.25" thickBot="1">
+      <c r="J76" s="33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="77" spans="5:20" ht="39" thickTop="1" thickBot="1">
+      <c r="J77" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="T77" s="44" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="5:20" ht="38.25" thickTop="1">
-      <c r="J76" s="33" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="77" spans="5:20" ht="37.5">
-      <c r="J77" s="33" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="78" spans="5:20">
-      <c r="J78" s="47" t="s">
-        <v>121</v>
+    <row r="78" spans="5:20" ht="19.5" thickTop="1">
+      <c r="J78" s="43" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="79" spans="5:20" ht="37.5">
       <c r="J79" s="33" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="80" spans="5:20">
       <c r="J80" s="33" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="81" spans="10:10">
       <c r="J81" s="33" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="82" spans="10:10">
-      <c r="J82" s="47" t="s">
-        <v>121</v>
+      <c r="J82" s="43" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="10:10" ht="19.5" thickBot="1">
-      <c r="J83" s="46" t="s">
-        <v>127</v>
+      <c r="J83" s="42" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="84" spans="10:10" ht="19.5" thickTop="1"/>
     <row r="86" spans="10:10" ht="19.5" thickBot="1"/>
     <row r="87" spans="10:10" ht="19.5" thickTop="1">
       <c r="J87" s="31" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="88" spans="10:10">
       <c r="J88" s="33" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="10:10">
       <c r="J89" s="33" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="90" spans="10:10" ht="37.5">
       <c r="J90" s="33" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="91" spans="10:10" ht="37.5">
       <c r="J91" s="33" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="10:10" ht="37.5">
       <c r="J92" s="33" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="93" spans="10:10" ht="37.5">
       <c r="J93" s="33" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="94" spans="10:10" ht="37.5">
       <c r="J94" s="33" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="95" spans="10:10">
-      <c r="J95" s="47" t="s">
-        <v>121</v>
+      <c r="J95" s="43" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="96" spans="10:10" ht="37.5">
       <c r="J96" s="33" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="97" spans="10:10">
       <c r="J97" s="33" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="98" spans="10:10">
       <c r="J98" s="33" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="99" spans="10:10">
-      <c r="J99" s="47" t="s">
-        <v>121</v>
+      <c r="J99" s="43" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="100" spans="10:10" ht="19.5" thickBot="1">
-      <c r="J100" s="46" t="s">
-        <v>127</v>
+      <c r="J100" s="42" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="101" spans="10:10" ht="19.5" thickTop="1"/>
     <row r="103" spans="10:10" ht="19.5" thickBot="1"/>
     <row r="104" spans="10:10" ht="19.5" thickTop="1">
       <c r="J104" s="31" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="105" spans="10:10">
       <c r="J105" s="33" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="106" spans="10:10">
       <c r="J106" s="33" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="107" spans="10:10" ht="37.5">
       <c r="J107" s="33" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="108" spans="10:10" ht="37.5">
       <c r="J108" s="33" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="109" spans="10:10" ht="37.5">
       <c r="J109" s="33" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="10:10" ht="37.5">
       <c r="J110" s="33" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="10:10" ht="37.5">
       <c r="J111" s="33" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="112" spans="10:10">
-      <c r="J112" s="47" t="s">
-        <v>121</v>
+      <c r="J112" s="43" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="113" spans="2:10" ht="37.5">
       <c r="J113" s="33" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="114" spans="2:10">
       <c r="J114" s="33" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="115" spans="2:10">
       <c r="J115" s="33" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="116" spans="2:10">
-      <c r="J116" s="47" t="s">
-        <v>121</v>
+      <c r="J116" s="43" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="2:10" ht="19.5" thickBot="1">
-      <c r="J117" s="46" t="s">
-        <v>127</v>
+      <c r="J117" s="42" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="118" spans="2:10" ht="19.5" thickTop="1"/>
     <row r="121" spans="2:10">
       <c r="B121" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="123" spans="2:10">
       <c r="E123" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F123" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="124" spans="2:10">
       <c r="E124" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F124" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="125" spans="2:10">
       <c r="F125" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="126" spans="2:10">
-      <c r="F126" s="43" t="s">
+      <c r="F126" s="40" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="127" spans="2:10">
       <c r="F127" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -12525,11 +12855,11 @@
     <mergeCell ref="V21:X21"/>
     <mergeCell ref="V23:X23"/>
     <mergeCell ref="F62:L62"/>
-    <mergeCell ref="P63:T63"/>
-    <mergeCell ref="H23:L23"/>
+    <mergeCell ref="P65:T65"/>
     <mergeCell ref="F21:N21"/>
     <mergeCell ref="P21:T21"/>
     <mergeCell ref="P23:R23"/>
+    <mergeCell ref="J23:L23"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: build erro with ALCONCURRENT_CONF_ENABLE_OD_NODE_PROFILE
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/Design_general_mem_alloc.xlsx
+++ b/libalconcurrent/doc/Design_general_mem_alloc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F911271-E4FA-421F-ABE3-8913D45A38F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECFE586-EE42-4197-B9AB-80CD0F76266B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="design overview" sheetId="4" r:id="rId1"/>
@@ -1203,7 +1203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1302,13 +1302,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1327,9 +1326,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -3516,13 +3515,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
+      <xdr:rowOff>200026</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>666750</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1123951</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3537,13 +3536,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8848725" y="6162675"/>
-          <a:ext cx="266700" cy="3810000"/>
+          <a:off x="8848725" y="6162676"/>
+          <a:ext cx="266700" cy="2362200"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
             <a:gd name="adj1" fmla="val 61905"/>
-            <a:gd name="adj2" fmla="val 57750"/>
+            <a:gd name="adj2" fmla="val 61783"/>
           </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
@@ -3628,15 +3627,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>2076450</xdr:colOff>
+      <xdr:colOff>2105025</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>1066800</xdr:rowOff>
+      <xdr:rowOff>1047750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1295400</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>1400175</xdr:rowOff>
+      <xdr:colOff>1323975</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3651,8 +3650,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11268075" y="8467725"/>
-          <a:ext cx="4638675" cy="333375"/>
+          <a:off x="11296650" y="8448675"/>
+          <a:ext cx="4638675" cy="238125"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3996,8 +3995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C554509-BFFA-4011-8804-F6F5DE023F7A}">
   <dimension ref="B3:X127"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -4094,55 +4093,55 @@
       </c>
     </row>
     <row r="21" spans="4:24">
-      <c r="F21" s="43" t="s">
+      <c r="F21" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="45"/>
-      <c r="P21" s="43" t="s">
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="46"/>
+      <c r="P21" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="Q21" s="44"/>
-      <c r="R21" s="44"/>
-      <c r="S21" s="44"/>
-      <c r="T21" s="45"/>
-      <c r="V21" s="43" t="s">
+      <c r="Q21" s="45"/>
+      <c r="R21" s="45"/>
+      <c r="S21" s="45"/>
+      <c r="T21" s="46"/>
+      <c r="V21" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="W21" s="44"/>
-      <c r="X21" s="45"/>
+      <c r="W21" s="45"/>
+      <c r="X21" s="46"/>
     </row>
     <row r="23" spans="4:24">
       <c r="F23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J23" s="46" t="s">
+      <c r="J23" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="K23" s="47"/>
-      <c r="L23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="49"/>
       <c r="N23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P23" s="43" t="s">
+      <c r="P23" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="44"/>
-      <c r="R23" s="45"/>
+      <c r="Q23" s="45"/>
+      <c r="R23" s="46"/>
       <c r="T23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="V23" s="43" t="s">
+      <c r="V23" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="W23" s="44"/>
-      <c r="X23" s="45"/>
+      <c r="W23" s="45"/>
+      <c r="X23" s="46"/>
     </row>
     <row r="24" spans="4:24" ht="38.25" thickBot="1">
       <c r="H24" s="17"/>
@@ -4210,7 +4209,7 @@
       <c r="F26" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="40" t="s">
+      <c r="H26" s="50" t="s">
         <v>75</v>
       </c>
       <c r="I26" s="2"/>
@@ -4272,11 +4271,11 @@
         <v>64</v>
       </c>
       <c r="U27" s="3"/>
-      <c r="V27" s="42" t="s">
+      <c r="V27" s="41" t="s">
         <v>78</v>
       </c>
       <c r="W27" s="3"/>
-      <c r="X27" s="42" t="s">
+      <c r="X27" s="41" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4367,7 +4366,7 @@
       <c r="P30" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="R30" s="41" t="s">
+      <c r="R30" s="40" t="s">
         <v>7</v>
       </c>
       <c r="T30" s="24" t="s">
@@ -4983,15 +4982,15 @@
       </c>
     </row>
     <row r="62" spans="2:15">
-      <c r="F62" s="43" t="s">
+      <c r="F62" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="G62" s="44"/>
-      <c r="H62" s="44"/>
-      <c r="I62" s="44"/>
-      <c r="J62" s="44"/>
-      <c r="K62" s="44"/>
-      <c r="L62" s="45"/>
+      <c r="G62" s="45"/>
+      <c r="H62" s="45"/>
+      <c r="I62" s="45"/>
+      <c r="J62" s="45"/>
+      <c r="K62" s="45"/>
+      <c r="L62" s="46"/>
     </row>
     <row r="64" spans="2:15" ht="19.5" thickBot="1">
       <c r="F64" t="s">
@@ -5005,13 +5004,13 @@
       <c r="F65" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="P65" s="43" t="s">
+      <c r="P65" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="Q65" s="44"/>
-      <c r="R65" s="44"/>
-      <c r="S65" s="44"/>
-      <c r="T65" s="45"/>
+      <c r="Q65" s="45"/>
+      <c r="R65" s="45"/>
+      <c r="S65" s="45"/>
+      <c r="T65" s="46"/>
     </row>
     <row r="66" spans="5:20" ht="37.5">
       <c r="E66" s="1" t="s">
@@ -5340,7 +5339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100EA77E-CB2D-494F-9C3C-65FD81893582}">
   <dimension ref="A5:W133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I133" sqref="I6:I133"/>
     </sheetView>
   </sheetViews>
@@ -9486,3693 +9485,3378 @@
       </c>
     </row>
     <row r="70" spans="1:23">
-      <c r="A70" s="49">
+      <c r="A70" s="42">
         <v>64</v>
       </c>
-      <c r="B70" s="49">
+      <c r="B70" s="42">
         <v>64</v>
       </c>
-      <c r="C70" s="49"/>
-      <c r="D70" s="49"/>
-      <c r="E70" s="49">
+      <c r="C70" s="42"/>
+      <c r="D70" s="42"/>
+      <c r="E70" s="42">
         <f t="shared" si="10"/>
         <v>576</v>
       </c>
-      <c r="F70" s="49">
+      <c r="F70" s="42">
         <f t="shared" ref="F70:F101" si="15">IF(E70*64 &gt; 65536, INT((E70*64+4096)/4096)*4096,65536)</f>
         <v>65536</v>
       </c>
-      <c r="G70" s="49">
+      <c r="G70" s="42">
         <f>1024*1024*2</f>
         <v>2097152</v>
       </c>
-      <c r="H70" s="49"/>
-      <c r="I70" s="49" t="str">
+      <c r="H70" s="42"/>
+      <c r="I70" s="42" t="str">
         <f t="shared" si="3"/>
         <v>{576,65536,2097152,64},</v>
       </c>
-      <c r="J70" s="49"/>
+      <c r="J70" s="42"/>
       <c r="K70">
         <f t="shared" ref="K70:K132" si="16">E70/1024</f>
         <v>0.5625</v>
       </c>
-      <c r="L70" s="49"/>
-      <c r="M70" s="49">
+      <c r="L70" s="42"/>
+      <c r="M70" s="42">
         <f t="shared" ref="M70:M133" si="17">E70-1</f>
         <v>575</v>
       </c>
-      <c r="N70" s="49">
+      <c r="N70" s="42">
         <f t="shared" ref="N70:N133" si="18">E70</f>
         <v>576</v>
       </c>
-      <c r="O70" s="49">
+      <c r="O70" s="42">
         <f t="shared" ref="O70:O133" si="19">E70+1</f>
         <v>577</v>
       </c>
-      <c r="P70" s="49"/>
-      <c r="Q70" s="49">
+      <c r="P70" s="42"/>
+      <c r="Q70" s="42">
         <f>INT((M70-512-1)/64)+64</f>
         <v>64</v>
       </c>
-      <c r="R70" s="49">
+      <c r="R70" s="42">
         <f t="shared" ref="R70:S70" si="20">INT((N70-512-1)/64)+64</f>
         <v>64</v>
       </c>
-      <c r="S70" s="49">
+      <c r="S70" s="42">
         <f t="shared" si="20"/>
         <v>65</v>
       </c>
-      <c r="T70" s="49"/>
-      <c r="U70" s="49" t="str">
+      <c r="T70" s="42"/>
+      <c r="U70" s="42" t="str">
         <f t="shared" ref="U70:U133" si="21">IF(Q70=$A70,"OK","NG")</f>
         <v>OK</v>
       </c>
-      <c r="V70" s="49" t="str">
+      <c r="V70" s="42" t="str">
         <f t="shared" ref="V70:V133" si="22">IF(R70=$A70,"OK","NG")</f>
         <v>OK</v>
       </c>
-      <c r="W70" s="49" t="str">
+      <c r="W70" s="42" t="str">
         <f t="shared" ref="W70:W133" si="23">IF(S70=($A70+1),"OK","NG")</f>
         <v>OK</v>
       </c>
     </row>
     <row r="71" spans="1:23">
-      <c r="A71" s="50">
+      <c r="A71">
         <v>65</v>
       </c>
-      <c r="B71" s="50">
+      <c r="B71">
         <v>64</v>
       </c>
-      <c r="C71" s="50"/>
-      <c r="D71" s="50"/>
-      <c r="E71" s="50">
+      <c r="E71">
         <f t="shared" si="10"/>
         <v>640</v>
       </c>
-      <c r="F71" s="50">
+      <c r="F71">
         <f t="shared" si="15"/>
         <v>65536</v>
       </c>
-      <c r="G71" s="50">
+      <c r="G71">
         <f t="shared" ref="G71:G76" si="24">1024*1024*2</f>
         <v>2097152</v>
       </c>
-      <c r="H71" s="50"/>
-      <c r="I71" s="50" t="str">
+      <c r="I71" t="str">
         <f t="shared" ref="I71:I133" si="25">"{"&amp; E71 &amp; ","&amp; F71 &amp; ","&amp; G71 &amp; ","&amp; A71 &amp; "},"</f>
         <v>{640,65536,2097152,65},</v>
       </c>
-      <c r="J71" s="50"/>
       <c r="K71">
         <f t="shared" si="16"/>
         <v>0.625</v>
       </c>
-      <c r="L71" s="50"/>
-      <c r="M71" s="50">
+      <c r="M71">
         <f t="shared" si="17"/>
         <v>639</v>
       </c>
-      <c r="N71" s="50">
+      <c r="N71">
         <f t="shared" si="18"/>
         <v>640</v>
       </c>
-      <c r="O71" s="50">
+      <c r="O71">
         <f t="shared" si="19"/>
         <v>641</v>
       </c>
-      <c r="P71" s="50"/>
-      <c r="Q71" s="50">
-        <f t="shared" ref="Q71:Q94" si="26">INT((M71-512-1)/64)+64</f>
+      <c r="Q71">
+        <f t="shared" ref="Q71:Q93" si="26">INT((M71-512-1)/64)+64</f>
         <v>65</v>
       </c>
-      <c r="R71" s="50">
+      <c r="R71">
         <f t="shared" ref="R71:R93" si="27">INT((N71-512-1)/64)+64</f>
         <v>65</v>
       </c>
-      <c r="S71" s="50">
+      <c r="S71">
         <f t="shared" ref="S71:S93" si="28">INT((O71-512-1)/64)+64</f>
         <v>66</v>
       </c>
-      <c r="T71" s="50"/>
-      <c r="U71" s="50" t="str">
+      <c r="U71" t="str">
         <f t="shared" si="21"/>
         <v>OK</v>
       </c>
-      <c r="V71" s="50" t="str">
+      <c r="V71" t="str">
         <f t="shared" si="22"/>
         <v>OK</v>
       </c>
-      <c r="W71" s="50" t="str">
+      <c r="W71" t="str">
         <f t="shared" si="23"/>
         <v>OK</v>
       </c>
     </row>
     <row r="72" spans="1:23">
-      <c r="A72" s="50">
+      <c r="A72">
         <v>66</v>
       </c>
-      <c r="B72" s="50">
+      <c r="B72">
         <v>64</v>
       </c>
-      <c r="C72" s="50"/>
-      <c r="D72" s="50"/>
-      <c r="E72" s="50">
+      <c r="E72">
         <f t="shared" ref="E72:E133" si="29">E71+B72</f>
         <v>704</v>
       </c>
-      <c r="F72" s="50">
+      <c r="F72">
         <f t="shared" si="15"/>
         <v>65536</v>
       </c>
-      <c r="G72" s="50">
+      <c r="G72">
         <f t="shared" si="24"/>
         <v>2097152</v>
       </c>
-      <c r="H72" s="50"/>
-      <c r="I72" s="50" t="str">
+      <c r="I72" t="str">
         <f t="shared" si="25"/>
         <v>{704,65536,2097152,66},</v>
       </c>
-      <c r="J72" s="50"/>
       <c r="K72">
         <f t="shared" si="16"/>
         <v>0.6875</v>
       </c>
-      <c r="L72" s="50"/>
-      <c r="M72" s="50">
+      <c r="M72">
         <f t="shared" si="17"/>
         <v>703</v>
       </c>
-      <c r="N72" s="50">
+      <c r="N72">
         <f t="shared" si="18"/>
         <v>704</v>
       </c>
-      <c r="O72" s="50">
+      <c r="O72">
         <f t="shared" si="19"/>
         <v>705</v>
       </c>
-      <c r="P72" s="50"/>
-      <c r="Q72" s="50">
+      <c r="Q72">
         <f t="shared" si="26"/>
         <v>66</v>
       </c>
-      <c r="R72" s="50">
+      <c r="R72">
         <f t="shared" si="27"/>
         <v>66</v>
       </c>
-      <c r="S72" s="50">
+      <c r="S72">
         <f t="shared" si="28"/>
         <v>67</v>
       </c>
-      <c r="T72" s="50"/>
-      <c r="U72" s="50" t="str">
+      <c r="U72" t="str">
         <f t="shared" si="21"/>
         <v>OK</v>
       </c>
-      <c r="V72" s="50" t="str">
+      <c r="V72" t="str">
         <f t="shared" si="22"/>
         <v>OK</v>
       </c>
-      <c r="W72" s="50" t="str">
+      <c r="W72" t="str">
         <f t="shared" si="23"/>
         <v>OK</v>
       </c>
     </row>
     <row r="73" spans="1:23">
-      <c r="A73" s="50">
+      <c r="A73">
         <v>67</v>
       </c>
-      <c r="B73" s="50">
+      <c r="B73">
         <v>64</v>
       </c>
-      <c r="C73" s="50"/>
-      <c r="D73" s="50"/>
-      <c r="E73" s="50">
+      <c r="E73">
         <f t="shared" si="29"/>
         <v>768</v>
       </c>
-      <c r="F73" s="50">
+      <c r="F73">
         <f t="shared" si="15"/>
         <v>65536</v>
       </c>
-      <c r="G73" s="50">
+      <c r="G73">
         <f t="shared" si="24"/>
         <v>2097152</v>
       </c>
-      <c r="H73" s="50"/>
-      <c r="I73" s="50" t="str">
+      <c r="I73" t="str">
         <f t="shared" si="25"/>
         <v>{768,65536,2097152,67},</v>
       </c>
-      <c r="J73" s="50"/>
       <c r="K73">
         <f t="shared" si="16"/>
         <v>0.75</v>
       </c>
-      <c r="L73" s="50"/>
-      <c r="M73" s="50">
+      <c r="M73">
         <f t="shared" si="17"/>
         <v>767</v>
       </c>
-      <c r="N73" s="50">
+      <c r="N73">
         <f t="shared" si="18"/>
         <v>768</v>
       </c>
-      <c r="O73" s="50">
+      <c r="O73">
         <f t="shared" si="19"/>
         <v>769</v>
       </c>
-      <c r="P73" s="50"/>
-      <c r="Q73" s="50">
+      <c r="Q73">
         <f t="shared" si="26"/>
         <v>67</v>
       </c>
-      <c r="R73" s="50">
+      <c r="R73">
         <f t="shared" si="27"/>
         <v>67</v>
       </c>
-      <c r="S73" s="50">
+      <c r="S73">
         <f t="shared" si="28"/>
         <v>68</v>
       </c>
-      <c r="T73" s="50"/>
-      <c r="U73" s="50" t="str">
+      <c r="U73" t="str">
         <f t="shared" si="21"/>
         <v>OK</v>
       </c>
-      <c r="V73" s="50" t="str">
+      <c r="V73" t="str">
         <f t="shared" si="22"/>
         <v>OK</v>
       </c>
-      <c r="W73" s="50" t="str">
+      <c r="W73" t="str">
         <f t="shared" si="23"/>
         <v>OK</v>
       </c>
     </row>
     <row r="74" spans="1:23">
-      <c r="A74" s="50">
+      <c r="A74">
         <v>68</v>
       </c>
-      <c r="B74" s="50">
+      <c r="B74">
         <v>64</v>
       </c>
-      <c r="C74" s="50"/>
-      <c r="D74" s="50"/>
-      <c r="E74" s="50">
+      <c r="E74">
         <f t="shared" si="29"/>
         <v>832</v>
       </c>
-      <c r="F74" s="50">
+      <c r="F74">
         <f t="shared" si="15"/>
         <v>65536</v>
       </c>
-      <c r="G74" s="50">
+      <c r="G74">
         <f t="shared" si="24"/>
         <v>2097152</v>
       </c>
-      <c r="H74" s="50"/>
-      <c r="I74" s="50" t="str">
+      <c r="I74" t="str">
         <f t="shared" si="25"/>
         <v>{832,65536,2097152,68},</v>
       </c>
-      <c r="J74" s="50"/>
       <c r="K74">
         <f t="shared" si="16"/>
         <v>0.8125</v>
       </c>
-      <c r="L74" s="50"/>
-      <c r="M74" s="50">
+      <c r="M74">
         <f t="shared" si="17"/>
         <v>831</v>
       </c>
-      <c r="N74" s="50">
+      <c r="N74">
         <f t="shared" si="18"/>
         <v>832</v>
       </c>
-      <c r="O74" s="50">
+      <c r="O74">
         <f t="shared" si="19"/>
         <v>833</v>
       </c>
-      <c r="P74" s="50"/>
-      <c r="Q74" s="50">
+      <c r="Q74">
         <f t="shared" si="26"/>
         <v>68</v>
       </c>
-      <c r="R74" s="50">
+      <c r="R74">
         <f t="shared" si="27"/>
         <v>68</v>
       </c>
-      <c r="S74" s="50">
+      <c r="S74">
         <f t="shared" si="28"/>
         <v>69</v>
       </c>
-      <c r="T74" s="50"/>
-      <c r="U74" s="50" t="str">
+      <c r="U74" t="str">
         <f t="shared" si="21"/>
         <v>OK</v>
       </c>
-      <c r="V74" s="50" t="str">
+      <c r="V74" t="str">
         <f t="shared" si="22"/>
         <v>OK</v>
       </c>
-      <c r="W74" s="50" t="str">
+      <c r="W74" t="str">
         <f t="shared" si="23"/>
         <v>OK</v>
       </c>
     </row>
     <row r="75" spans="1:23">
-      <c r="A75" s="50">
+      <c r="A75">
         <v>69</v>
       </c>
-      <c r="B75" s="50">
+      <c r="B75">
         <v>64</v>
       </c>
-      <c r="C75" s="50"/>
-      <c r="D75" s="50"/>
-      <c r="E75" s="50">
+      <c r="E75">
         <f t="shared" si="29"/>
         <v>896</v>
       </c>
-      <c r="F75" s="50">
+      <c r="F75">
         <f t="shared" si="15"/>
         <v>65536</v>
       </c>
-      <c r="G75" s="50">
+      <c r="G75">
         <f t="shared" si="24"/>
         <v>2097152</v>
       </c>
-      <c r="H75" s="50"/>
-      <c r="I75" s="50" t="str">
+      <c r="I75" t="str">
         <f t="shared" si="25"/>
         <v>{896,65536,2097152,69},</v>
       </c>
-      <c r="J75" s="50"/>
       <c r="K75">
         <f t="shared" si="16"/>
         <v>0.875</v>
       </c>
-      <c r="L75" s="50"/>
-      <c r="M75" s="50">
+      <c r="M75">
         <f t="shared" si="17"/>
         <v>895</v>
       </c>
-      <c r="N75" s="50">
+      <c r="N75">
         <f t="shared" si="18"/>
         <v>896</v>
       </c>
-      <c r="O75" s="50">
+      <c r="O75">
         <f t="shared" si="19"/>
         <v>897</v>
       </c>
-      <c r="P75" s="50"/>
-      <c r="Q75" s="50">
+      <c r="Q75">
         <f t="shared" si="26"/>
         <v>69</v>
       </c>
-      <c r="R75" s="50">
+      <c r="R75">
         <f t="shared" si="27"/>
         <v>69</v>
       </c>
-      <c r="S75" s="50">
+      <c r="S75">
         <f t="shared" si="28"/>
         <v>70</v>
       </c>
-      <c r="T75" s="50"/>
-      <c r="U75" s="50" t="str">
+      <c r="U75" t="str">
         <f t="shared" si="21"/>
         <v>OK</v>
       </c>
-      <c r="V75" s="50" t="str">
+      <c r="V75" t="str">
         <f t="shared" si="22"/>
         <v>OK</v>
       </c>
-      <c r="W75" s="50" t="str">
+      <c r="W75" t="str">
         <f t="shared" si="23"/>
         <v>OK</v>
       </c>
     </row>
     <row r="76" spans="1:23">
-      <c r="A76" s="50">
+      <c r="A76">
         <v>70</v>
       </c>
-      <c r="B76" s="50">
+      <c r="B76">
         <v>64</v>
       </c>
-      <c r="C76" s="50"/>
-      <c r="D76" s="50"/>
-      <c r="E76" s="50">
+      <c r="E76">
         <f t="shared" si="29"/>
         <v>960</v>
       </c>
-      <c r="F76" s="50">
+      <c r="F76">
         <f t="shared" si="15"/>
         <v>65536</v>
       </c>
-      <c r="G76" s="50">
+      <c r="G76">
         <f t="shared" si="24"/>
         <v>2097152</v>
       </c>
-      <c r="H76" s="50"/>
-      <c r="I76" s="50" t="str">
+      <c r="I76" t="str">
         <f t="shared" si="25"/>
         <v>{960,65536,2097152,70},</v>
       </c>
-      <c r="J76" s="50"/>
       <c r="K76">
         <f t="shared" si="16"/>
         <v>0.9375</v>
       </c>
-      <c r="L76" s="50"/>
-      <c r="M76" s="50">
+      <c r="M76">
         <f t="shared" si="17"/>
         <v>959</v>
       </c>
-      <c r="N76" s="50">
+      <c r="N76">
         <f t="shared" si="18"/>
         <v>960</v>
       </c>
-      <c r="O76" s="50">
+      <c r="O76">
         <f t="shared" si="19"/>
         <v>961</v>
       </c>
-      <c r="P76" s="50"/>
-      <c r="Q76" s="50">
+      <c r="Q76">
         <f t="shared" si="26"/>
         <v>70</v>
       </c>
-      <c r="R76" s="50">
+      <c r="R76">
         <f t="shared" si="27"/>
         <v>70</v>
       </c>
-      <c r="S76" s="50">
+      <c r="S76">
         <f t="shared" si="28"/>
         <v>71</v>
       </c>
-      <c r="T76" s="50"/>
-      <c r="U76" s="50" t="str">
+      <c r="U76" t="str">
         <f t="shared" si="21"/>
         <v>OK</v>
       </c>
-      <c r="V76" s="50" t="str">
+      <c r="V76" t="str">
         <f t="shared" si="22"/>
         <v>OK</v>
       </c>
-      <c r="W76" s="50" t="str">
+      <c r="W76" t="str">
         <f t="shared" si="23"/>
         <v>OK</v>
       </c>
     </row>
     <row r="77" spans="1:23">
-      <c r="A77" s="50">
+      <c r="A77">
         <v>71</v>
       </c>
-      <c r="B77" s="50">
+      <c r="B77">
         <v>64</v>
       </c>
-      <c r="C77" s="50"/>
-      <c r="D77" s="50"/>
-      <c r="E77" s="50">
+      <c r="E77">
         <f t="shared" si="29"/>
         <v>1024</v>
       </c>
-      <c r="F77" s="50">
+      <c r="F77">
         <f t="shared" si="15"/>
         <v>65536</v>
       </c>
-      <c r="G77" s="50">
+      <c r="G77">
         <f>1024*1024*4</f>
         <v>4194304</v>
       </c>
-      <c r="H77" s="50"/>
-      <c r="I77" s="50" t="str">
+      <c r="I77" t="str">
         <f t="shared" si="25"/>
         <v>{1024,65536,4194304,71},</v>
       </c>
-      <c r="J77" s="50"/>
       <c r="K77">
         <f t="shared" si="16"/>
         <v>1</v>
       </c>
-      <c r="L77" s="50"/>
-      <c r="M77" s="50">
+      <c r="M77">
         <f t="shared" si="17"/>
         <v>1023</v>
       </c>
-      <c r="N77" s="50">
+      <c r="N77">
         <f t="shared" si="18"/>
         <v>1024</v>
       </c>
-      <c r="O77" s="50">
+      <c r="O77">
         <f t="shared" si="19"/>
         <v>1025</v>
       </c>
-      <c r="P77" s="50"/>
-      <c r="Q77" s="50">
+      <c r="Q77">
         <f t="shared" si="26"/>
         <v>71</v>
       </c>
-      <c r="R77" s="50">
+      <c r="R77">
         <f t="shared" si="27"/>
         <v>71</v>
       </c>
-      <c r="S77" s="50">
+      <c r="S77">
         <f t="shared" si="28"/>
         <v>72</v>
       </c>
-      <c r="T77" s="50"/>
-      <c r="U77" s="50" t="str">
+      <c r="U77" t="str">
         <f t="shared" si="21"/>
         <v>OK</v>
       </c>
-      <c r="V77" s="50" t="str">
+      <c r="V77" t="str">
         <f t="shared" si="22"/>
         <v>OK</v>
       </c>
-      <c r="W77" s="50" t="str">
+      <c r="W77" t="str">
         <f t="shared" si="23"/>
         <v>OK</v>
       </c>
     </row>
     <row r="78" spans="1:23">
-      <c r="A78" s="50">
+      <c r="A78">
         <v>72</v>
       </c>
-      <c r="B78" s="50">
+      <c r="B78">
         <v>128</v>
       </c>
-      <c r="C78" s="50"/>
-      <c r="D78" s="50"/>
-      <c r="E78" s="50">
+      <c r="E78">
         <f t="shared" si="29"/>
         <v>1152</v>
       </c>
-      <c r="F78" s="50">
+      <c r="F78">
         <f t="shared" si="15"/>
         <v>77824</v>
       </c>
-      <c r="G78" s="50">
+      <c r="G78">
         <f t="shared" ref="G78:G133" si="30">1024*1024*4</f>
         <v>4194304</v>
       </c>
-      <c r="H78" s="50"/>
-      <c r="I78" s="50" t="str">
+      <c r="I78" t="str">
         <f t="shared" si="25"/>
         <v>{1152,77824,4194304,72},</v>
       </c>
-      <c r="J78" s="50"/>
       <c r="K78">
         <f t="shared" si="16"/>
         <v>1.125</v>
       </c>
-      <c r="L78" s="50"/>
-      <c r="M78" s="50">
+      <c r="M78">
         <f t="shared" si="17"/>
         <v>1151</v>
       </c>
-      <c r="N78" s="50">
+      <c r="N78">
         <f t="shared" si="18"/>
         <v>1152</v>
       </c>
-      <c r="O78" s="50">
+      <c r="O78">
         <f t="shared" si="19"/>
         <v>1153</v>
       </c>
-      <c r="P78" s="50"/>
-      <c r="Q78" s="50">
+      <c r="Q78">
         <f>INT((M78-1024-1)/128)+64+8</f>
         <v>72</v>
       </c>
-      <c r="R78" s="50">
+      <c r="R78">
         <f t="shared" ref="R78:S78" si="31">INT((N78-1024-1)/128)+64+8</f>
         <v>72</v>
       </c>
-      <c r="S78" s="50">
+      <c r="S78">
         <f t="shared" si="31"/>
         <v>73</v>
       </c>
-      <c r="T78" s="50"/>
-      <c r="U78" s="50" t="str">
+      <c r="U78" t="str">
         <f t="shared" si="21"/>
         <v>OK</v>
       </c>
-      <c r="V78" s="50" t="str">
+      <c r="V78" t="str">
         <f t="shared" si="22"/>
         <v>OK</v>
       </c>
-      <c r="W78" s="50" t="str">
+      <c r="W78" t="str">
         <f t="shared" si="23"/>
         <v>OK</v>
       </c>
     </row>
     <row r="79" spans="1:23">
-      <c r="A79" s="50">
+      <c r="A79">
         <v>73</v>
       </c>
-      <c r="B79" s="50">
+      <c r="B79">
         <v>128</v>
       </c>
-      <c r="C79" s="50"/>
-      <c r="D79" s="50"/>
-      <c r="E79" s="50">
+      <c r="E79">
         <f t="shared" si="29"/>
         <v>1280</v>
       </c>
-      <c r="F79" s="50">
+      <c r="F79">
         <f t="shared" si="15"/>
         <v>86016</v>
       </c>
-      <c r="G79" s="50">
+      <c r="G79">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H79" s="50"/>
-      <c r="I79" s="50" t="str">
+      <c r="I79" t="str">
         <f t="shared" si="25"/>
         <v>{1280,86016,4194304,73},</v>
       </c>
-      <c r="J79" s="50"/>
       <c r="K79">
         <f t="shared" si="16"/>
         <v>1.25</v>
       </c>
-      <c r="L79" s="50"/>
-      <c r="M79" s="50">
+      <c r="M79">
         <f t="shared" si="17"/>
         <v>1279</v>
       </c>
-      <c r="N79" s="50">
+      <c r="N79">
         <f t="shared" si="18"/>
         <v>1280</v>
       </c>
-      <c r="O79" s="50">
+      <c r="O79">
         <f t="shared" si="19"/>
         <v>1281</v>
       </c>
-      <c r="P79" s="50"/>
-      <c r="Q79" s="50">
+      <c r="Q79">
         <f t="shared" ref="Q79:Q85" si="32">INT((M79-1024-1)/128)+64+8</f>
         <v>73</v>
       </c>
-      <c r="R79" s="50">
+      <c r="R79">
         <f t="shared" ref="R79:R85" si="33">INT((N79-1024-1)/128)+64+8</f>
         <v>73</v>
       </c>
-      <c r="S79" s="50">
+      <c r="S79">
         <f t="shared" ref="S79:S85" si="34">INT((O79-1024-1)/128)+64+8</f>
         <v>74</v>
       </c>
-      <c r="T79" s="50"/>
-      <c r="U79" s="50" t="str">
+      <c r="U79" t="str">
         <f t="shared" si="21"/>
         <v>OK</v>
       </c>
-      <c r="V79" s="50" t="str">
+      <c r="V79" t="str">
         <f t="shared" si="22"/>
         <v>OK</v>
       </c>
-      <c r="W79" s="50" t="str">
+      <c r="W79" t="str">
         <f t="shared" si="23"/>
         <v>OK</v>
       </c>
     </row>
     <row r="80" spans="1:23">
-      <c r="A80" s="50">
+      <c r="A80">
         <v>74</v>
       </c>
-      <c r="B80" s="50">
+      <c r="B80">
         <v>128</v>
       </c>
-      <c r="C80" s="50"/>
-      <c r="D80" s="50"/>
-      <c r="E80" s="50">
+      <c r="E80">
         <f t="shared" si="29"/>
         <v>1408</v>
       </c>
-      <c r="F80" s="50">
+      <c r="F80">
         <f t="shared" si="15"/>
         <v>94208</v>
       </c>
-      <c r="G80" s="50">
+      <c r="G80">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H80" s="50"/>
-      <c r="I80" s="50" t="str">
+      <c r="I80" t="str">
         <f t="shared" si="25"/>
         <v>{1408,94208,4194304,74},</v>
       </c>
-      <c r="J80" s="50"/>
       <c r="K80">
         <f t="shared" si="16"/>
         <v>1.375</v>
       </c>
-      <c r="L80" s="50"/>
-      <c r="M80" s="50">
+      <c r="M80">
         <f t="shared" si="17"/>
         <v>1407</v>
       </c>
-      <c r="N80" s="50">
+      <c r="N80">
         <f t="shared" si="18"/>
         <v>1408</v>
       </c>
-      <c r="O80" s="50">
+      <c r="O80">
         <f t="shared" si="19"/>
         <v>1409</v>
       </c>
-      <c r="P80" s="50"/>
-      <c r="Q80" s="50">
+      <c r="Q80">
         <f t="shared" si="32"/>
         <v>74</v>
       </c>
-      <c r="R80" s="50">
+      <c r="R80">
         <f t="shared" si="33"/>
         <v>74</v>
       </c>
-      <c r="S80" s="50">
+      <c r="S80">
         <f t="shared" si="34"/>
         <v>75</v>
       </c>
-      <c r="T80" s="50"/>
-      <c r="U80" s="50" t="str">
+      <c r="U80" t="str">
         <f t="shared" si="21"/>
         <v>OK</v>
       </c>
-      <c r="V80" s="50" t="str">
+      <c r="V80" t="str">
         <f t="shared" si="22"/>
         <v>OK</v>
       </c>
-      <c r="W80" s="50" t="str">
+      <c r="W80" t="str">
         <f t="shared" si="23"/>
         <v>OK</v>
       </c>
     </row>
     <row r="81" spans="1:23">
-      <c r="A81" s="50">
+      <c r="A81">
         <v>75</v>
       </c>
-      <c r="B81" s="50">
+      <c r="B81">
         <v>128</v>
       </c>
-      <c r="C81" s="50"/>
-      <c r="D81" s="50"/>
-      <c r="E81" s="50">
+      <c r="E81">
         <f t="shared" si="29"/>
         <v>1536</v>
       </c>
-      <c r="F81" s="50">
+      <c r="F81">
         <f t="shared" si="15"/>
         <v>102400</v>
       </c>
-      <c r="G81" s="50">
+      <c r="G81">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H81" s="50"/>
-      <c r="I81" s="50" t="str">
+      <c r="I81" t="str">
         <f t="shared" si="25"/>
         <v>{1536,102400,4194304,75},</v>
       </c>
-      <c r="J81" s="50"/>
       <c r="K81">
         <f t="shared" si="16"/>
         <v>1.5</v>
       </c>
-      <c r="L81" s="50"/>
-      <c r="M81" s="50">
+      <c r="M81">
         <f t="shared" si="17"/>
         <v>1535</v>
       </c>
-      <c r="N81" s="50">
+      <c r="N81">
         <f t="shared" si="18"/>
         <v>1536</v>
       </c>
-      <c r="O81" s="50">
+      <c r="O81">
         <f t="shared" si="19"/>
         <v>1537</v>
       </c>
-      <c r="P81" s="50"/>
-      <c r="Q81" s="50">
+      <c r="Q81">
         <f t="shared" si="32"/>
         <v>75</v>
       </c>
-      <c r="R81" s="50">
+      <c r="R81">
         <f t="shared" si="33"/>
         <v>75</v>
       </c>
-      <c r="S81" s="50">
+      <c r="S81">
         <f t="shared" si="34"/>
         <v>76</v>
       </c>
-      <c r="T81" s="50"/>
-      <c r="U81" s="50" t="str">
+      <c r="U81" t="str">
         <f t="shared" si="21"/>
         <v>OK</v>
       </c>
-      <c r="V81" s="50" t="str">
+      <c r="V81" t="str">
         <f t="shared" si="22"/>
         <v>OK</v>
       </c>
-      <c r="W81" s="50" t="str">
+      <c r="W81" t="str">
         <f t="shared" si="23"/>
         <v>OK</v>
       </c>
     </row>
     <row r="82" spans="1:23">
-      <c r="A82" s="50">
+      <c r="A82">
         <v>76</v>
       </c>
-      <c r="B82" s="50">
+      <c r="B82">
         <v>128</v>
       </c>
-      <c r="C82" s="50"/>
-      <c r="D82" s="50"/>
-      <c r="E82" s="50">
+      <c r="E82">
         <f t="shared" si="29"/>
         <v>1664</v>
       </c>
-      <c r="F82" s="50">
+      <c r="F82">
         <f t="shared" si="15"/>
         <v>110592</v>
       </c>
-      <c r="G82" s="50">
+      <c r="G82">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H82" s="50"/>
-      <c r="I82" s="50" t="str">
+      <c r="I82" t="str">
         <f t="shared" si="25"/>
         <v>{1664,110592,4194304,76},</v>
       </c>
-      <c r="J82" s="50"/>
       <c r="K82">
         <f t="shared" si="16"/>
         <v>1.625</v>
       </c>
-      <c r="L82" s="50"/>
-      <c r="M82" s="50">
+      <c r="M82">
         <f t="shared" si="17"/>
         <v>1663</v>
       </c>
-      <c r="N82" s="50">
+      <c r="N82">
         <f t="shared" si="18"/>
         <v>1664</v>
       </c>
-      <c r="O82" s="50">
+      <c r="O82">
         <f t="shared" si="19"/>
         <v>1665</v>
       </c>
-      <c r="P82" s="50"/>
-      <c r="Q82" s="50">
+      <c r="Q82">
         <f t="shared" si="32"/>
         <v>76</v>
       </c>
-      <c r="R82" s="50">
+      <c r="R82">
         <f t="shared" si="33"/>
         <v>76</v>
       </c>
-      <c r="S82" s="50">
+      <c r="S82">
         <f t="shared" si="34"/>
         <v>77</v>
       </c>
-      <c r="T82" s="50"/>
-      <c r="U82" s="50" t="str">
+      <c r="U82" t="str">
         <f t="shared" si="21"/>
         <v>OK</v>
       </c>
-      <c r="V82" s="50" t="str">
+      <c r="V82" t="str">
         <f t="shared" si="22"/>
         <v>OK</v>
       </c>
-      <c r="W82" s="50" t="str">
+      <c r="W82" t="str">
         <f t="shared" si="23"/>
         <v>OK</v>
       </c>
     </row>
     <row r="83" spans="1:23">
-      <c r="A83" s="50">
+      <c r="A83">
         <v>77</v>
       </c>
-      <c r="B83" s="50">
+      <c r="B83">
         <v>128</v>
       </c>
-      <c r="C83" s="50"/>
-      <c r="D83" s="50"/>
-      <c r="E83" s="50">
+      <c r="E83">
         <f t="shared" si="29"/>
         <v>1792</v>
       </c>
-      <c r="F83" s="50">
+      <c r="F83">
         <f t="shared" si="15"/>
         <v>118784</v>
       </c>
-      <c r="G83" s="50">
+      <c r="G83">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H83" s="50"/>
-      <c r="I83" s="50" t="str">
+      <c r="I83" t="str">
         <f t="shared" si="25"/>
         <v>{1792,118784,4194304,77},</v>
       </c>
-      <c r="J83" s="50"/>
       <c r="K83">
         <f t="shared" si="16"/>
         <v>1.75</v>
       </c>
-      <c r="L83" s="50"/>
-      <c r="M83" s="50">
+      <c r="M83">
         <f t="shared" si="17"/>
         <v>1791</v>
       </c>
-      <c r="N83" s="50">
+      <c r="N83">
         <f t="shared" si="18"/>
         <v>1792</v>
       </c>
-      <c r="O83" s="50">
+      <c r="O83">
         <f t="shared" si="19"/>
         <v>1793</v>
       </c>
-      <c r="P83" s="50"/>
-      <c r="Q83" s="50">
+      <c r="Q83">
         <f t="shared" si="32"/>
         <v>77</v>
       </c>
-      <c r="R83" s="50">
+      <c r="R83">
         <f t="shared" si="33"/>
         <v>77</v>
       </c>
-      <c r="S83" s="50">
+      <c r="S83">
         <f t="shared" si="34"/>
         <v>78</v>
       </c>
-      <c r="T83" s="50"/>
-      <c r="U83" s="50" t="str">
+      <c r="U83" t="str">
         <f t="shared" si="21"/>
         <v>OK</v>
       </c>
-      <c r="V83" s="50" t="str">
+      <c r="V83" t="str">
         <f t="shared" si="22"/>
         <v>OK</v>
       </c>
-      <c r="W83" s="50" t="str">
+      <c r="W83" t="str">
         <f t="shared" si="23"/>
         <v>OK</v>
       </c>
     </row>
     <row r="84" spans="1:23">
-      <c r="A84" s="50">
+      <c r="A84">
         <v>78</v>
       </c>
-      <c r="B84" s="50">
+      <c r="B84">
         <v>128</v>
       </c>
-      <c r="C84" s="50"/>
-      <c r="D84" s="50"/>
-      <c r="E84" s="50">
+      <c r="E84">
         <f t="shared" si="29"/>
         <v>1920</v>
       </c>
-      <c r="F84" s="50">
+      <c r="F84">
         <f t="shared" si="15"/>
         <v>126976</v>
       </c>
-      <c r="G84" s="50">
+      <c r="G84">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H84" s="50"/>
-      <c r="I84" s="50" t="str">
+      <c r="I84" t="str">
         <f t="shared" si="25"/>
         <v>{1920,126976,4194304,78},</v>
       </c>
-      <c r="J84" s="50"/>
       <c r="K84">
         <f t="shared" si="16"/>
         <v>1.875</v>
       </c>
-      <c r="L84" s="50"/>
-      <c r="M84" s="50">
+      <c r="M84">
         <f t="shared" si="17"/>
         <v>1919</v>
       </c>
-      <c r="N84" s="50">
+      <c r="N84">
         <f t="shared" si="18"/>
         <v>1920</v>
       </c>
-      <c r="O84" s="50">
+      <c r="O84">
         <f t="shared" si="19"/>
         <v>1921</v>
       </c>
-      <c r="P84" s="50"/>
-      <c r="Q84" s="50">
+      <c r="Q84">
         <f t="shared" si="32"/>
         <v>78</v>
       </c>
-      <c r="R84" s="50">
+      <c r="R84">
         <f t="shared" si="33"/>
         <v>78</v>
       </c>
-      <c r="S84" s="50">
+      <c r="S84">
         <f t="shared" si="34"/>
         <v>79</v>
       </c>
-      <c r="T84" s="50"/>
-      <c r="U84" s="50" t="str">
+      <c r="U84" t="str">
         <f t="shared" si="21"/>
         <v>OK</v>
       </c>
-      <c r="V84" s="50" t="str">
+      <c r="V84" t="str">
         <f t="shared" si="22"/>
         <v>OK</v>
       </c>
-      <c r="W84" s="50" t="str">
+      <c r="W84" t="str">
         <f t="shared" si="23"/>
         <v>OK</v>
       </c>
     </row>
     <row r="85" spans="1:23">
-      <c r="A85" s="50">
+      <c r="A85">
         <v>79</v>
       </c>
-      <c r="B85" s="50">
+      <c r="B85">
         <v>128</v>
       </c>
-      <c r="C85" s="50"/>
-      <c r="D85" s="50"/>
-      <c r="E85" s="50">
+      <c r="E85">
         <f t="shared" si="29"/>
         <v>2048</v>
       </c>
-      <c r="F85" s="50">
+      <c r="F85">
         <f t="shared" si="15"/>
         <v>135168</v>
       </c>
-      <c r="G85" s="50">
+      <c r="G85">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H85" s="50"/>
-      <c r="I85" s="50" t="str">
+      <c r="I85" t="str">
         <f t="shared" si="25"/>
         <v>{2048,135168,4194304,79},</v>
       </c>
-      <c r="J85" s="50"/>
       <c r="K85">
         <f t="shared" si="16"/>
         <v>2</v>
       </c>
-      <c r="L85" s="50"/>
-      <c r="M85" s="50">
+      <c r="M85">
         <f t="shared" si="17"/>
         <v>2047</v>
       </c>
-      <c r="N85" s="50">
+      <c r="N85">
         <f t="shared" si="18"/>
         <v>2048</v>
       </c>
-      <c r="O85" s="50">
+      <c r="O85">
         <f t="shared" si="19"/>
         <v>2049</v>
       </c>
-      <c r="P85" s="50"/>
-      <c r="Q85" s="50">
+      <c r="Q85">
         <f t="shared" si="32"/>
         <v>79</v>
       </c>
-      <c r="R85" s="50">
+      <c r="R85">
         <f t="shared" si="33"/>
         <v>79</v>
       </c>
-      <c r="S85" s="50">
+      <c r="S85">
         <f t="shared" si="34"/>
         <v>80</v>
       </c>
-      <c r="T85" s="50"/>
-      <c r="U85" s="50" t="str">
+      <c r="U85" t="str">
         <f t="shared" si="21"/>
         <v>OK</v>
       </c>
-      <c r="V85" s="50" t="str">
+      <c r="V85" t="str">
         <f t="shared" si="22"/>
         <v>OK</v>
       </c>
-      <c r="W85" s="50" t="str">
+      <c r="W85" t="str">
         <f t="shared" si="23"/>
         <v>OK</v>
       </c>
     </row>
     <row r="86" spans="1:23">
-      <c r="A86" s="50">
+      <c r="A86">
         <v>80</v>
       </c>
-      <c r="B86" s="50">
+      <c r="B86">
         <v>256</v>
       </c>
-      <c r="C86" s="50"/>
-      <c r="D86" s="50"/>
-      <c r="E86" s="50">
+      <c r="E86">
         <f t="shared" si="29"/>
         <v>2304</v>
       </c>
-      <c r="F86" s="50">
+      <c r="F86">
         <f t="shared" si="15"/>
         <v>151552</v>
       </c>
-      <c r="G86" s="50">
+      <c r="G86">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H86" s="50"/>
-      <c r="I86" s="50" t="str">
+      <c r="I86" t="str">
         <f t="shared" si="25"/>
         <v>{2304,151552,4194304,80},</v>
       </c>
-      <c r="J86" s="50"/>
       <c r="K86">
         <f t="shared" si="16"/>
         <v>2.25</v>
       </c>
-      <c r="L86" s="50"/>
-      <c r="M86" s="50">
+      <c r="M86">
         <f t="shared" si="17"/>
         <v>2303</v>
       </c>
-      <c r="N86" s="50">
+      <c r="N86">
         <f t="shared" si="18"/>
         <v>2304</v>
       </c>
-      <c r="O86" s="50">
+      <c r="O86">
         <f t="shared" si="19"/>
         <v>2305</v>
       </c>
-      <c r="P86" s="50"/>
-      <c r="Q86" s="50">
+      <c r="Q86">
         <f t="shared" si="26"/>
         <v>91</v>
       </c>
-      <c r="R86" s="50">
+      <c r="R86">
         <f t="shared" si="27"/>
         <v>91</v>
       </c>
-      <c r="S86" s="50">
+      <c r="S86">
         <f t="shared" si="28"/>
         <v>92</v>
       </c>
-      <c r="T86" s="50"/>
-      <c r="U86" s="50" t="str">
+      <c r="U86" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V86" s="50" t="str">
+      <c r="V86" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W86" s="50" t="str">
+      <c r="W86" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="87" spans="1:23">
-      <c r="A87" s="50">
+      <c r="A87">
         <v>81</v>
       </c>
-      <c r="B87" s="50">
+      <c r="B87">
         <v>256</v>
       </c>
-      <c r="C87" s="50"/>
-      <c r="D87" s="50"/>
-      <c r="E87" s="50">
+      <c r="E87">
         <f t="shared" si="29"/>
         <v>2560</v>
       </c>
-      <c r="F87" s="50">
+      <c r="F87">
         <f t="shared" si="15"/>
         <v>167936</v>
       </c>
-      <c r="G87" s="50">
+      <c r="G87">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H87" s="50"/>
-      <c r="I87" s="50" t="str">
+      <c r="I87" t="str">
         <f t="shared" si="25"/>
         <v>{2560,167936,4194304,81},</v>
       </c>
-      <c r="J87" s="50"/>
       <c r="K87">
         <f t="shared" si="16"/>
         <v>2.5</v>
       </c>
-      <c r="L87" s="50"/>
-      <c r="M87" s="50">
+      <c r="M87">
         <f t="shared" si="17"/>
         <v>2559</v>
       </c>
-      <c r="N87" s="50">
+      <c r="N87">
         <f t="shared" si="18"/>
         <v>2560</v>
       </c>
-      <c r="O87" s="50">
+      <c r="O87">
         <f t="shared" si="19"/>
         <v>2561</v>
       </c>
-      <c r="P87" s="50"/>
-      <c r="Q87" s="50">
+      <c r="Q87">
         <f t="shared" si="26"/>
         <v>95</v>
       </c>
-      <c r="R87" s="50">
+      <c r="R87">
         <f t="shared" si="27"/>
         <v>95</v>
       </c>
-      <c r="S87" s="50">
+      <c r="S87">
         <f t="shared" si="28"/>
         <v>96</v>
       </c>
-      <c r="T87" s="50"/>
-      <c r="U87" s="50" t="str">
+      <c r="U87" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V87" s="50" t="str">
+      <c r="V87" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W87" s="50" t="str">
+      <c r="W87" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="88" spans="1:23">
-      <c r="A88" s="50">
+      <c r="A88">
         <v>82</v>
       </c>
-      <c r="B88" s="50">
+      <c r="B88">
         <v>256</v>
       </c>
-      <c r="C88" s="50"/>
-      <c r="D88" s="50"/>
-      <c r="E88" s="50">
+      <c r="E88">
         <f t="shared" si="29"/>
         <v>2816</v>
       </c>
-      <c r="F88" s="50">
+      <c r="F88">
         <f t="shared" si="15"/>
         <v>184320</v>
       </c>
-      <c r="G88" s="50">
+      <c r="G88">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H88" s="50"/>
-      <c r="I88" s="50" t="str">
+      <c r="I88" t="str">
         <f t="shared" si="25"/>
         <v>{2816,184320,4194304,82},</v>
       </c>
-      <c r="J88" s="50"/>
       <c r="K88">
         <f t="shared" si="16"/>
         <v>2.75</v>
       </c>
-      <c r="L88" s="50"/>
-      <c r="M88" s="50">
+      <c r="M88">
         <f t="shared" si="17"/>
         <v>2815</v>
       </c>
-      <c r="N88" s="50">
+      <c r="N88">
         <f t="shared" si="18"/>
         <v>2816</v>
       </c>
-      <c r="O88" s="50">
+      <c r="O88">
         <f t="shared" si="19"/>
         <v>2817</v>
       </c>
-      <c r="P88" s="50"/>
-      <c r="Q88" s="50">
+      <c r="Q88">
         <f t="shared" si="26"/>
         <v>99</v>
       </c>
-      <c r="R88" s="50">
+      <c r="R88">
         <f t="shared" si="27"/>
         <v>99</v>
       </c>
-      <c r="S88" s="50">
+      <c r="S88">
         <f t="shared" si="28"/>
         <v>100</v>
       </c>
-      <c r="T88" s="50"/>
-      <c r="U88" s="50" t="str">
+      <c r="U88" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V88" s="50" t="str">
+      <c r="V88" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W88" s="50" t="str">
+      <c r="W88" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="89" spans="1:23">
-      <c r="A89" s="50">
+      <c r="A89">
         <v>83</v>
       </c>
-      <c r="B89" s="50">
+      <c r="B89">
         <v>256</v>
       </c>
-      <c r="C89" s="50"/>
-      <c r="D89" s="50"/>
-      <c r="E89" s="50">
+      <c r="E89">
         <f t="shared" si="29"/>
         <v>3072</v>
       </c>
-      <c r="F89" s="50">
+      <c r="F89">
         <f t="shared" si="15"/>
         <v>200704</v>
       </c>
-      <c r="G89" s="50">
+      <c r="G89">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H89" s="50"/>
-      <c r="I89" s="50" t="str">
+      <c r="I89" t="str">
         <f t="shared" si="25"/>
         <v>{3072,200704,4194304,83},</v>
       </c>
-      <c r="J89" s="50"/>
       <c r="K89">
         <f t="shared" si="16"/>
         <v>3</v>
       </c>
-      <c r="L89" s="50"/>
-      <c r="M89" s="50">
+      <c r="M89">
         <f t="shared" si="17"/>
         <v>3071</v>
       </c>
-      <c r="N89" s="50">
+      <c r="N89">
         <f t="shared" si="18"/>
         <v>3072</v>
       </c>
-      <c r="O89" s="50">
+      <c r="O89">
         <f t="shared" si="19"/>
         <v>3073</v>
       </c>
-      <c r="P89" s="50"/>
-      <c r="Q89" s="50">
+      <c r="Q89">
         <f t="shared" si="26"/>
         <v>103</v>
       </c>
-      <c r="R89" s="50">
+      <c r="R89">
         <f t="shared" si="27"/>
         <v>103</v>
       </c>
-      <c r="S89" s="50">
+      <c r="S89">
         <f t="shared" si="28"/>
         <v>104</v>
       </c>
-      <c r="T89" s="50"/>
-      <c r="U89" s="50" t="str">
+      <c r="U89" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V89" s="50" t="str">
+      <c r="V89" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W89" s="50" t="str">
+      <c r="W89" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="90" spans="1:23">
-      <c r="A90" s="50">
+      <c r="A90">
         <v>84</v>
       </c>
-      <c r="B90" s="50">
+      <c r="B90">
         <v>256</v>
       </c>
-      <c r="C90" s="50"/>
-      <c r="D90" s="50"/>
-      <c r="E90" s="50">
+      <c r="E90">
         <f t="shared" si="29"/>
         <v>3328</v>
       </c>
-      <c r="F90" s="50">
+      <c r="F90">
         <f t="shared" si="15"/>
         <v>217088</v>
       </c>
-      <c r="G90" s="50">
+      <c r="G90">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H90" s="50"/>
-      <c r="I90" s="50" t="str">
+      <c r="I90" t="str">
         <f t="shared" si="25"/>
         <v>{3328,217088,4194304,84},</v>
       </c>
-      <c r="J90" s="50"/>
       <c r="K90">
         <f t="shared" si="16"/>
         <v>3.25</v>
       </c>
-      <c r="L90" s="50"/>
-      <c r="M90" s="50">
+      <c r="M90">
         <f t="shared" si="17"/>
         <v>3327</v>
       </c>
-      <c r="N90" s="50">
+      <c r="N90">
         <f t="shared" si="18"/>
         <v>3328</v>
       </c>
-      <c r="O90" s="50">
+      <c r="O90">
         <f t="shared" si="19"/>
         <v>3329</v>
       </c>
-      <c r="P90" s="50"/>
-      <c r="Q90" s="50">
+      <c r="Q90">
         <f t="shared" si="26"/>
         <v>107</v>
       </c>
-      <c r="R90" s="50">
+      <c r="R90">
         <f t="shared" si="27"/>
         <v>107</v>
       </c>
-      <c r="S90" s="50">
+      <c r="S90">
         <f t="shared" si="28"/>
         <v>108</v>
       </c>
-      <c r="T90" s="50"/>
-      <c r="U90" s="50" t="str">
+      <c r="U90" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V90" s="50" t="str">
+      <c r="V90" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W90" s="50" t="str">
+      <c r="W90" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="91" spans="1:23">
-      <c r="A91" s="50">
+      <c r="A91">
         <v>85</v>
       </c>
-      <c r="B91" s="50">
+      <c r="B91">
         <v>256</v>
       </c>
-      <c r="C91" s="50"/>
-      <c r="D91" s="50"/>
-      <c r="E91" s="50">
+      <c r="E91">
         <f t="shared" si="29"/>
         <v>3584</v>
       </c>
-      <c r="F91" s="50">
+      <c r="F91">
         <f t="shared" si="15"/>
         <v>233472</v>
       </c>
-      <c r="G91" s="50">
+      <c r="G91">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H91" s="50"/>
-      <c r="I91" s="50" t="str">
+      <c r="I91" t="str">
         <f t="shared" si="25"/>
         <v>{3584,233472,4194304,85},</v>
       </c>
-      <c r="J91" s="50"/>
       <c r="K91">
         <f t="shared" si="16"/>
         <v>3.5</v>
       </c>
-      <c r="L91" s="50"/>
-      <c r="M91" s="50">
+      <c r="M91">
         <f t="shared" si="17"/>
         <v>3583</v>
       </c>
-      <c r="N91" s="50">
+      <c r="N91">
         <f t="shared" si="18"/>
         <v>3584</v>
       </c>
-      <c r="O91" s="50">
+      <c r="O91">
         <f t="shared" si="19"/>
         <v>3585</v>
       </c>
-      <c r="P91" s="50"/>
-      <c r="Q91" s="50">
+      <c r="Q91">
         <f t="shared" si="26"/>
         <v>111</v>
       </c>
-      <c r="R91" s="50">
+      <c r="R91">
         <f t="shared" si="27"/>
         <v>111</v>
       </c>
-      <c r="S91" s="50">
+      <c r="S91">
         <f t="shared" si="28"/>
         <v>112</v>
       </c>
-      <c r="T91" s="50"/>
-      <c r="U91" s="50" t="str">
+      <c r="U91" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V91" s="50" t="str">
+      <c r="V91" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W91" s="50" t="str">
+      <c r="W91" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="92" spans="1:23">
-      <c r="A92" s="50">
+      <c r="A92">
         <v>86</v>
       </c>
-      <c r="B92" s="50">
+      <c r="B92">
         <v>256</v>
       </c>
-      <c r="C92" s="50"/>
-      <c r="D92" s="50"/>
-      <c r="E92" s="50">
+      <c r="E92">
         <f t="shared" si="29"/>
         <v>3840</v>
       </c>
-      <c r="F92" s="50">
+      <c r="F92">
         <f t="shared" si="15"/>
         <v>249856</v>
       </c>
-      <c r="G92" s="50">
+      <c r="G92">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H92" s="50"/>
-      <c r="I92" s="50" t="str">
+      <c r="I92" t="str">
         <f t="shared" si="25"/>
         <v>{3840,249856,4194304,86},</v>
       </c>
-      <c r="J92" s="50"/>
       <c r="K92">
         <f t="shared" si="16"/>
         <v>3.75</v>
       </c>
-      <c r="L92" s="50"/>
-      <c r="M92" s="50">
+      <c r="M92">
         <f t="shared" si="17"/>
         <v>3839</v>
       </c>
-      <c r="N92" s="50">
+      <c r="N92">
         <f t="shared" si="18"/>
         <v>3840</v>
       </c>
-      <c r="O92" s="50">
+      <c r="O92">
         <f t="shared" si="19"/>
         <v>3841</v>
       </c>
-      <c r="P92" s="50"/>
-      <c r="Q92" s="50">
+      <c r="Q92">
         <f t="shared" si="26"/>
         <v>115</v>
       </c>
-      <c r="R92" s="50">
+      <c r="R92">
         <f t="shared" si="27"/>
         <v>115</v>
       </c>
-      <c r="S92" s="50">
+      <c r="S92">
         <f t="shared" si="28"/>
         <v>116</v>
       </c>
-      <c r="T92" s="50"/>
-      <c r="U92" s="50" t="str">
+      <c r="U92" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V92" s="50" t="str">
+      <c r="V92" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W92" s="50" t="str">
+      <c r="W92" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="93" spans="1:23">
-      <c r="A93" s="51">
+      <c r="A93" s="43">
         <v>87</v>
       </c>
-      <c r="B93" s="50">
+      <c r="B93">
         <v>256</v>
       </c>
-      <c r="C93" s="51"/>
-      <c r="D93" s="51"/>
-      <c r="E93" s="51">
+      <c r="C93" s="43"/>
+      <c r="D93" s="43"/>
+      <c r="E93" s="43">
         <f t="shared" si="29"/>
         <v>4096</v>
       </c>
-      <c r="F93" s="51">
+      <c r="F93" s="43">
         <f t="shared" si="15"/>
         <v>266240</v>
       </c>
-      <c r="G93" s="51">
+      <c r="G93" s="43">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H93" s="51"/>
-      <c r="I93" s="51" t="str">
+      <c r="H93" s="43"/>
+      <c r="I93" s="43" t="str">
         <f t="shared" si="25"/>
         <v>{4096,266240,4194304,87},</v>
       </c>
-      <c r="J93" s="51"/>
+      <c r="J93" s="43"/>
       <c r="K93">
         <f t="shared" si="16"/>
         <v>4</v>
       </c>
-      <c r="L93" s="51"/>
-      <c r="M93" s="51">
+      <c r="L93" s="43"/>
+      <c r="M93" s="43">
         <f t="shared" si="17"/>
         <v>4095</v>
       </c>
-      <c r="N93" s="51">
+      <c r="N93" s="43">
         <f t="shared" si="18"/>
         <v>4096</v>
       </c>
-      <c r="O93" s="51">
+      <c r="O93" s="43">
         <f t="shared" si="19"/>
         <v>4097</v>
       </c>
-      <c r="P93" s="51"/>
-      <c r="Q93" s="51">
+      <c r="P93" s="43"/>
+      <c r="Q93" s="43">
         <f t="shared" si="26"/>
         <v>119</v>
       </c>
-      <c r="R93" s="51">
+      <c r="R93" s="43">
         <f t="shared" si="27"/>
         <v>119</v>
       </c>
-      <c r="S93" s="51">
+      <c r="S93" s="43">
         <f t="shared" si="28"/>
         <v>120</v>
       </c>
-      <c r="T93" s="51"/>
-      <c r="U93" s="51" t="str">
+      <c r="T93" s="43"/>
+      <c r="U93" s="43" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V93" s="51" t="str">
+      <c r="V93" s="43" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W93" s="51" t="str">
+      <c r="W93" s="43" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="94" spans="1:23">
-      <c r="A94" s="49">
+      <c r="A94" s="42">
         <v>88</v>
       </c>
-      <c r="B94" s="49">
+      <c r="B94" s="42">
         <v>512</v>
       </c>
-      <c r="C94" s="49"/>
-      <c r="D94" s="49"/>
-      <c r="E94" s="49">
+      <c r="C94" s="42"/>
+      <c r="D94" s="42"/>
+      <c r="E94" s="42">
         <f t="shared" si="29"/>
         <v>4608</v>
       </c>
-      <c r="F94" s="49">
+      <c r="F94" s="42">
         <f t="shared" si="15"/>
         <v>299008</v>
       </c>
-      <c r="G94" s="49">
+      <c r="G94" s="42">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H94" s="49"/>
-      <c r="I94" s="49" t="str">
+      <c r="H94" s="42"/>
+      <c r="I94" s="42" t="str">
         <f t="shared" si="25"/>
         <v>{4608,299008,4194304,88},</v>
       </c>
-      <c r="J94" s="49"/>
+      <c r="J94" s="42"/>
       <c r="K94">
         <f t="shared" si="16"/>
         <v>4.5</v>
       </c>
-      <c r="L94" s="49"/>
-      <c r="M94" s="49">
+      <c r="L94" s="42"/>
+      <c r="M94" s="42">
         <f t="shared" si="17"/>
         <v>4607</v>
       </c>
-      <c r="N94" s="49">
+      <c r="N94" s="42">
         <f t="shared" si="18"/>
         <v>4608</v>
       </c>
-      <c r="O94" s="49">
+      <c r="O94" s="42">
         <f t="shared" si="19"/>
         <v>4609</v>
       </c>
-      <c r="P94" s="49"/>
-      <c r="Q94" s="49">
+      <c r="P94" s="42"/>
+      <c r="Q94" s="42">
         <f>INT((M94-2048-1)/128)+88</f>
         <v>107</v>
       </c>
-      <c r="R94" s="49">
+      <c r="R94" s="42">
         <f t="shared" ref="R94:S94" si="35">INT((N94-2048-1)/128)+88</f>
         <v>107</v>
       </c>
-      <c r="S94" s="49">
+      <c r="S94" s="42">
         <f t="shared" si="35"/>
         <v>108</v>
       </c>
-      <c r="T94" s="49"/>
-      <c r="U94" s="49" t="str">
+      <c r="T94" s="42"/>
+      <c r="U94" s="42" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V94" s="49" t="str">
+      <c r="V94" s="42" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W94" s="49" t="str">
+      <c r="W94" s="42" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="95" spans="1:23">
-      <c r="A95" s="50">
+      <c r="A95">
         <v>89</v>
       </c>
-      <c r="B95" s="49">
+      <c r="B95" s="42">
         <v>512</v>
       </c>
-      <c r="C95" s="50"/>
-      <c r="D95" s="50"/>
-      <c r="E95" s="50">
+      <c r="E95">
         <f t="shared" si="29"/>
         <v>5120</v>
       </c>
-      <c r="F95" s="50">
+      <c r="F95">
         <f t="shared" si="15"/>
         <v>331776</v>
       </c>
-      <c r="G95" s="50">
+      <c r="G95">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H95" s="50"/>
-      <c r="I95" s="50" t="str">
+      <c r="I95" t="str">
         <f t="shared" si="25"/>
         <v>{5120,331776,4194304,89},</v>
       </c>
-      <c r="J95" s="50"/>
       <c r="K95">
         <f t="shared" si="16"/>
         <v>5</v>
       </c>
-      <c r="L95" s="50"/>
-      <c r="M95" s="50">
+      <c r="M95">
         <f t="shared" si="17"/>
         <v>5119</v>
       </c>
-      <c r="N95" s="50">
+      <c r="N95">
         <f t="shared" si="18"/>
         <v>5120</v>
       </c>
-      <c r="O95" s="50">
+      <c r="O95">
         <f t="shared" si="19"/>
         <v>5121</v>
       </c>
-      <c r="P95" s="50"/>
-      <c r="Q95" s="50">
-        <f t="shared" ref="Q95:Q110" si="36">INT((M95-2048-1)/128)+88</f>
+      <c r="Q95">
+        <f t="shared" ref="Q95:Q109" si="36">INT((M95-2048-1)/128)+88</f>
         <v>111</v>
       </c>
-      <c r="R95" s="50">
+      <c r="R95">
         <f t="shared" ref="R95:R109" si="37">INT((N95-2048-1)/128)+88</f>
         <v>111</v>
       </c>
-      <c r="S95" s="50">
+      <c r="S95">
         <f t="shared" ref="S95:S109" si="38">INT((O95-2048-1)/128)+88</f>
         <v>112</v>
       </c>
-      <c r="T95" s="50"/>
-      <c r="U95" s="50" t="str">
+      <c r="U95" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V95" s="50" t="str">
+      <c r="V95" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W95" s="50" t="str">
+      <c r="W95" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="96" spans="1:23">
-      <c r="A96" s="50">
+      <c r="A96">
         <v>90</v>
       </c>
-      <c r="B96" s="49">
+      <c r="B96" s="42">
         <v>512</v>
       </c>
-      <c r="C96" s="50"/>
-      <c r="D96" s="50"/>
-      <c r="E96" s="50">
+      <c r="E96">
         <f t="shared" si="29"/>
         <v>5632</v>
       </c>
-      <c r="F96" s="50">
+      <c r="F96">
         <f t="shared" si="15"/>
         <v>364544</v>
       </c>
-      <c r="G96" s="50">
+      <c r="G96">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H96" s="50"/>
-      <c r="I96" s="50" t="str">
+      <c r="I96" t="str">
         <f t="shared" si="25"/>
         <v>{5632,364544,4194304,90},</v>
       </c>
-      <c r="J96" s="50"/>
       <c r="K96">
         <f t="shared" si="16"/>
         <v>5.5</v>
       </c>
-      <c r="L96" s="50"/>
-      <c r="M96" s="50">
+      <c r="M96">
         <f t="shared" si="17"/>
         <v>5631</v>
       </c>
-      <c r="N96" s="50">
+      <c r="N96">
         <f t="shared" si="18"/>
         <v>5632</v>
       </c>
-      <c r="O96" s="50">
+      <c r="O96">
         <f t="shared" si="19"/>
         <v>5633</v>
       </c>
-      <c r="P96" s="50"/>
-      <c r="Q96" s="50">
+      <c r="Q96">
         <f t="shared" si="36"/>
         <v>115</v>
       </c>
-      <c r="R96" s="50">
+      <c r="R96">
         <f t="shared" si="37"/>
         <v>115</v>
       </c>
-      <c r="S96" s="50">
+      <c r="S96">
         <f t="shared" si="38"/>
         <v>116</v>
       </c>
-      <c r="T96" s="50"/>
-      <c r="U96" s="50" t="str">
+      <c r="U96" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V96" s="50" t="str">
+      <c r="V96" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W96" s="50" t="str">
+      <c r="W96" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="97" spans="1:23">
-      <c r="A97" s="50">
+      <c r="A97">
         <v>91</v>
       </c>
-      <c r="B97" s="49">
+      <c r="B97" s="42">
         <v>512</v>
       </c>
-      <c r="C97" s="50"/>
-      <c r="D97" s="50"/>
-      <c r="E97" s="50">
+      <c r="E97">
         <f t="shared" si="29"/>
         <v>6144</v>
       </c>
-      <c r="F97" s="50">
+      <c r="F97">
         <f t="shared" si="15"/>
         <v>397312</v>
       </c>
-      <c r="G97" s="50">
+      <c r="G97">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H97" s="50"/>
-      <c r="I97" s="50" t="str">
+      <c r="I97" t="str">
         <f t="shared" si="25"/>
         <v>{6144,397312,4194304,91},</v>
       </c>
-      <c r="J97" s="50"/>
       <c r="K97">
         <f t="shared" si="16"/>
         <v>6</v>
       </c>
-      <c r="L97" s="50"/>
-      <c r="M97" s="50">
+      <c r="M97">
         <f t="shared" si="17"/>
         <v>6143</v>
       </c>
-      <c r="N97" s="50">
+      <c r="N97">
         <f t="shared" si="18"/>
         <v>6144</v>
       </c>
-      <c r="O97" s="50">
+      <c r="O97">
         <f t="shared" si="19"/>
         <v>6145</v>
       </c>
-      <c r="P97" s="50"/>
-      <c r="Q97" s="50">
+      <c r="Q97">
         <f t="shared" si="36"/>
         <v>119</v>
       </c>
-      <c r="R97" s="50">
+      <c r="R97">
         <f t="shared" si="37"/>
         <v>119</v>
       </c>
-      <c r="S97" s="50">
+      <c r="S97">
         <f t="shared" si="38"/>
         <v>120</v>
       </c>
-      <c r="T97" s="50"/>
-      <c r="U97" s="50" t="str">
+      <c r="U97" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V97" s="50" t="str">
+      <c r="V97" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W97" s="50" t="str">
+      <c r="W97" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="98" spans="1:23">
-      <c r="A98" s="50">
+      <c r="A98">
         <v>92</v>
       </c>
-      <c r="B98" s="49">
+      <c r="B98" s="42">
         <v>512</v>
       </c>
-      <c r="C98" s="50"/>
-      <c r="D98" s="50"/>
-      <c r="E98" s="50">
+      <c r="E98">
         <f t="shared" si="29"/>
         <v>6656</v>
       </c>
-      <c r="F98" s="50">
+      <c r="F98">
         <f t="shared" si="15"/>
         <v>430080</v>
       </c>
-      <c r="G98" s="50">
+      <c r="G98">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H98" s="50"/>
-      <c r="I98" s="50" t="str">
+      <c r="I98" t="str">
         <f t="shared" si="25"/>
         <v>{6656,430080,4194304,92},</v>
       </c>
-      <c r="J98" s="50"/>
       <c r="K98">
         <f t="shared" si="16"/>
         <v>6.5</v>
       </c>
-      <c r="L98" s="50"/>
-      <c r="M98" s="50">
+      <c r="M98">
         <f t="shared" si="17"/>
         <v>6655</v>
       </c>
-      <c r="N98" s="50">
+      <c r="N98">
         <f t="shared" si="18"/>
         <v>6656</v>
       </c>
-      <c r="O98" s="50">
+      <c r="O98">
         <f t="shared" si="19"/>
         <v>6657</v>
       </c>
-      <c r="P98" s="50"/>
-      <c r="Q98" s="50">
+      <c r="Q98">
         <f t="shared" si="36"/>
         <v>123</v>
       </c>
-      <c r="R98" s="50">
+      <c r="R98">
         <f t="shared" si="37"/>
         <v>123</v>
       </c>
-      <c r="S98" s="50">
+      <c r="S98">
         <f t="shared" si="38"/>
         <v>124</v>
       </c>
-      <c r="T98" s="50"/>
-      <c r="U98" s="50" t="str">
+      <c r="U98" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V98" s="50" t="str">
+      <c r="V98" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W98" s="50" t="str">
+      <c r="W98" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="99" spans="1:23">
-      <c r="A99" s="50">
+      <c r="A99">
         <v>93</v>
       </c>
-      <c r="B99" s="49">
+      <c r="B99" s="42">
         <v>512</v>
       </c>
-      <c r="C99" s="50"/>
-      <c r="D99" s="50"/>
-      <c r="E99" s="50">
+      <c r="E99">
         <f t="shared" si="29"/>
         <v>7168</v>
       </c>
-      <c r="F99" s="50">
+      <c r="F99">
         <f t="shared" si="15"/>
         <v>462848</v>
       </c>
-      <c r="G99" s="50">
+      <c r="G99">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H99" s="50"/>
-      <c r="I99" s="50" t="str">
+      <c r="I99" t="str">
         <f t="shared" si="25"/>
         <v>{7168,462848,4194304,93},</v>
       </c>
-      <c r="J99" s="50"/>
       <c r="K99">
         <f t="shared" si="16"/>
         <v>7</v>
       </c>
-      <c r="L99" s="50"/>
-      <c r="M99" s="50">
+      <c r="M99">
         <f t="shared" si="17"/>
         <v>7167</v>
       </c>
-      <c r="N99" s="50">
+      <c r="N99">
         <f t="shared" si="18"/>
         <v>7168</v>
       </c>
-      <c r="O99" s="50">
+      <c r="O99">
         <f t="shared" si="19"/>
         <v>7169</v>
       </c>
-      <c r="P99" s="50"/>
-      <c r="Q99" s="50">
+      <c r="Q99">
         <f t="shared" si="36"/>
         <v>127</v>
       </c>
-      <c r="R99" s="50">
+      <c r="R99">
         <f t="shared" si="37"/>
         <v>127</v>
       </c>
-      <c r="S99" s="50">
+      <c r="S99">
         <f t="shared" si="38"/>
         <v>128</v>
       </c>
-      <c r="T99" s="50"/>
-      <c r="U99" s="50" t="str">
+      <c r="U99" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V99" s="50" t="str">
+      <c r="V99" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W99" s="50" t="str">
+      <c r="W99" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="100" spans="1:23">
-      <c r="A100" s="50">
+      <c r="A100">
         <v>94</v>
       </c>
-      <c r="B100" s="49">
+      <c r="B100" s="42">
         <v>512</v>
       </c>
-      <c r="C100" s="50"/>
-      <c r="D100" s="50"/>
-      <c r="E100" s="50">
+      <c r="E100">
         <f t="shared" si="29"/>
         <v>7680</v>
       </c>
-      <c r="F100" s="50">
+      <c r="F100">
         <f t="shared" si="15"/>
         <v>495616</v>
       </c>
-      <c r="G100" s="50">
+      <c r="G100">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H100" s="50"/>
-      <c r="I100" s="50" t="str">
+      <c r="I100" t="str">
         <f t="shared" si="25"/>
         <v>{7680,495616,4194304,94},</v>
       </c>
-      <c r="J100" s="50"/>
       <c r="K100">
         <f t="shared" si="16"/>
         <v>7.5</v>
       </c>
-      <c r="L100" s="50"/>
-      <c r="M100" s="50">
+      <c r="M100">
         <f t="shared" si="17"/>
         <v>7679</v>
       </c>
-      <c r="N100" s="50">
+      <c r="N100">
         <f t="shared" si="18"/>
         <v>7680</v>
       </c>
-      <c r="O100" s="50">
+      <c r="O100">
         <f t="shared" si="19"/>
         <v>7681</v>
       </c>
-      <c r="P100" s="50"/>
-      <c r="Q100" s="50">
+      <c r="Q100">
         <f t="shared" si="36"/>
         <v>131</v>
       </c>
-      <c r="R100" s="50">
+      <c r="R100">
         <f t="shared" si="37"/>
         <v>131</v>
       </c>
-      <c r="S100" s="50">
+      <c r="S100">
         <f t="shared" si="38"/>
         <v>132</v>
       </c>
-      <c r="T100" s="50"/>
-      <c r="U100" s="50" t="str">
+      <c r="U100" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V100" s="50" t="str">
+      <c r="V100" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W100" s="50" t="str">
+      <c r="W100" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="101" spans="1:23">
-      <c r="A101" s="50">
+      <c r="A101">
         <v>95</v>
       </c>
-      <c r="B101" s="49">
+      <c r="B101" s="42">
         <v>512</v>
       </c>
-      <c r="C101" s="50"/>
-      <c r="D101" s="50"/>
-      <c r="E101" s="50">
+      <c r="E101">
         <f t="shared" si="29"/>
         <v>8192</v>
       </c>
-      <c r="F101" s="50">
+      <c r="F101">
         <f t="shared" si="15"/>
         <v>528384</v>
       </c>
-      <c r="G101" s="50">
+      <c r="G101">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H101" s="50"/>
-      <c r="I101" s="50" t="str">
+      <c r="I101" t="str">
         <f t="shared" si="25"/>
         <v>{8192,528384,4194304,95},</v>
       </c>
-      <c r="J101" s="50"/>
       <c r="K101">
         <f t="shared" si="16"/>
         <v>8</v>
       </c>
-      <c r="L101" s="50"/>
-      <c r="M101" s="50">
+      <c r="M101">
         <f t="shared" si="17"/>
         <v>8191</v>
       </c>
-      <c r="N101" s="50">
+      <c r="N101">
         <f t="shared" si="18"/>
         <v>8192</v>
       </c>
-      <c r="O101" s="50">
+      <c r="O101">
         <f t="shared" si="19"/>
         <v>8193</v>
       </c>
-      <c r="P101" s="50"/>
-      <c r="Q101" s="50">
+      <c r="Q101">
         <f t="shared" si="36"/>
         <v>135</v>
       </c>
-      <c r="R101" s="50">
+      <c r="R101">
         <f t="shared" si="37"/>
         <v>135</v>
       </c>
-      <c r="S101" s="50">
+      <c r="S101">
         <f t="shared" si="38"/>
         <v>136</v>
       </c>
-      <c r="T101" s="50"/>
-      <c r="U101" s="50" t="str">
+      <c r="U101" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V101" s="50" t="str">
+      <c r="V101" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W101" s="50" t="str">
+      <c r="W101" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="102" spans="1:23">
-      <c r="A102" s="50">
+      <c r="A102">
         <v>96</v>
       </c>
-      <c r="B102" s="49">
+      <c r="B102" s="42">
         <v>1024</v>
       </c>
-      <c r="C102" s="50"/>
-      <c r="D102" s="50"/>
-      <c r="E102" s="50">
+      <c r="E102">
         <f t="shared" si="29"/>
         <v>9216</v>
       </c>
-      <c r="F102" s="50">
+      <c r="F102">
         <f>IF(E102*32 &gt;F$101, INT((E102*32+4096)/4096)*4096,F$101)</f>
         <v>528384</v>
       </c>
-      <c r="G102" s="50">
+      <c r="G102">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H102" s="50"/>
-      <c r="I102" s="50" t="str">
+      <c r="I102" t="str">
         <f t="shared" si="25"/>
         <v>{9216,528384,4194304,96},</v>
       </c>
-      <c r="J102" s="50"/>
       <c r="K102">
         <f t="shared" si="16"/>
         <v>9</v>
       </c>
-      <c r="L102" s="50"/>
-      <c r="M102" s="50">
+      <c r="M102">
         <f t="shared" si="17"/>
         <v>9215</v>
       </c>
-      <c r="N102" s="50">
+      <c r="N102">
         <f t="shared" si="18"/>
         <v>9216</v>
       </c>
-      <c r="O102" s="50">
+      <c r="O102">
         <f t="shared" si="19"/>
         <v>9217</v>
       </c>
-      <c r="P102" s="50"/>
-      <c r="Q102" s="50">
+      <c r="Q102">
         <f t="shared" si="36"/>
         <v>143</v>
       </c>
-      <c r="R102" s="50">
+      <c r="R102">
         <f t="shared" si="37"/>
         <v>143</v>
       </c>
-      <c r="S102" s="50">
+      <c r="S102">
         <f t="shared" si="38"/>
         <v>144</v>
       </c>
-      <c r="T102" s="50"/>
-      <c r="U102" s="50" t="str">
+      <c r="U102" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V102" s="50" t="str">
+      <c r="V102" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W102" s="50" t="str">
+      <c r="W102" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="103" spans="1:23">
-      <c r="A103" s="50">
+      <c r="A103">
         <v>97</v>
       </c>
-      <c r="B103" s="49">
+      <c r="B103" s="42">
         <v>1024</v>
       </c>
-      <c r="C103" s="50"/>
-      <c r="D103" s="50"/>
-      <c r="E103" s="50">
+      <c r="E103">
         <f t="shared" si="29"/>
         <v>10240</v>
       </c>
-      <c r="F103" s="50">
+      <c r="F103">
         <f t="shared" ref="F103:F117" si="39">IF(E103*32 &gt;F$101, INT((E103*32+4096)/4096)*4096,F$101)</f>
         <v>528384</v>
       </c>
-      <c r="G103" s="50">
+      <c r="G103">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H103" s="50"/>
-      <c r="I103" s="50" t="str">
+      <c r="I103" t="str">
         <f t="shared" si="25"/>
         <v>{10240,528384,4194304,97},</v>
       </c>
-      <c r="J103" s="50"/>
       <c r="K103">
         <f t="shared" si="16"/>
         <v>10</v>
       </c>
-      <c r="L103" s="50"/>
-      <c r="M103" s="50">
+      <c r="M103">
         <f t="shared" si="17"/>
         <v>10239</v>
       </c>
-      <c r="N103" s="50">
+      <c r="N103">
         <f t="shared" si="18"/>
         <v>10240</v>
       </c>
-      <c r="O103" s="50">
+      <c r="O103">
         <f t="shared" si="19"/>
         <v>10241</v>
       </c>
-      <c r="P103" s="50"/>
-      <c r="Q103" s="50">
+      <c r="Q103">
         <f t="shared" si="36"/>
         <v>151</v>
       </c>
-      <c r="R103" s="50">
+      <c r="R103">
         <f t="shared" si="37"/>
         <v>151</v>
       </c>
-      <c r="S103" s="50">
+      <c r="S103">
         <f t="shared" si="38"/>
         <v>152</v>
       </c>
-      <c r="T103" s="50"/>
-      <c r="U103" s="50" t="str">
+      <c r="U103" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V103" s="50" t="str">
+      <c r="V103" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W103" s="50" t="str">
+      <c r="W103" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="104" spans="1:23">
-      <c r="A104" s="50">
+      <c r="A104">
         <v>98</v>
       </c>
-      <c r="B104" s="49">
+      <c r="B104" s="42">
         <v>1024</v>
       </c>
-      <c r="C104" s="50"/>
-      <c r="D104" s="50"/>
-      <c r="E104" s="50">
+      <c r="E104">
         <f t="shared" si="29"/>
         <v>11264</v>
       </c>
-      <c r="F104" s="50">
+      <c r="F104">
         <f t="shared" si="39"/>
         <v>528384</v>
       </c>
-      <c r="G104" s="50">
+      <c r="G104">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H104" s="50"/>
-      <c r="I104" s="50" t="str">
+      <c r="I104" t="str">
         <f t="shared" si="25"/>
         <v>{11264,528384,4194304,98},</v>
       </c>
-      <c r="J104" s="50"/>
       <c r="K104">
         <f t="shared" si="16"/>
         <v>11</v>
       </c>
-      <c r="L104" s="50"/>
-      <c r="M104" s="50">
+      <c r="M104">
         <f t="shared" si="17"/>
         <v>11263</v>
       </c>
-      <c r="N104" s="50">
+      <c r="N104">
         <f t="shared" si="18"/>
         <v>11264</v>
       </c>
-      <c r="O104" s="50">
+      <c r="O104">
         <f t="shared" si="19"/>
         <v>11265</v>
       </c>
-      <c r="P104" s="50"/>
-      <c r="Q104" s="50">
+      <c r="Q104">
         <f t="shared" si="36"/>
         <v>159</v>
       </c>
-      <c r="R104" s="50">
+      <c r="R104">
         <f t="shared" si="37"/>
         <v>159</v>
       </c>
-      <c r="S104" s="50">
+      <c r="S104">
         <f t="shared" si="38"/>
         <v>160</v>
       </c>
-      <c r="T104" s="50"/>
-      <c r="U104" s="50" t="str">
+      <c r="U104" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V104" s="50" t="str">
+      <c r="V104" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W104" s="50" t="str">
+      <c r="W104" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="105" spans="1:23">
-      <c r="A105" s="50">
+      <c r="A105">
         <v>99</v>
       </c>
-      <c r="B105" s="49">
+      <c r="B105" s="42">
         <v>1024</v>
       </c>
-      <c r="C105" s="50"/>
-      <c r="D105" s="50"/>
-      <c r="E105" s="50">
+      <c r="E105">
         <f t="shared" si="29"/>
         <v>12288</v>
       </c>
-      <c r="F105" s="50">
+      <c r="F105">
         <f t="shared" si="39"/>
         <v>528384</v>
       </c>
-      <c r="G105" s="50">
+      <c r="G105">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H105" s="50"/>
-      <c r="I105" s="50" t="str">
+      <c r="I105" t="str">
         <f t="shared" si="25"/>
         <v>{12288,528384,4194304,99},</v>
       </c>
-      <c r="J105" s="50"/>
       <c r="K105">
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
-      <c r="L105" s="50"/>
-      <c r="M105" s="50">
+      <c r="M105">
         <f t="shared" si="17"/>
         <v>12287</v>
       </c>
-      <c r="N105" s="50">
+      <c r="N105">
         <f t="shared" si="18"/>
         <v>12288</v>
       </c>
-      <c r="O105" s="50">
+      <c r="O105">
         <f t="shared" si="19"/>
         <v>12289</v>
       </c>
-      <c r="P105" s="50"/>
-      <c r="Q105" s="50">
+      <c r="Q105">
         <f t="shared" si="36"/>
         <v>167</v>
       </c>
-      <c r="R105" s="50">
+      <c r="R105">
         <f t="shared" si="37"/>
         <v>167</v>
       </c>
-      <c r="S105" s="50">
+      <c r="S105">
         <f t="shared" si="38"/>
         <v>168</v>
       </c>
-      <c r="T105" s="50"/>
-      <c r="U105" s="50" t="str">
+      <c r="U105" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V105" s="50" t="str">
+      <c r="V105" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W105" s="50" t="str">
+      <c r="W105" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="106" spans="1:23">
-      <c r="A106" s="50">
+      <c r="A106">
         <v>100</v>
       </c>
-      <c r="B106" s="49">
+      <c r="B106" s="42">
         <v>1024</v>
       </c>
-      <c r="C106" s="50"/>
-      <c r="D106" s="50"/>
-      <c r="E106" s="50">
+      <c r="E106">
         <f t="shared" si="29"/>
         <v>13312</v>
       </c>
-      <c r="F106" s="50">
+      <c r="F106">
         <f t="shared" si="39"/>
         <v>528384</v>
       </c>
-      <c r="G106" s="50">
+      <c r="G106">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H106" s="50"/>
-      <c r="I106" s="50" t="str">
+      <c r="I106" t="str">
         <f t="shared" si="25"/>
         <v>{13312,528384,4194304,100},</v>
       </c>
-      <c r="J106" s="50"/>
       <c r="K106">
         <f t="shared" si="16"/>
         <v>13</v>
       </c>
-      <c r="L106" s="50"/>
-      <c r="M106" s="50">
+      <c r="M106">
         <f t="shared" si="17"/>
         <v>13311</v>
       </c>
-      <c r="N106" s="50">
+      <c r="N106">
         <f t="shared" si="18"/>
         <v>13312</v>
       </c>
-      <c r="O106" s="50">
+      <c r="O106">
         <f t="shared" si="19"/>
         <v>13313</v>
       </c>
-      <c r="P106" s="50"/>
-      <c r="Q106" s="50">
+      <c r="Q106">
         <f t="shared" si="36"/>
         <v>175</v>
       </c>
-      <c r="R106" s="50">
+      <c r="R106">
         <f t="shared" si="37"/>
         <v>175</v>
       </c>
-      <c r="S106" s="50">
+      <c r="S106">
         <f t="shared" si="38"/>
         <v>176</v>
       </c>
-      <c r="T106" s="50"/>
-      <c r="U106" s="50" t="str">
+      <c r="U106" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V106" s="50" t="str">
+      <c r="V106" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W106" s="50" t="str">
+      <c r="W106" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="107" spans="1:23">
-      <c r="A107" s="50">
+      <c r="A107">
         <v>101</v>
       </c>
-      <c r="B107" s="49">
+      <c r="B107" s="42">
         <v>1024</v>
       </c>
-      <c r="C107" s="50"/>
-      <c r="D107" s="50"/>
-      <c r="E107" s="50">
+      <c r="E107">
         <f t="shared" si="29"/>
         <v>14336</v>
       </c>
-      <c r="F107" s="50">
+      <c r="F107">
         <f t="shared" si="39"/>
         <v>528384</v>
       </c>
-      <c r="G107" s="50">
+      <c r="G107">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H107" s="50"/>
-      <c r="I107" s="50" t="str">
+      <c r="I107" t="str">
         <f t="shared" si="25"/>
         <v>{14336,528384,4194304,101},</v>
       </c>
-      <c r="J107" s="50"/>
       <c r="K107">
         <f t="shared" si="16"/>
         <v>14</v>
       </c>
-      <c r="L107" s="50"/>
-      <c r="M107" s="50">
+      <c r="M107">
         <f t="shared" si="17"/>
         <v>14335</v>
       </c>
-      <c r="N107" s="50">
+      <c r="N107">
         <f t="shared" si="18"/>
         <v>14336</v>
       </c>
-      <c r="O107" s="50">
+      <c r="O107">
         <f t="shared" si="19"/>
         <v>14337</v>
       </c>
-      <c r="P107" s="50"/>
-      <c r="Q107" s="50">
+      <c r="Q107">
         <f t="shared" si="36"/>
         <v>183</v>
       </c>
-      <c r="R107" s="50">
+      <c r="R107">
         <f t="shared" si="37"/>
         <v>183</v>
       </c>
-      <c r="S107" s="50">
+      <c r="S107">
         <f t="shared" si="38"/>
         <v>184</v>
       </c>
-      <c r="T107" s="50"/>
-      <c r="U107" s="50" t="str">
+      <c r="U107" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V107" s="50" t="str">
+      <c r="V107" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W107" s="50" t="str">
+      <c r="W107" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="108" spans="1:23">
-      <c r="A108" s="50">
+      <c r="A108">
         <v>102</v>
       </c>
-      <c r="B108" s="49">
+      <c r="B108" s="42">
         <v>1024</v>
       </c>
-      <c r="C108" s="50"/>
-      <c r="D108" s="50"/>
-      <c r="E108" s="50">
+      <c r="E108">
         <f t="shared" si="29"/>
         <v>15360</v>
       </c>
-      <c r="F108" s="50">
+      <c r="F108">
         <f t="shared" si="39"/>
         <v>528384</v>
       </c>
-      <c r="G108" s="50">
+      <c r="G108">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H108" s="50"/>
-      <c r="I108" s="50" t="str">
+      <c r="I108" t="str">
         <f t="shared" si="25"/>
         <v>{15360,528384,4194304,102},</v>
       </c>
-      <c r="J108" s="50"/>
       <c r="K108">
         <f t="shared" si="16"/>
         <v>15</v>
       </c>
-      <c r="L108" s="50"/>
-      <c r="M108" s="50">
+      <c r="M108">
         <f t="shared" si="17"/>
         <v>15359</v>
       </c>
-      <c r="N108" s="50">
+      <c r="N108">
         <f t="shared" si="18"/>
         <v>15360</v>
       </c>
-      <c r="O108" s="50">
+      <c r="O108">
         <f t="shared" si="19"/>
         <v>15361</v>
       </c>
-      <c r="P108" s="50"/>
-      <c r="Q108" s="50">
+      <c r="Q108">
         <f t="shared" si="36"/>
         <v>191</v>
       </c>
-      <c r="R108" s="50">
+      <c r="R108">
         <f t="shared" si="37"/>
         <v>191</v>
       </c>
-      <c r="S108" s="50">
+      <c r="S108">
         <f t="shared" si="38"/>
         <v>192</v>
       </c>
-      <c r="T108" s="50"/>
-      <c r="U108" s="50" t="str">
+      <c r="U108" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V108" s="50" t="str">
+      <c r="V108" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W108" s="50" t="str">
+      <c r="W108" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="109" spans="1:23">
-      <c r="A109" s="51">
+      <c r="A109" s="43">
         <v>103</v>
       </c>
-      <c r="B109" s="49">
+      <c r="B109" s="42">
         <v>1024</v>
       </c>
-      <c r="C109" s="51"/>
-      <c r="D109" s="51"/>
-      <c r="E109" s="51">
+      <c r="C109" s="43"/>
+      <c r="D109" s="43"/>
+      <c r="E109" s="43">
         <f t="shared" si="29"/>
         <v>16384</v>
       </c>
-      <c r="F109" s="51">
+      <c r="F109" s="43">
         <f t="shared" si="39"/>
         <v>528384</v>
       </c>
-      <c r="G109" s="51">
+      <c r="G109" s="43">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H109" s="51"/>
-      <c r="I109" s="51" t="str">
+      <c r="H109" s="43"/>
+      <c r="I109" s="43" t="str">
         <f t="shared" si="25"/>
         <v>{16384,528384,4194304,103},</v>
       </c>
-      <c r="J109" s="51"/>
+      <c r="J109" s="43"/>
       <c r="K109">
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-      <c r="L109" s="51"/>
-      <c r="M109" s="51">
+      <c r="L109" s="43"/>
+      <c r="M109" s="43">
         <f t="shared" si="17"/>
         <v>16383</v>
       </c>
-      <c r="N109" s="51">
+      <c r="N109" s="43">
         <f t="shared" si="18"/>
         <v>16384</v>
       </c>
-      <c r="O109" s="51">
+      <c r="O109" s="43">
         <f t="shared" si="19"/>
         <v>16385</v>
       </c>
-      <c r="P109" s="51"/>
-      <c r="Q109" s="51">
+      <c r="P109" s="43"/>
+      <c r="Q109" s="43">
         <f t="shared" si="36"/>
         <v>199</v>
       </c>
-      <c r="R109" s="51">
+      <c r="R109" s="43">
         <f t="shared" si="37"/>
         <v>199</v>
       </c>
-      <c r="S109" s="51">
+      <c r="S109" s="43">
         <f t="shared" si="38"/>
         <v>200</v>
       </c>
-      <c r="T109" s="51"/>
-      <c r="U109" s="51" t="str">
+      <c r="T109" s="43"/>
+      <c r="U109" s="43" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V109" s="51" t="str">
+      <c r="V109" s="43" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W109" s="51" t="str">
+      <c r="W109" s="43" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="110" spans="1:23">
-      <c r="A110" s="49">
+      <c r="A110" s="42">
         <v>104</v>
       </c>
-      <c r="B110" s="49">
+      <c r="B110" s="42">
         <v>2048</v>
       </c>
-      <c r="C110" s="49"/>
-      <c r="D110" s="49"/>
-      <c r="E110" s="49">
+      <c r="C110" s="42"/>
+      <c r="D110" s="42"/>
+      <c r="E110" s="42">
         <f t="shared" si="29"/>
         <v>18432</v>
       </c>
-      <c r="F110" s="49">
+      <c r="F110" s="42">
         <f t="shared" si="39"/>
         <v>593920</v>
       </c>
-      <c r="G110" s="49">
+      <c r="G110" s="42">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H110" s="49"/>
-      <c r="I110" s="49" t="str">
+      <c r="H110" s="42"/>
+      <c r="I110" s="42" t="str">
         <f t="shared" si="25"/>
         <v>{18432,593920,4194304,104},</v>
       </c>
-      <c r="J110" s="49"/>
+      <c r="J110" s="42"/>
       <c r="K110">
         <f t="shared" si="16"/>
         <v>18</v>
       </c>
-      <c r="L110" s="49"/>
-      <c r="M110" s="49">
+      <c r="L110" s="42"/>
+      <c r="M110" s="42">
         <f t="shared" si="17"/>
         <v>18431</v>
       </c>
-      <c r="N110" s="49">
+      <c r="N110" s="42">
         <f t="shared" si="18"/>
         <v>18432</v>
       </c>
-      <c r="O110" s="49">
+      <c r="O110" s="42">
         <f t="shared" si="19"/>
         <v>18433</v>
       </c>
-      <c r="P110" s="49"/>
-      <c r="Q110" s="49">
+      <c r="P110" s="42"/>
+      <c r="Q110" s="42">
         <f>INT((M110-4096-1)/256)+104</f>
         <v>159</v>
       </c>
-      <c r="R110" s="49">
+      <c r="R110" s="42">
         <f t="shared" ref="R110:S110" si="40">INT((N110-4096-1)/256)+104</f>
         <v>159</v>
       </c>
-      <c r="S110" s="49">
+      <c r="S110" s="42">
         <f t="shared" si="40"/>
         <v>160</v>
       </c>
-      <c r="T110" s="49"/>
-      <c r="U110" s="49" t="str">
+      <c r="T110" s="42"/>
+      <c r="U110" s="42" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V110" s="49" t="str">
+      <c r="V110" s="42" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W110" s="49" t="str">
+      <c r="W110" s="42" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="111" spans="1:23">
-      <c r="A111" s="50">
+      <c r="A111">
         <v>105</v>
       </c>
-      <c r="B111" s="49">
+      <c r="B111" s="42">
         <v>2048</v>
       </c>
-      <c r="C111" s="50"/>
-      <c r="D111" s="50"/>
-      <c r="E111" s="50">
+      <c r="E111">
         <f t="shared" si="29"/>
         <v>20480</v>
       </c>
-      <c r="F111" s="50">
+      <c r="F111">
         <f t="shared" si="39"/>
         <v>659456</v>
       </c>
-      <c r="G111" s="50">
+      <c r="G111">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H111" s="50"/>
-      <c r="I111" s="50" t="str">
+      <c r="I111" t="str">
         <f t="shared" si="25"/>
         <v>{20480,659456,4194304,105},</v>
       </c>
-      <c r="J111" s="50"/>
       <c r="K111">
         <f t="shared" si="16"/>
         <v>20</v>
       </c>
-      <c r="L111" s="50"/>
-      <c r="M111" s="50">
+      <c r="M111">
         <f t="shared" si="17"/>
         <v>20479</v>
       </c>
-      <c r="N111" s="50">
+      <c r="N111">
         <f t="shared" si="18"/>
         <v>20480</v>
       </c>
-      <c r="O111" s="50">
+      <c r="O111">
         <f t="shared" si="19"/>
         <v>20481</v>
       </c>
-      <c r="P111" s="50"/>
-      <c r="Q111" s="50">
+      <c r="Q111">
         <f t="shared" ref="Q111:Q117" si="41">INT((M111-4096-1)/256)+104</f>
         <v>167</v>
       </c>
-      <c r="R111" s="50">
+      <c r="R111">
         <f t="shared" ref="R111:R117" si="42">INT((N111-4096-1)/256)+104</f>
         <v>167</v>
       </c>
-      <c r="S111" s="50">
+      <c r="S111">
         <f t="shared" ref="S111:S117" si="43">INT((O111-4096-1)/256)+104</f>
         <v>168</v>
       </c>
-      <c r="T111" s="50"/>
-      <c r="U111" s="50" t="str">
+      <c r="U111" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V111" s="50" t="str">
+      <c r="V111" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W111" s="50" t="str">
+      <c r="W111" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="112" spans="1:23">
-      <c r="A112" s="50">
+      <c r="A112">
         <v>106</v>
       </c>
-      <c r="B112" s="49">
+      <c r="B112" s="42">
         <v>2048</v>
       </c>
-      <c r="C112" s="50"/>
-      <c r="D112" s="50"/>
-      <c r="E112" s="50">
+      <c r="E112">
         <f t="shared" si="29"/>
         <v>22528</v>
       </c>
-      <c r="F112" s="50">
+      <c r="F112">
         <f t="shared" si="39"/>
         <v>724992</v>
       </c>
-      <c r="G112" s="50">
+      <c r="G112">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H112" s="50"/>
-      <c r="I112" s="50" t="str">
+      <c r="I112" t="str">
         <f t="shared" si="25"/>
         <v>{22528,724992,4194304,106},</v>
       </c>
-      <c r="J112" s="50"/>
       <c r="K112">
         <f t="shared" si="16"/>
         <v>22</v>
       </c>
-      <c r="L112" s="50"/>
-      <c r="M112" s="50">
+      <c r="M112">
         <f t="shared" si="17"/>
         <v>22527</v>
       </c>
-      <c r="N112" s="50">
+      <c r="N112">
         <f t="shared" si="18"/>
         <v>22528</v>
       </c>
-      <c r="O112" s="50">
+      <c r="O112">
         <f t="shared" si="19"/>
         <v>22529</v>
       </c>
-      <c r="P112" s="50"/>
-      <c r="Q112" s="50">
+      <c r="Q112">
         <f t="shared" si="41"/>
         <v>175</v>
       </c>
-      <c r="R112" s="50">
+      <c r="R112">
         <f t="shared" si="42"/>
         <v>175</v>
       </c>
-      <c r="S112" s="50">
+      <c r="S112">
         <f t="shared" si="43"/>
         <v>176</v>
       </c>
-      <c r="T112" s="50"/>
-      <c r="U112" s="50" t="str">
+      <c r="U112" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V112" s="50" t="str">
+      <c r="V112" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W112" s="50" t="str">
+      <c r="W112" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="113" spans="1:23">
-      <c r="A113" s="50">
+      <c r="A113">
         <v>107</v>
       </c>
-      <c r="B113" s="49">
+      <c r="B113" s="42">
         <v>2048</v>
       </c>
-      <c r="C113" s="50"/>
-      <c r="D113" s="50"/>
-      <c r="E113" s="50">
+      <c r="E113">
         <f t="shared" si="29"/>
         <v>24576</v>
       </c>
-      <c r="F113" s="50">
+      <c r="F113">
         <f t="shared" si="39"/>
         <v>790528</v>
       </c>
-      <c r="G113" s="50">
+      <c r="G113">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H113" s="50"/>
-      <c r="I113" s="50" t="str">
+      <c r="I113" t="str">
         <f t="shared" si="25"/>
         <v>{24576,790528,4194304,107},</v>
       </c>
-      <c r="J113" s="50"/>
       <c r="K113">
         <f t="shared" si="16"/>
         <v>24</v>
       </c>
-      <c r="L113" s="50"/>
-      <c r="M113" s="50">
+      <c r="M113">
         <f t="shared" si="17"/>
         <v>24575</v>
       </c>
-      <c r="N113" s="50">
+      <c r="N113">
         <f t="shared" si="18"/>
         <v>24576</v>
       </c>
-      <c r="O113" s="50">
+      <c r="O113">
         <f t="shared" si="19"/>
         <v>24577</v>
       </c>
-      <c r="P113" s="50"/>
-      <c r="Q113" s="50">
+      <c r="Q113">
         <f t="shared" si="41"/>
         <v>183</v>
       </c>
-      <c r="R113" s="50">
+      <c r="R113">
         <f t="shared" si="42"/>
         <v>183</v>
       </c>
-      <c r="S113" s="50">
+      <c r="S113">
         <f t="shared" si="43"/>
         <v>184</v>
       </c>
-      <c r="T113" s="50"/>
-      <c r="U113" s="50" t="str">
+      <c r="U113" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V113" s="50" t="str">
+      <c r="V113" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W113" s="50" t="str">
+      <c r="W113" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="114" spans="1:23">
-      <c r="A114" s="50">
+      <c r="A114">
         <v>108</v>
       </c>
-      <c r="B114" s="49">
+      <c r="B114" s="42">
         <v>2048</v>
       </c>
-      <c r="C114" s="50"/>
-      <c r="D114" s="50"/>
-      <c r="E114" s="50">
+      <c r="E114">
         <f t="shared" si="29"/>
         <v>26624</v>
       </c>
-      <c r="F114" s="50">
+      <c r="F114">
         <f t="shared" si="39"/>
         <v>856064</v>
       </c>
-      <c r="G114" s="50">
+      <c r="G114">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H114" s="50"/>
-      <c r="I114" s="50" t="str">
+      <c r="I114" t="str">
         <f t="shared" si="25"/>
         <v>{26624,856064,4194304,108},</v>
       </c>
-      <c r="J114" s="50"/>
       <c r="K114">
         <f t="shared" si="16"/>
         <v>26</v>
       </c>
-      <c r="L114" s="50"/>
-      <c r="M114" s="50">
+      <c r="M114">
         <f t="shared" si="17"/>
         <v>26623</v>
       </c>
-      <c r="N114" s="50">
+      <c r="N114">
         <f t="shared" si="18"/>
         <v>26624</v>
       </c>
-      <c r="O114" s="50">
+      <c r="O114">
         <f t="shared" si="19"/>
         <v>26625</v>
       </c>
-      <c r="P114" s="50"/>
-      <c r="Q114" s="50">
+      <c r="Q114">
         <f t="shared" si="41"/>
         <v>191</v>
       </c>
-      <c r="R114" s="50">
+      <c r="R114">
         <f t="shared" si="42"/>
         <v>191</v>
       </c>
-      <c r="S114" s="50">
+      <c r="S114">
         <f t="shared" si="43"/>
         <v>192</v>
       </c>
-      <c r="T114" s="50"/>
-      <c r="U114" s="50" t="str">
+      <c r="U114" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V114" s="50" t="str">
+      <c r="V114" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W114" s="50" t="str">
+      <c r="W114" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="115" spans="1:23">
-      <c r="A115" s="50">
+      <c r="A115">
         <v>109</v>
       </c>
-      <c r="B115" s="49">
+      <c r="B115" s="42">
         <v>2048</v>
       </c>
-      <c r="C115" s="50"/>
-      <c r="D115" s="50"/>
-      <c r="E115" s="50">
+      <c r="E115">
         <f t="shared" si="29"/>
         <v>28672</v>
       </c>
-      <c r="F115" s="50">
+      <c r="F115">
         <f t="shared" si="39"/>
         <v>921600</v>
       </c>
-      <c r="G115" s="50">
+      <c r="G115">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H115" s="50"/>
-      <c r="I115" s="50" t="str">
+      <c r="I115" t="str">
         <f t="shared" si="25"/>
         <v>{28672,921600,4194304,109},</v>
       </c>
-      <c r="J115" s="50"/>
       <c r="K115">
         <f t="shared" si="16"/>
         <v>28</v>
       </c>
-      <c r="L115" s="50"/>
-      <c r="M115" s="50">
+      <c r="M115">
         <f t="shared" si="17"/>
         <v>28671</v>
       </c>
-      <c r="N115" s="50">
+      <c r="N115">
         <f t="shared" si="18"/>
         <v>28672</v>
       </c>
-      <c r="O115" s="50">
+      <c r="O115">
         <f t="shared" si="19"/>
         <v>28673</v>
       </c>
-      <c r="P115" s="50"/>
-      <c r="Q115" s="50">
+      <c r="Q115">
         <f t="shared" si="41"/>
         <v>199</v>
       </c>
-      <c r="R115" s="50">
+      <c r="R115">
         <f t="shared" si="42"/>
         <v>199</v>
       </c>
-      <c r="S115" s="50">
+      <c r="S115">
         <f t="shared" si="43"/>
         <v>200</v>
       </c>
-      <c r="T115" s="50"/>
-      <c r="U115" s="50" t="str">
+      <c r="U115" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V115" s="50" t="str">
+      <c r="V115" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W115" s="50" t="str">
+      <c r="W115" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="116" spans="1:23">
-      <c r="A116" s="50">
+      <c r="A116">
         <v>110</v>
       </c>
-      <c r="B116" s="49">
+      <c r="B116" s="42">
         <v>2048</v>
       </c>
-      <c r="C116" s="50"/>
-      <c r="D116" s="50"/>
-      <c r="E116" s="50">
+      <c r="E116">
         <f t="shared" si="29"/>
         <v>30720</v>
       </c>
-      <c r="F116" s="50">
+      <c r="F116">
         <f t="shared" si="39"/>
         <v>987136</v>
       </c>
-      <c r="G116" s="50">
+      <c r="G116">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H116" s="50"/>
-      <c r="I116" s="50" t="str">
+      <c r="I116" t="str">
         <f t="shared" si="25"/>
         <v>{30720,987136,4194304,110},</v>
       </c>
-      <c r="J116" s="50"/>
       <c r="K116">
         <f t="shared" si="16"/>
         <v>30</v>
       </c>
-      <c r="L116" s="50"/>
-      <c r="M116" s="50">
+      <c r="M116">
         <f t="shared" si="17"/>
         <v>30719</v>
       </c>
-      <c r="N116" s="50">
+      <c r="N116">
         <f t="shared" si="18"/>
         <v>30720</v>
       </c>
-      <c r="O116" s="50">
+      <c r="O116">
         <f t="shared" si="19"/>
         <v>30721</v>
       </c>
-      <c r="P116" s="50"/>
-      <c r="Q116" s="50">
+      <c r="Q116">
         <f t="shared" si="41"/>
         <v>207</v>
       </c>
-      <c r="R116" s="50">
+      <c r="R116">
         <f t="shared" si="42"/>
         <v>207</v>
       </c>
-      <c r="S116" s="50">
+      <c r="S116">
         <f t="shared" si="43"/>
         <v>208</v>
       </c>
-      <c r="T116" s="50"/>
-      <c r="U116" s="50" t="str">
+      <c r="U116" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V116" s="50" t="str">
+      <c r="V116" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W116" s="50" t="str">
+      <c r="W116" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="117" spans="1:23">
-      <c r="A117" s="50">
+      <c r="A117">
         <v>111</v>
       </c>
-      <c r="B117" s="49">
+      <c r="B117" s="42">
         <v>2048</v>
       </c>
-      <c r="C117" s="50"/>
-      <c r="D117" s="50"/>
-      <c r="E117" s="50">
+      <c r="E117">
         <f t="shared" si="29"/>
         <v>32768</v>
       </c>
-      <c r="F117" s="50">
+      <c r="F117">
         <f t="shared" si="39"/>
         <v>1052672</v>
       </c>
-      <c r="G117" s="50">
+      <c r="G117">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H117" s="50"/>
-      <c r="I117" s="50" t="str">
+      <c r="I117" t="str">
         <f t="shared" si="25"/>
         <v>{32768,1052672,4194304,111},</v>
       </c>
-      <c r="J117" s="50"/>
       <c r="K117">
         <f t="shared" si="16"/>
         <v>32</v>
       </c>
-      <c r="L117" s="50"/>
-      <c r="M117" s="50">
+      <c r="M117">
         <f t="shared" si="17"/>
         <v>32767</v>
       </c>
-      <c r="N117" s="50">
+      <c r="N117">
         <f t="shared" si="18"/>
         <v>32768</v>
       </c>
-      <c r="O117" s="50">
+      <c r="O117">
         <f t="shared" si="19"/>
         <v>32769</v>
       </c>
-      <c r="P117" s="50"/>
-      <c r="Q117" s="50">
+      <c r="Q117">
         <f t="shared" si="41"/>
         <v>215</v>
       </c>
-      <c r="R117" s="50">
+      <c r="R117">
         <f t="shared" si="42"/>
         <v>215</v>
       </c>
-      <c r="S117" s="50">
+      <c r="S117">
         <f t="shared" si="43"/>
         <v>216</v>
       </c>
-      <c r="T117" s="50"/>
-      <c r="U117" s="50" t="str">
+      <c r="U117" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V117" s="50" t="str">
+      <c r="V117" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W117" s="50" t="str">
+      <c r="W117" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="118" spans="1:23">
-      <c r="A118" s="49">
+      <c r="A118" s="42">
         <v>112</v>
       </c>
-      <c r="B118" s="49">
+      <c r="B118" s="42">
         <v>4096</v>
       </c>
-      <c r="C118" s="49"/>
-      <c r="D118" s="49"/>
-      <c r="E118" s="49">
+      <c r="C118" s="42"/>
+      <c r="D118" s="42"/>
+      <c r="E118" s="42">
         <f t="shared" si="29"/>
         <v>36864</v>
       </c>
-      <c r="F118" s="49">
+      <c r="F118" s="42">
         <f>IF(E118*16 &gt;F$117, INT((E118*16+4096)/4096)*4096,F$117)</f>
         <v>1052672</v>
       </c>
-      <c r="G118" s="49">
+      <c r="G118" s="42">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H118" s="49"/>
-      <c r="I118" s="49" t="str">
+      <c r="H118" s="42"/>
+      <c r="I118" s="42" t="str">
         <f t="shared" si="25"/>
         <v>{36864,1052672,4194304,112},</v>
       </c>
-      <c r="J118" s="49"/>
-      <c r="K118" s="49">
+      <c r="J118" s="42"/>
+      <c r="K118" s="42">
         <f t="shared" si="16"/>
         <v>36</v>
       </c>
-      <c r="L118" s="49"/>
-      <c r="M118" s="49">
+      <c r="L118" s="42"/>
+      <c r="M118" s="42">
         <f t="shared" si="17"/>
         <v>36863</v>
       </c>
-      <c r="N118" s="49">
+      <c r="N118" s="42">
         <f t="shared" si="18"/>
         <v>36864</v>
       </c>
-      <c r="O118" s="49">
+      <c r="O118" s="42">
         <f t="shared" si="19"/>
         <v>36865</v>
       </c>
-      <c r="P118" s="49"/>
-      <c r="Q118" s="49">
+      <c r="P118" s="42"/>
+      <c r="Q118" s="42">
         <f>INT((M118-6144-1)/512)+112</f>
         <v>171</v>
       </c>
-      <c r="R118" s="49">
+      <c r="R118" s="42">
         <f t="shared" ref="R118:S118" si="44">INT((N118-6144-1)/512)+112</f>
         <v>171</v>
       </c>
-      <c r="S118" s="49">
+      <c r="S118" s="42">
         <f t="shared" si="44"/>
         <v>172</v>
       </c>
-      <c r="T118" s="49"/>
-      <c r="U118" s="49" t="str">
+      <c r="T118" s="42"/>
+      <c r="U118" s="42" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V118" s="49" t="str">
+      <c r="V118" s="42" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W118" s="49" t="str">
+      <c r="W118" s="42" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="119" spans="1:23">
-      <c r="A119" s="50">
+      <c r="A119">
         <v>113</v>
       </c>
-      <c r="B119" s="49">
+      <c r="B119" s="42">
         <v>4096</v>
       </c>
-      <c r="C119" s="50"/>
-      <c r="D119" s="50"/>
-      <c r="E119" s="50">
+      <c r="E119">
         <f t="shared" si="29"/>
         <v>40960</v>
       </c>
-      <c r="F119" s="50">
+      <c r="F119">
         <f t="shared" ref="F119:F125" si="45">IF(E119*16 &gt;F$117, INT((E119*16+4096)/4096)*4096,F$117)</f>
         <v>1052672</v>
       </c>
-      <c r="G119" s="50">
+      <c r="G119">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H119" s="50"/>
-      <c r="I119" s="50" t="str">
+      <c r="I119" t="str">
         <f t="shared" si="25"/>
         <v>{40960,1052672,4194304,113},</v>
       </c>
-      <c r="J119" s="50"/>
-      <c r="K119" s="50">
+      <c r="K119">
         <f t="shared" si="16"/>
         <v>40</v>
       </c>
-      <c r="L119" s="50"/>
-      <c r="M119" s="50">
+      <c r="M119">
         <f t="shared" si="17"/>
         <v>40959</v>
       </c>
-      <c r="N119" s="50">
+      <c r="N119">
         <f t="shared" si="18"/>
         <v>40960</v>
       </c>
-      <c r="O119" s="50">
+      <c r="O119">
         <f t="shared" si="19"/>
         <v>40961</v>
       </c>
-      <c r="P119" s="50"/>
-      <c r="Q119" s="50">
+      <c r="Q119">
         <f t="shared" ref="Q119:Q121" si="46">INT((M119-6144-1)/512)+112</f>
         <v>179</v>
       </c>
-      <c r="R119" s="50">
+      <c r="R119">
         <f t="shared" ref="R119:R121" si="47">INT((N119-6144-1)/512)+112</f>
         <v>179</v>
       </c>
-      <c r="S119" s="50">
+      <c r="S119">
         <f t="shared" ref="S119:S121" si="48">INT((O119-6144-1)/512)+112</f>
         <v>180</v>
       </c>
-      <c r="T119" s="50"/>
-      <c r="U119" s="50" t="str">
+      <c r="U119" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V119" s="50" t="str">
+      <c r="V119" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W119" s="50" t="str">
+      <c r="W119" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="120" spans="1:23">
-      <c r="A120" s="50">
+      <c r="A120">
         <v>114</v>
       </c>
-      <c r="B120" s="49">
+      <c r="B120" s="42">
         <v>4096</v>
       </c>
-      <c r="C120" s="50"/>
-      <c r="D120" s="50"/>
-      <c r="E120" s="50">
+      <c r="E120">
         <f t="shared" si="29"/>
         <v>45056</v>
       </c>
-      <c r="F120" s="50">
+      <c r="F120">
         <f t="shared" si="45"/>
         <v>1052672</v>
       </c>
-      <c r="G120" s="50">
+      <c r="G120">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H120" s="50"/>
-      <c r="I120" s="50" t="str">
+      <c r="I120" t="str">
         <f t="shared" si="25"/>
         <v>{45056,1052672,4194304,114},</v>
       </c>
-      <c r="J120" s="50"/>
-      <c r="K120" s="50">
+      <c r="K120">
         <f t="shared" si="16"/>
         <v>44</v>
       </c>
-      <c r="L120" s="50"/>
-      <c r="M120" s="50">
+      <c r="M120">
         <f t="shared" si="17"/>
         <v>45055</v>
       </c>
-      <c r="N120" s="50">
+      <c r="N120">
         <f t="shared" si="18"/>
         <v>45056</v>
       </c>
-      <c r="O120" s="50">
+      <c r="O120">
         <f t="shared" si="19"/>
         <v>45057</v>
       </c>
-      <c r="P120" s="50"/>
-      <c r="Q120" s="50">
+      <c r="Q120">
         <f t="shared" si="46"/>
         <v>187</v>
       </c>
-      <c r="R120" s="50">
+      <c r="R120">
         <f t="shared" si="47"/>
         <v>187</v>
       </c>
-      <c r="S120" s="50">
+      <c r="S120">
         <f t="shared" si="48"/>
         <v>188</v>
       </c>
-      <c r="T120" s="50"/>
-      <c r="U120" s="50" t="str">
+      <c r="U120" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V120" s="50" t="str">
+      <c r="V120" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W120" s="50" t="str">
+      <c r="W120" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
     </row>
     <row r="121" spans="1:23">
-      <c r="A121" s="51">
+      <c r="A121" s="43">
         <v>115</v>
       </c>
-      <c r="B121" s="49">
+      <c r="B121" s="42">
         <v>4096</v>
       </c>
-      <c r="C121" s="51"/>
-      <c r="D121" s="51"/>
-      <c r="E121" s="51">
+      <c r="C121" s="43"/>
+      <c r="D121" s="43"/>
+      <c r="E121" s="43">
         <f t="shared" si="29"/>
         <v>49152</v>
       </c>
-      <c r="F121" s="51">
+      <c r="F121" s="43">
         <f t="shared" si="45"/>
         <v>1052672</v>
       </c>
-      <c r="G121" s="51">
+      <c r="G121" s="43">
         <f t="shared" si="30"/>
         <v>4194304</v>
       </c>
-      <c r="H121" s="51"/>
-      <c r="I121" s="51" t="str">
+      <c r="H121" s="43"/>
+      <c r="I121" s="43" t="str">
         <f t="shared" si="25"/>
         <v>{49152,1052672,4194304,115},</v>
       </c>
-      <c r="J121" s="51"/>
-      <c r="K121" s="51">
+      <c r="J121" s="43"/>
+      <c r="K121" s="43">
         <f t="shared" si="16"/>
         <v>48</v>
       </c>
-      <c r="L121" s="51"/>
-      <c r="M121" s="51">
+      <c r="L121" s="43"/>
+      <c r="M121" s="43">
         <f t="shared" si="17"/>
         <v>49151</v>
       </c>
-      <c r="N121" s="51">
+      <c r="N121" s="43">
         <f t="shared" si="18"/>
         <v>49152</v>
       </c>
-      <c r="O121" s="51">
+      <c r="O121" s="43">
         <f t="shared" si="19"/>
         <v>49153</v>
       </c>
-      <c r="P121" s="51"/>
-      <c r="Q121" s="51">
+      <c r="P121" s="43"/>
+      <c r="Q121" s="43">
         <f t="shared" si="46"/>
         <v>195</v>
       </c>
-      <c r="R121" s="51">
+      <c r="R121" s="43">
         <f t="shared" si="47"/>
         <v>195</v>
       </c>
-      <c r="S121" s="51">
+      <c r="S121" s="43">
         <f t="shared" si="48"/>
         <v>196</v>
       </c>
-      <c r="T121" s="51"/>
-      <c r="U121" s="51" t="str">
+      <c r="T121" s="43"/>
+      <c r="U121" s="43" t="str">
         <f t="shared" si="21"/>
         <v>NG</v>
       </c>
-      <c r="V121" s="51" t="str">
+      <c r="V121" s="43" t="str">
         <f t="shared" si="22"/>
         <v>NG</v>
       </c>
-      <c r="W121" s="51" t="str">
+      <c r="W121" s="43" t="str">
         <f t="shared" si="23"/>
         <v>NG</v>
       </c>
@@ -13181,7 +12865,7 @@
       <c r="A122">
         <v>116</v>
       </c>
-      <c r="B122" s="49">
+      <c r="B122" s="42">
         <v>4096</v>
       </c>
       <c r="E122">
@@ -13217,15 +12901,15 @@
         <v>53249</v>
       </c>
       <c r="Q122">
-        <f t="shared" ref="Q70:Q133" si="49">INT((M122-1)/8)</f>
+        <f t="shared" ref="Q122:Q133" si="49">INT((M122-1)/8)</f>
         <v>6655</v>
       </c>
       <c r="R122">
-        <f t="shared" ref="R70:R133" si="50">INT((N122-1)/8)</f>
+        <f t="shared" ref="R122:R133" si="50">INT((N122-1)/8)</f>
         <v>6655</v>
       </c>
       <c r="S122">
-        <f t="shared" ref="S70:S133" si="51">INT((O122-1)/8)</f>
+        <f t="shared" ref="S122:S133" si="51">INT((O122-1)/8)</f>
         <v>6656</v>
       </c>
       <c r="U122" t="str">
@@ -13245,7 +12929,7 @@
       <c r="A123">
         <v>117</v>
       </c>
-      <c r="B123" s="49">
+      <c r="B123" s="42">
         <v>4096</v>
       </c>
       <c r="E123">
@@ -13309,7 +12993,7 @@
       <c r="A124">
         <v>118</v>
       </c>
-      <c r="B124" s="49">
+      <c r="B124" s="42">
         <v>4096</v>
       </c>
       <c r="E124">
@@ -13373,7 +13057,7 @@
       <c r="A125">
         <v>119</v>
       </c>
-      <c r="B125" s="49">
+      <c r="B125" s="42">
         <v>4096</v>
       </c>
       <c r="E125">
@@ -13955,14 +13639,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="U6:W133">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="NG">
-      <formula>NOT(ISERROR(SEARCH("NG",U6)))</formula>
+  <conditionalFormatting sqref="T6">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="NG">
+      <formula>NOT(ISERROR(SEARCH("NG",T6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T6">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="NG">
-      <formula>NOT(ISERROR(SEARCH("NG",T6)))</formula>
+  <conditionalFormatting sqref="U6:W133">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="NG">
+      <formula>NOT(ISERROR(SEARCH("NG",U6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>